<commit_message>
fixed breaking changes on inst add  Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/LUSID Excel - Setting up your IBOR template Global Equity Fund.xlsx
+++ b/LUSID Excel - Setting up your IBOR template Global Equity Fund.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusSekhon\Dev\sample-excel\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EE6566-21C0-4FBD-9C04-16BCCE03AFC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E3777-B513-4323-981D-CD52F305C035}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" activeTab="9" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
   </bookViews>
@@ -1359,7 +1359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1393,6 +1393,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9261"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1454,7 +1460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1685,6 +1691,9 @@
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1713,1150 +1722,1150 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.45f29de5428d4e99882dfebacb0ed41d">
+    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>134a27bf-0545-4a70-8413-63d754c4a2aa</stp>
-        <tr r="F55" s="9"/>
-        <tr r="I57" s="9"/>
-        <tr r="H54" s="9"/>
-        <tr r="J51" s="9"/>
-        <tr r="G59" s="9"/>
-        <tr r="F61" s="9"/>
-        <tr r="J54" s="9"/>
-        <tr r="J55" s="9"/>
-        <tr r="J58" s="9"/>
-        <tr r="I53" s="9"/>
-        <tr r="F54" s="9"/>
-        <tr r="G56" s="9"/>
-        <tr r="G53" s="9"/>
-        <tr r="H57" s="9"/>
-        <tr r="J60" s="9"/>
-        <tr r="F59" s="9"/>
-        <tr r="G57" s="9"/>
-        <tr r="I55" s="9"/>
-        <tr r="F57" s="9"/>
-        <tr r="H53" s="9"/>
-        <tr r="I58" s="9"/>
-        <tr r="I60" s="9"/>
-        <tr r="I59" s="9"/>
-        <tr r="F56" s="9"/>
-        <tr r="I56" s="9"/>
-        <tr r="H60" s="9"/>
-        <tr r="H55" s="9"/>
-        <tr r="F53" s="9"/>
-        <tr r="J61" s="9"/>
-        <tr r="F51" s="9"/>
-        <tr r="H61" s="9"/>
-        <tr r="I61" s="9"/>
-        <tr r="J52" s="9"/>
-        <tr r="G51" s="9"/>
-        <tr r="J59" s="9"/>
-        <tr r="F58" s="9"/>
-        <tr r="J57" s="9"/>
-        <tr r="J56" s="9"/>
-        <tr r="G58" s="9"/>
-        <tr r="G54" s="9"/>
-        <tr r="I54" s="9"/>
-        <tr r="F52" s="9"/>
-        <tr r="H52" s="9"/>
-        <tr r="H59" s="9"/>
-        <tr r="J53" s="9"/>
-        <tr r="I52" s="9"/>
-        <tr r="G61" s="9"/>
-        <tr r="H51" s="9"/>
-        <tr r="H58" s="9"/>
-        <tr r="I51" s="9"/>
-        <tr r="H56" s="9"/>
-        <tr r="G52" s="9"/>
-        <tr r="F60" s="9"/>
-        <tr r="G55" s="9"/>
-        <tr r="G60" s="9"/>
+        <stp>d833a068-0729-410c-8d42-3c60a8e5e6c9</stp>
+        <tr r="W40" s="6"/>
+        <tr r="T33" s="6"/>
+        <tr r="AB37" s="6"/>
+        <tr r="S38" s="6"/>
+        <tr r="V35" s="6"/>
+        <tr r="R49" s="6"/>
+        <tr r="F47" s="6"/>
+        <tr r="AH33" s="6"/>
+        <tr r="V42" s="6"/>
+        <tr r="W52" s="6"/>
+        <tr r="O52" s="6"/>
+        <tr r="R45" s="6"/>
+        <tr r="AF51" s="6"/>
+        <tr r="T50" s="6"/>
+        <tr r="W48" s="6"/>
+        <tr r="Q44" s="6"/>
+        <tr r="T41" s="6"/>
+        <tr r="V39" s="6"/>
+        <tr r="W42" s="6"/>
+        <tr r="N36" s="6"/>
+        <tr r="I34" s="6"/>
+        <tr r="Z48" s="6"/>
+        <tr r="O43" s="6"/>
+        <tr r="S39" s="6"/>
+        <tr r="J49" s="6"/>
+        <tr r="M40" s="6"/>
+        <tr r="O38" s="6"/>
+        <tr r="AD41" s="6"/>
+        <tr r="AE41" s="6"/>
+        <tr r="AB33" s="6"/>
+        <tr r="J42" s="6"/>
+        <tr r="AG49" s="6"/>
+        <tr r="W36" s="6"/>
+        <tr r="AH48" s="6"/>
+        <tr r="X43" s="6"/>
+        <tr r="O45" s="6"/>
+        <tr r="R41" s="6"/>
+        <tr r="V33" s="6"/>
+        <tr r="Z34" s="6"/>
+        <tr r="H49" s="6"/>
+        <tr r="AH43" s="6"/>
+        <tr r="S44" s="6"/>
+        <tr r="J44" s="6"/>
+        <tr r="E48" s="6"/>
+        <tr r="X38" s="6"/>
+        <tr r="AB41" s="6"/>
+        <tr r="L40" s="6"/>
+        <tr r="T43" s="6"/>
+        <tr r="O46" s="6"/>
+        <tr r="G39" s="6"/>
+        <tr r="P35" s="6"/>
+        <tr r="I39" s="6"/>
+        <tr r="G47" s="6"/>
+        <tr r="E42" s="6"/>
+        <tr r="U43" s="6"/>
+        <tr r="J47" s="6"/>
+        <tr r="H35" s="6"/>
+        <tr r="AF45" s="6"/>
+        <tr r="M48" s="6"/>
+        <tr r="Q45" s="6"/>
+        <tr r="AA47" s="6"/>
+        <tr r="P48" s="6"/>
+        <tr r="K48" s="6"/>
+        <tr r="U36" s="6"/>
+        <tr r="AA33" s="6"/>
+        <tr r="AH37" s="6"/>
+        <tr r="AD47" s="6"/>
+        <tr r="AB39" s="6"/>
+        <tr r="AC43" s="6"/>
+        <tr r="U34" s="6"/>
+        <tr r="J46" s="6"/>
+        <tr r="S52" s="6"/>
+        <tr r="S50" s="6"/>
+        <tr r="Q46" s="6"/>
+        <tr r="Y41" s="6"/>
+        <tr r="H36" s="6"/>
+        <tr r="J40" s="6"/>
+        <tr r="AA48" s="6"/>
+        <tr r="S48" s="6"/>
+        <tr r="I47" s="6"/>
+        <tr r="AA43" s="6"/>
+        <tr r="G49" s="6"/>
+        <tr r="AH34" s="6"/>
+        <tr r="AG52" s="6"/>
+        <tr r="L46" s="6"/>
+        <tr r="M46" s="6"/>
+        <tr r="H51" s="6"/>
+        <tr r="Y36" s="6"/>
+        <tr r="P38" s="6"/>
+        <tr r="AA44" s="6"/>
+        <tr r="E45" s="6"/>
+        <tr r="S42" s="6"/>
+        <tr r="M37" s="6"/>
+        <tr r="F51" s="6"/>
+        <tr r="H44" s="6"/>
+        <tr r="W37" s="6"/>
+        <tr r="E49" s="6"/>
+        <tr r="J35" s="6"/>
+        <tr r="AC48" s="6"/>
+        <tr r="AF33" s="6"/>
+        <tr r="T52" s="6"/>
+        <tr r="S46" s="6"/>
+        <tr r="E43" s="6"/>
+        <tr r="U52" s="6"/>
+        <tr r="I48" s="6"/>
+        <tr r="G42" s="6"/>
+        <tr r="W41" s="6"/>
+        <tr r="AA52" s="6"/>
+        <tr r="Y45" s="6"/>
+        <tr r="AB38" s="6"/>
+        <tr r="AF34" s="6"/>
+        <tr r="M42" s="6"/>
+        <tr r="N35" s="6"/>
+        <tr r="AE38" s="6"/>
+        <tr r="U49" s="6"/>
+        <tr r="T48" s="6"/>
+        <tr r="AE43" s="6"/>
+        <tr r="Z38" s="6"/>
+        <tr r="Q51" s="6"/>
+        <tr r="Q50" s="6"/>
+        <tr r="M38" s="6"/>
+        <tr r="V38" s="6"/>
+        <tr r="AC46" s="6"/>
+        <tr r="M43" s="6"/>
+        <tr r="AA42" s="6"/>
+        <tr r="S40" s="6"/>
+        <tr r="X41" s="6"/>
+        <tr r="AA46" s="6"/>
+        <tr r="AB44" s="6"/>
+        <tr r="AE45" s="6"/>
+        <tr r="U37" s="6"/>
+        <tr r="U38" s="6"/>
+        <tr r="Q38" s="6"/>
+        <tr r="Y38" s="6"/>
+        <tr r="H33" s="6"/>
+        <tr r="V34" s="6"/>
+        <tr r="X44" s="6"/>
+        <tr r="U48" s="6"/>
+        <tr r="R51" s="6"/>
+        <tr r="W35" s="6"/>
+        <tr r="L52" s="6"/>
+        <tr r="AE50" s="6"/>
+        <tr r="X42" s="6"/>
+        <tr r="I33" s="6"/>
+        <tr r="X52" s="6"/>
+        <tr r="AA45" s="6"/>
+        <tr r="R48" s="6"/>
+        <tr r="AH40" s="6"/>
+        <tr r="AB42" s="6"/>
+        <tr r="AA49" s="6"/>
+        <tr r="Z33" s="6"/>
+        <tr r="AF49" s="6"/>
+        <tr r="AA34" s="6"/>
+        <tr r="K37" s="6"/>
+        <tr r="Z40" s="6"/>
+        <tr r="AE34" s="6"/>
+        <tr r="N46" s="6"/>
+        <tr r="AH38" s="6"/>
+        <tr r="G48" s="6"/>
+        <tr r="P47" s="6"/>
+        <tr r="I44" s="6"/>
+        <tr r="Z52" s="6"/>
+        <tr r="W51" s="6"/>
+        <tr r="K43" s="6"/>
+        <tr r="F44" s="6"/>
+        <tr r="X50" s="6"/>
+        <tr r="X37" s="6"/>
+        <tr r="Z46" s="6"/>
+        <tr r="P39" s="6"/>
+        <tr r="Q52" s="6"/>
+        <tr r="AG44" s="6"/>
+        <tr r="N49" s="6"/>
+        <tr r="F36" s="6"/>
+        <tr r="Y37" s="6"/>
+        <tr r="Y46" s="6"/>
+        <tr r="AD43" s="6"/>
+        <tr r="N38" s="6"/>
+        <tr r="H34" s="6"/>
+        <tr r="R42" s="6"/>
+        <tr r="AE40" s="6"/>
+        <tr r="AB50" s="6"/>
+        <tr r="AB35" s="6"/>
+        <tr r="Y52" s="6"/>
+        <tr r="AF46" s="6"/>
+        <tr r="J50" s="6"/>
+        <tr r="AD46" s="6"/>
+        <tr r="I40" s="6"/>
+        <tr r="AD52" s="6"/>
+        <tr r="J48" s="6"/>
+        <tr r="AH52" s="6"/>
+        <tr r="U51" s="6"/>
+        <tr r="N40" s="6"/>
+        <tr r="AF40" s="6"/>
+        <tr r="S41" s="6"/>
+        <tr r="Z49" s="6"/>
+        <tr r="T45" s="6"/>
+        <tr r="T35" s="6"/>
+        <tr r="AA51" s="6"/>
+        <tr r="P51" s="6"/>
+        <tr r="X45" s="6"/>
+        <tr r="E38" s="6"/>
+        <tr r="V49" s="6"/>
+        <tr r="AH45" s="6"/>
+        <tr r="F49" s="6"/>
+        <tr r="L33" s="6"/>
+        <tr r="I38" s="6"/>
+        <tr r="R47" s="6"/>
+        <tr r="X36" s="6"/>
+        <tr r="V46" s="6"/>
+        <tr r="U40" s="6"/>
+        <tr r="G52" s="6"/>
+        <tr r="T51" s="6"/>
+        <tr r="Z51" s="6"/>
+        <tr r="O37" s="6"/>
+        <tr r="AG51" s="6"/>
+        <tr r="X40" s="6"/>
+        <tr r="I52" s="6"/>
+        <tr r="L35" s="6"/>
+        <tr r="AH44" s="6"/>
+        <tr r="K52" s="6"/>
+        <tr r="O44" s="6"/>
+        <tr r="S37" s="6"/>
+        <tr r="Y34" s="6"/>
+        <tr r="E46" s="6"/>
+        <tr r="AF52" s="6"/>
+        <tr r="K44" s="6"/>
+        <tr r="E52" s="6"/>
+        <tr r="Q33" s="6"/>
+        <tr r="S33" s="6"/>
+        <tr r="X34" s="6"/>
+        <tr r="AE33" s="6"/>
+        <tr r="S36" s="6"/>
+        <tr r="S47" s="6"/>
+        <tr r="AF39" s="6"/>
+        <tr r="U35" s="6"/>
+        <tr r="M51" s="6"/>
+        <tr r="K45" s="6"/>
+        <tr r="F33" s="6"/>
+        <tr r="O47" s="6"/>
+        <tr r="AH42" s="6"/>
+        <tr r="AH50" s="6"/>
+        <tr r="G45" s="6"/>
+        <tr r="L47" s="6"/>
+        <tr r="O36" s="6"/>
+        <tr r="AD45" s="6"/>
+        <tr r="F48" s="6"/>
+        <tr r="N42" s="6"/>
+        <tr r="F38" s="6"/>
+        <tr r="R46" s="6"/>
+        <tr r="F46" s="6"/>
+        <tr r="AH41" s="6"/>
+        <tr r="Q34" s="6"/>
+        <tr r="AC39" s="6"/>
+        <tr r="T39" s="6"/>
+        <tr r="AE36" s="6"/>
+        <tr r="H40" s="6"/>
+        <tr r="AF43" s="6"/>
+        <tr r="R39" s="6"/>
+        <tr r="P43" s="6"/>
+        <tr r="O48" s="6"/>
+        <tr r="AB43" s="6"/>
+        <tr r="I35" s="6"/>
+        <tr r="V51" s="6"/>
+        <tr r="AF35" s="6"/>
+        <tr r="Z43" s="6"/>
+        <tr r="Q37" s="6"/>
+        <tr r="N52" s="6"/>
+        <tr r="L43" s="6"/>
+        <tr r="G37" s="6"/>
+        <tr r="P37" s="6"/>
+        <tr r="Y42" s="6"/>
+        <tr r="R36" s="6"/>
+        <tr r="S43" s="6"/>
+        <tr r="T36" s="6"/>
+        <tr r="L42" s="6"/>
+        <tr r="N48" s="6"/>
+        <tr r="F37" s="6"/>
+        <tr r="I37" s="6"/>
+        <tr r="Q49" s="6"/>
+        <tr r="AB48" s="6"/>
+        <tr r="G34" s="6"/>
+        <tr r="M49" s="6"/>
+        <tr r="V50" s="6"/>
+        <tr r="AF47" s="6"/>
+        <tr r="H42" s="6"/>
+        <tr r="P50" s="6"/>
+        <tr r="AH46" s="6"/>
+        <tr r="I43" s="6"/>
+        <tr r="Q36" s="6"/>
+        <tr r="H52" s="6"/>
+        <tr r="T38" s="6"/>
+        <tr r="H39" s="6"/>
+        <tr r="AF48" s="6"/>
+        <tr r="M33" s="6"/>
+        <tr r="O34" s="6"/>
+        <tr r="L45" s="6"/>
+        <tr r="M41" s="6"/>
+        <tr r="J41" s="6"/>
+        <tr r="W43" s="6"/>
+        <tr r="L49" s="6"/>
+        <tr r="W38" s="6"/>
+        <tr r="AA36" s="6"/>
+        <tr r="S49" s="6"/>
+        <tr r="Y51" s="6"/>
+        <tr r="AH36" s="6"/>
+        <tr r="AF37" s="6"/>
+        <tr r="N50" s="6"/>
+        <tr r="T34" s="6"/>
+        <tr r="G35" s="6"/>
+        <tr r="J43" s="6"/>
+        <tr r="J38" s="6"/>
+        <tr r="M44" s="6"/>
+        <tr r="N33" s="6"/>
+        <tr r="W49" s="6"/>
+        <tr r="AG48" s="6"/>
+        <tr r="V37" s="6"/>
+        <tr r="G51" s="6"/>
+        <tr r="AD51" s="6"/>
+        <tr r="AC33" s="6"/>
+        <tr r="G38" s="6"/>
+        <tr r="F45" s="6"/>
+        <tr r="S34" s="6"/>
+        <tr r="N44" s="6"/>
+        <tr r="AH51" s="6"/>
+        <tr r="V40" s="6"/>
+        <tr r="E33" s="6"/>
+        <tr r="H47" s="6"/>
+        <tr r="H41" s="6"/>
+        <tr r="Z47" s="6"/>
+        <tr r="V43" s="6"/>
+        <tr r="P41" s="6"/>
+        <tr r="U47" s="6"/>
+        <tr r="E51" s="6"/>
+        <tr r="V41" s="6"/>
+        <tr r="AC35" s="6"/>
+        <tr r="K51" s="6"/>
+        <tr r="W33" s="6"/>
+        <tr r="L34" s="6"/>
+        <tr r="AG43" s="6"/>
+        <tr r="Y35" s="6"/>
+        <tr r="U41" s="6"/>
+        <tr r="N37" s="6"/>
+        <tr r="AG41" s="6"/>
+        <tr r="W39" s="6"/>
+        <tr r="M50" s="6"/>
+        <tr r="N45" s="6"/>
+        <tr r="I51" s="6"/>
+        <tr r="F50" s="6"/>
+        <tr r="K39" s="6"/>
+        <tr r="AE37" s="6"/>
+        <tr r="AF41" s="6"/>
+        <tr r="F42" s="6"/>
+        <tr r="H37" s="6"/>
+        <tr r="R52" s="6"/>
+        <tr r="E44" s="6"/>
+        <tr r="AB40" s="6"/>
+        <tr r="S51" s="6"/>
+        <tr r="J34" s="6"/>
+        <tr r="H50" s="6"/>
+        <tr r="AE42" s="6"/>
+        <tr r="AC40" s="6"/>
+        <tr r="Z41" s="6"/>
+        <tr r="AG35" s="6"/>
+        <tr r="AC37" s="6"/>
+        <tr r="Q40" s="6"/>
+        <tr r="AH47" s="6"/>
+        <tr r="K42" s="6"/>
+        <tr r="R50" s="6"/>
+        <tr r="AF44" s="6"/>
+        <tr r="K47" s="6"/>
+        <tr r="T44" s="6"/>
+        <tr r="AA39" s="6"/>
+        <tr r="AE35" s="6"/>
+        <tr r="AC51" s="6"/>
+        <tr r="I36" s="6"/>
+        <tr r="Z39" s="6"/>
+        <tr r="L39" s="6"/>
+        <tr r="X35" s="6"/>
+        <tr r="AD42" s="6"/>
+        <tr r="E37" s="6"/>
+        <tr r="U42" s="6"/>
+        <tr r="V47" s="6"/>
+        <tr r="AB36" s="6"/>
+        <tr r="F34" s="6"/>
+        <tr r="N39" s="6"/>
+        <tr r="S45" s="6"/>
+        <tr r="L41" s="6"/>
+        <tr r="P40" s="6"/>
+        <tr r="N51" s="6"/>
+        <tr r="W44" s="6"/>
+        <tr r="AC42" s="6"/>
+        <tr r="AC47" s="6"/>
+        <tr r="AD50" s="6"/>
+        <tr r="M52" s="6"/>
+        <tr r="U44" s="6"/>
+        <tr r="AC52" s="6"/>
+        <tr r="J36" s="6"/>
+        <tr r="J52" s="6"/>
+        <tr r="S35" s="6"/>
+        <tr r="AD49" s="6"/>
+        <tr r="O33" s="6"/>
+        <tr r="AA40" s="6"/>
+        <tr r="J45" s="6"/>
+        <tr r="Y44" s="6"/>
+        <tr r="E35" s="6"/>
+        <tr r="X47" s="6"/>
+        <tr r="P36" s="6"/>
+        <tr r="U50" s="6"/>
+        <tr r="H45" s="6"/>
+        <tr r="P52" s="6"/>
+        <tr r="Z37" s="6"/>
+        <tr r="Y48" s="6"/>
+        <tr r="AE46" s="6"/>
+        <tr r="X49" s="6"/>
+        <tr r="AB49" s="6"/>
+        <tr r="K33" s="6"/>
+        <tr r="AG39" s="6"/>
+        <tr r="AC44" s="6"/>
+        <tr r="M47" s="6"/>
+        <tr r="AD38" s="6"/>
+        <tr r="AG33" s="6"/>
+        <tr r="M36" s="6"/>
+        <tr r="AG42" s="6"/>
+        <tr r="K35" s="6"/>
+        <tr r="AD40" s="6"/>
+        <tr r="L38" s="6"/>
+        <tr r="X51" s="6"/>
+        <tr r="Z44" s="6"/>
+        <tr r="L36" s="6"/>
+        <tr r="K46" s="6"/>
+        <tr r="AA37" s="6"/>
+        <tr r="Q42" s="6"/>
+        <tr r="F52" s="6"/>
+        <tr r="G44" s="6"/>
+        <tr r="T42" s="6"/>
+        <tr r="R38" s="6"/>
+        <tr r="AC41" s="6"/>
+        <tr r="F35" s="6"/>
+        <tr r="AC38" s="6"/>
+        <tr r="F41" s="6"/>
+        <tr r="P46" s="6"/>
+        <tr r="L51" s="6"/>
+        <tr r="E34" s="6"/>
+        <tr r="F43" s="6"/>
+        <tr r="O35" s="6"/>
+        <tr r="AH35" s="6"/>
+        <tr r="H46" s="6"/>
+        <tr r="Q43" s="6"/>
+        <tr r="U45" s="6"/>
+        <tr r="I49" s="6"/>
+        <tr r="M45" s="6"/>
+        <tr r="AA41" s="6"/>
+        <tr r="P34" s="6"/>
+        <tr r="G33" s="6"/>
+        <tr r="Q35" s="6"/>
+        <tr r="AE47" s="6"/>
+        <tr r="Y47" s="6"/>
+        <tr r="J51" s="6"/>
+        <tr r="L44" s="6"/>
+        <tr r="Y50" s="6"/>
+        <tr r="O41" s="6"/>
+        <tr r="K41" s="6"/>
+        <tr r="AG37" s="6"/>
+        <tr r="E47" s="6"/>
+        <tr r="R40" s="6"/>
+        <tr r="AG34" s="6"/>
+        <tr r="AC36" s="6"/>
+        <tr r="U39" s="6"/>
+        <tr r="AD33" s="6"/>
+        <tr r="I46" s="6"/>
+        <tr r="AH39" s="6"/>
+        <tr r="N34" s="6"/>
+        <tr r="I45" s="6"/>
+        <tr r="V45" s="6"/>
+        <tr r="R35" s="6"/>
+        <tr r="AD39" s="6"/>
+        <tr r="E41" s="6"/>
+        <tr r="Z36" s="6"/>
+        <tr r="Y33" s="6"/>
+        <tr r="O40" s="6"/>
+        <tr r="AG40" s="6"/>
+        <tr r="L50" s="6"/>
+        <tr r="AB34" s="6"/>
+        <tr r="AC50" s="6"/>
+        <tr r="G41" s="6"/>
+        <tr r="Q47" s="6"/>
+        <tr r="AE44" s="6"/>
+        <tr r="Y49" s="6"/>
+        <tr r="Z42" s="6"/>
+        <tr r="AE49" s="6"/>
+        <tr r="AB52" s="6"/>
+        <tr r="R33" s="6"/>
+        <tr r="T37" s="6"/>
+        <tr r="U33" s="6"/>
+        <tr r="R44" s="6"/>
+        <tr r="J37" s="6"/>
+        <tr r="V44" s="6"/>
+        <tr r="AA35" s="6"/>
+        <tr r="L48" s="6"/>
+        <tr r="AE39" s="6"/>
+        <tr r="X48" s="6"/>
+        <tr r="K50" s="6"/>
+        <tr r="W45" s="6"/>
+        <tr r="AC45" s="6"/>
+        <tr r="K34" s="6"/>
+        <tr r="Q48" s="6"/>
+        <tr r="M34" s="6"/>
+        <tr r="J39" s="6"/>
+        <tr r="N41" s="6"/>
+        <tr r="AF42" s="6"/>
+        <tr r="E39" s="6"/>
+        <tr r="AB45" s="6"/>
+        <tr r="AC49" s="6"/>
+        <tr r="AD35" s="6"/>
+        <tr r="R34" s="6"/>
+        <tr r="F39" s="6"/>
+        <tr r="U46" s="6"/>
+        <tr r="V52" s="6"/>
+        <tr r="Z45" s="6"/>
+        <tr r="X39" s="6"/>
+        <tr r="P33" s="6"/>
+        <tr r="AF36" s="6"/>
+        <tr r="V48" s="6"/>
+        <tr r="V36" s="6"/>
+        <tr r="K38" s="6"/>
+        <tr r="E36" s="6"/>
+        <tr r="P45" s="6"/>
+        <tr r="O51" s="6"/>
+        <tr r="L37" s="6"/>
+        <tr r="R37" s="6"/>
+        <tr r="P49" s="6"/>
+        <tr r="H38" s="6"/>
+        <tr r="AD37" s="6"/>
+        <tr r="AD36" s="6"/>
+        <tr r="K49" s="6"/>
+        <tr r="Q41" s="6"/>
+        <tr r="H43" s="6"/>
+        <tr r="I41" s="6"/>
+        <tr r="Y40" s="6"/>
+        <tr r="R43" s="6"/>
+        <tr r="E40" s="6"/>
+        <tr r="K36" s="6"/>
+        <tr r="Z35" s="6"/>
+        <tr r="AG50" s="6"/>
+        <tr r="P42" s="6"/>
+        <tr r="T47" s="6"/>
+        <tr r="W46" s="6"/>
+        <tr r="AD34" s="6"/>
+        <tr r="AG47" s="6"/>
+        <tr r="AA38" s="6"/>
+        <tr r="AG46" s="6"/>
+        <tr r="M35" s="6"/>
+        <tr r="T40" s="6"/>
+        <tr r="M39" s="6"/>
+        <tr r="AG38" s="6"/>
+        <tr r="P44" s="6"/>
+        <tr r="AH49" s="6"/>
+        <tr r="T46" s="6"/>
+        <tr r="AG36" s="6"/>
+        <tr r="O42" s="6"/>
+        <tr r="O39" s="6"/>
+        <tr r="G46" s="6"/>
+        <tr r="T49" s="6"/>
+        <tr r="AE51" s="6"/>
+        <tr r="W50" s="6"/>
+        <tr r="AE48" s="6"/>
+        <tr r="W34" s="6"/>
+        <tr r="O50" s="6"/>
+        <tr r="AB47" s="6"/>
+        <tr r="G40" s="6"/>
+        <tr r="G43" s="6"/>
+        <tr r="AE52" s="6"/>
+        <tr r="Y39" s="6"/>
+        <tr r="N47" s="6"/>
+        <tr r="F40" s="6"/>
+        <tr r="AF50" s="6"/>
+        <tr r="AC34" s="6"/>
+        <tr r="G36" s="6"/>
+        <tr r="W47" s="6"/>
+        <tr r="AD44" s="6"/>
+        <tr r="AB46" s="6"/>
+        <tr r="AG45" s="6"/>
+        <tr r="X46" s="6"/>
+        <tr r="H48" s="6"/>
+        <tr r="I50" s="6"/>
+        <tr r="Y43" s="6"/>
+        <tr r="Q39" s="6"/>
+        <tr r="Z50" s="6"/>
+        <tr r="AF38" s="6"/>
+        <tr r="N43" s="6"/>
+        <tr r="J33" s="6"/>
+        <tr r="G50" s="6"/>
+        <tr r="K40" s="6"/>
+        <tr r="AA50" s="6"/>
+        <tr r="I42" s="6"/>
+        <tr r="AD48" s="6"/>
+        <tr r="AB51" s="6"/>
+        <tr r="E50" s="6"/>
+        <tr r="X33" s="6"/>
+        <tr r="O49" s="6"/>
       </tp>
     </main>
-    <main first="rtdsrv.45f29de5428d4e99882dfebacb0ed41d">
+    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>6f35c29e-541b-473c-9013-e6273625c087</stp>
-        <tr r="L36" s="8"/>
-        <tr r="I50" s="8"/>
-        <tr r="E34" s="8"/>
-        <tr r="I47" s="8"/>
-        <tr r="J34" s="8"/>
-        <tr r="F32" s="8"/>
-        <tr r="H41" s="8"/>
-        <tr r="F33" s="8"/>
-        <tr r="G40" s="8"/>
-        <tr r="H48" s="8"/>
-        <tr r="L43" s="8"/>
-        <tr r="L50" s="8"/>
-        <tr r="J49" s="8"/>
-        <tr r="K36" s="8"/>
-        <tr r="J36" s="8"/>
-        <tr r="L46" s="8"/>
-        <tr r="F47" s="8"/>
-        <tr r="J38" s="8"/>
-        <tr r="F36" s="8"/>
-        <tr r="I48" s="8"/>
-        <tr r="F45" s="8"/>
-        <tr r="K34" s="8"/>
-        <tr r="L48" s="8"/>
-        <tr r="E51" s="8"/>
-        <tr r="I43" s="8"/>
-        <tr r="L47" s="8"/>
-        <tr r="H49" s="8"/>
-        <tr r="G42" s="8"/>
-        <tr r="L33" s="8"/>
-        <tr r="I46" s="8"/>
-        <tr r="E44" s="8"/>
-        <tr r="E35" s="8"/>
-        <tr r="K38" s="8"/>
-        <tr r="G38" s="8"/>
-        <tr r="K43" s="8"/>
-        <tr r="K35" s="8"/>
-        <tr r="H36" s="8"/>
-        <tr r="I45" s="8"/>
-        <tr r="K47" s="8"/>
-        <tr r="J48" s="8"/>
-        <tr r="G47" s="8"/>
-        <tr r="I39" s="8"/>
-        <tr r="F39" s="8"/>
-        <tr r="L44" s="8"/>
-        <tr r="K41" s="8"/>
-        <tr r="J33" s="8"/>
-        <tr r="I33" s="8"/>
-        <tr r="E39" s="8"/>
-        <tr r="E38" s="8"/>
-        <tr r="J39" s="8"/>
-        <tr r="G48" s="8"/>
-        <tr r="E40" s="8"/>
-        <tr r="H45" s="8"/>
-        <tr r="L34" s="8"/>
-        <tr r="E49" s="8"/>
-        <tr r="H40" s="8"/>
-        <tr r="G33" s="8"/>
-        <tr r="H34" s="8"/>
-        <tr r="E42" s="8"/>
-        <tr r="J32" s="8"/>
-        <tr r="E41" s="8"/>
-        <tr r="H50" s="8"/>
-        <tr r="I41" s="8"/>
-        <tr r="G43" s="8"/>
-        <tr r="L32" s="8"/>
-        <tr r="J31" s="8"/>
-        <tr r="G39" s="8"/>
-        <tr r="J35" s="8"/>
-        <tr r="J50" s="8"/>
-        <tr r="F49" s="8"/>
-        <tr r="E48" s="8"/>
-        <tr r="E37" s="8"/>
-        <tr r="J46" s="8"/>
-        <tr r="G45" s="8"/>
-        <tr r="I36" s="8"/>
-        <tr r="H31" s="8"/>
-        <tr r="E46" s="8"/>
-        <tr r="L35" s="8"/>
-        <tr r="K51" s="8"/>
-        <tr r="I34" s="8"/>
-        <tr r="L31" s="8"/>
-        <tr r="K39" s="8"/>
-        <tr r="F41" s="8"/>
-        <tr r="E47" s="8"/>
-        <tr r="H43" s="8"/>
-        <tr r="J44" s="8"/>
-        <tr r="G35" s="8"/>
-        <tr r="K46" s="8"/>
-        <tr r="G36" s="8"/>
-        <tr r="F51" s="8"/>
-        <tr r="I37" s="8"/>
-        <tr r="F35" s="8"/>
-        <tr r="I31" s="8"/>
-        <tr r="I32" s="8"/>
-        <tr r="L39" s="8"/>
-        <tr r="F40" s="8"/>
-        <tr r="J43" s="8"/>
-        <tr r="H51" s="8"/>
-        <tr r="K49" s="8"/>
-        <tr r="I44" s="8"/>
-        <tr r="L40" s="8"/>
-        <tr r="E33" s="8"/>
-        <tr r="E36" s="8"/>
-        <tr r="E43" s="8"/>
-        <tr r="F44" s="8"/>
-        <tr r="F38" s="8"/>
-        <tr r="J40" s="8"/>
-        <tr r="K42" s="8"/>
-        <tr r="J42" s="8"/>
-        <tr r="J47" s="8"/>
-        <tr r="F34" s="8"/>
-        <tr r="L51" s="8"/>
-        <tr r="K37" s="8"/>
-        <tr r="I42" s="8"/>
-        <tr r="L38" s="8"/>
-        <tr r="G32" s="8"/>
-        <tr r="F43" s="8"/>
-        <tr r="I35" s="8"/>
-        <tr r="J45" s="8"/>
-        <tr r="F48" s="8"/>
-        <tr r="G49" s="8"/>
-        <tr r="F42" s="8"/>
-        <tr r="I51" s="8"/>
-        <tr r="L41" s="8"/>
-        <tr r="I38" s="8"/>
-        <tr r="H39" s="8"/>
-        <tr r="J41" s="8"/>
-        <tr r="J51" s="8"/>
-        <tr r="K44" s="8"/>
-        <tr r="L42" s="8"/>
-        <tr r="G51" s="8"/>
-        <tr r="L45" s="8"/>
-        <tr r="F37" s="8"/>
-        <tr r="F50" s="8"/>
-        <tr r="K50" s="8"/>
-        <tr r="J37" s="8"/>
-        <tr r="F46" s="8"/>
-        <tr r="H44" s="8"/>
-        <tr r="E45" s="8"/>
-        <tr r="I40" s="8"/>
-        <tr r="K32" s="8"/>
-        <tr r="H38" s="8"/>
-        <tr r="H47" s="8"/>
-        <tr r="E50" s="8"/>
-        <tr r="F31" s="8"/>
-        <tr r="K48" s="8"/>
-        <tr r="E31" s="8"/>
-        <tr r="L37" s="8"/>
-        <tr r="H37" s="8"/>
-        <tr r="K45" s="8"/>
-        <tr r="G34" s="8"/>
-        <tr r="E32" s="8"/>
-        <tr r="H33" s="8"/>
-        <tr r="G46" s="8"/>
-        <tr r="G50" s="8"/>
-        <tr r="K40" s="8"/>
-        <tr r="H46" s="8"/>
-        <tr r="G31" s="8"/>
-        <tr r="L49" s="8"/>
-        <tr r="I49" s="8"/>
-        <tr r="G41" s="8"/>
-        <tr r="G44" s="8"/>
-        <tr r="G37" s="8"/>
-        <tr r="H35" s="8"/>
-        <tr r="K31" s="8"/>
-        <tr r="H42" s="8"/>
-        <tr r="H32" s="8"/>
-        <tr r="K33" s="8"/>
+        <stp>d7709217-a847-4050-bf37-dfa215753290</stp>
+        <tr r="I59" s="9"/>
+        <tr r="I52" s="9"/>
+        <tr r="G54" s="9"/>
+        <tr r="I54" s="9"/>
+        <tr r="J54" s="9"/>
+        <tr r="F54" s="9"/>
+        <tr r="G53" s="9"/>
+        <tr r="G59" s="9"/>
+        <tr r="F57" s="9"/>
+        <tr r="G56" s="9"/>
+        <tr r="F61" s="9"/>
+        <tr r="H55" s="9"/>
+        <tr r="F58" s="9"/>
+        <tr r="G58" s="9"/>
+        <tr r="H52" s="9"/>
+        <tr r="G60" s="9"/>
+        <tr r="H56" s="9"/>
+        <tr r="J57" s="9"/>
+        <tr r="H60" s="9"/>
+        <tr r="J59" s="9"/>
+        <tr r="H61" s="9"/>
+        <tr r="I51" s="9"/>
+        <tr r="I53" s="9"/>
+        <tr r="H54" s="9"/>
+        <tr r="F51" s="9"/>
+        <tr r="F52" s="9"/>
+        <tr r="G55" s="9"/>
+        <tr r="F60" s="9"/>
+        <tr r="H51" s="9"/>
+        <tr r="J52" s="9"/>
+        <tr r="H53" s="9"/>
+        <tr r="F55" s="9"/>
+        <tr r="J55" s="9"/>
+        <tr r="G57" s="9"/>
+        <tr r="J58" s="9"/>
+        <tr r="I58" s="9"/>
+        <tr r="F53" s="9"/>
+        <tr r="H57" s="9"/>
+        <tr r="G52" s="9"/>
+        <tr r="J56" s="9"/>
+        <tr r="I60" s="9"/>
+        <tr r="I57" s="9"/>
+        <tr r="J53" s="9"/>
+        <tr r="I55" s="9"/>
+        <tr r="J51" s="9"/>
+        <tr r="H59" s="9"/>
+        <tr r="I61" s="9"/>
+        <tr r="I56" s="9"/>
+        <tr r="H58" s="9"/>
+        <tr r="F59" s="9"/>
+        <tr r="F56" s="9"/>
+        <tr r="G61" s="9"/>
+        <tr r="G51" s="9"/>
+        <tr r="J61" s="9"/>
+        <tr r="J60" s="9"/>
       </tp>
     </main>
-    <main first="rtdsrv.45f29de5428d4e99882dfebacb0ed41d">
+    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>1ab6ce37-9319-4f23-a32f-d83061e040f7</stp>
+        <stp>e0843967-a1c6-46f8-b426-ef144313232e</stp>
+        <tr r="E47" s="5"/>
+        <tr r="H55" s="5"/>
+        <tr r="F52" s="5"/>
+        <tr r="F49" s="5"/>
+        <tr r="E46" s="5"/>
+        <tr r="H54" s="5"/>
+        <tr r="F53" s="5"/>
+        <tr r="E53" s="5"/>
+        <tr r="E54" s="5"/>
+        <tr r="F47" s="5"/>
+        <tr r="H50" s="5"/>
+        <tr r="E52" s="5"/>
+        <tr r="G54" s="5"/>
+        <tr r="F50" s="5"/>
+        <tr r="E48" s="5"/>
+        <tr r="G51" s="5"/>
+        <tr r="E55" s="5"/>
+        <tr r="F48" s="5"/>
+        <tr r="H51" s="5"/>
+        <tr r="G49" s="5"/>
+        <tr r="F51" s="5"/>
+        <tr r="E51" s="5"/>
+        <tr r="G47" s="5"/>
+        <tr r="H48" s="5"/>
+        <tr r="F54" s="5"/>
         <tr r="G55" s="5"/>
-        <tr r="E46" s="5"/>
-        <tr r="H51" s="5"/>
-        <tr r="E55" s="5"/>
-        <tr r="F51" s="5"/>
-        <tr r="G47" s="5"/>
+        <tr r="G48" s="5"/>
+        <tr r="F46" s="5"/>
+        <tr r="G52" s="5"/>
+        <tr r="E50" s="5"/>
+        <tr r="H46" s="5"/>
+        <tr r="G50" s="5"/>
+        <tr r="H49" s="5"/>
+        <tr r="G53" s="5"/>
+        <tr r="H52" s="5"/>
+        <tr r="E49" s="5"/>
+        <tr r="H47" s="5"/>
+        <tr r="G46" s="5"/>
+        <tr r="F55" s="5"/>
         <tr r="H53" s="5"/>
-        <tr r="F54" s="5"/>
-        <tr r="F49" s="5"/>
-        <tr r="G49" s="5"/>
-        <tr r="F55" s="5"/>
-        <tr r="H49" s="5"/>
-        <tr r="E50" s="5"/>
-        <tr r="H55" s="5"/>
-        <tr r="H54" s="5"/>
-        <tr r="E51" s="5"/>
-        <tr r="G54" s="5"/>
-        <tr r="F47" s="5"/>
-        <tr r="H52" s="5"/>
-        <tr r="H47" s="5"/>
-        <tr r="F50" s="5"/>
-        <tr r="G50" s="5"/>
-        <tr r="E53" s="5"/>
-        <tr r="F46" s="5"/>
-        <tr r="F53" s="5"/>
-        <tr r="G53" s="5"/>
-        <tr r="H46" s="5"/>
-        <tr r="H50" s="5"/>
-        <tr r="E47" s="5"/>
-        <tr r="E48" s="5"/>
-        <tr r="F48" s="5"/>
-        <tr r="G51" s="5"/>
-        <tr r="E49" s="5"/>
-        <tr r="F52" s="5"/>
-        <tr r="G52" s="5"/>
-        <tr r="G48" s="5"/>
-        <tr r="G46" s="5"/>
-        <tr r="H48" s="5"/>
-        <tr r="E52" s="5"/>
-        <tr r="E54" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>5aa3ec71-3ced-4a03-96da-e87baed63a9f</stp>
+        <tr r="L43" s="8"/>
+        <tr r="H42" s="8"/>
+        <tr r="L42" s="8"/>
+        <tr r="G46" s="8"/>
+        <tr r="H35" s="8"/>
+        <tr r="I33" s="8"/>
+        <tr r="K37" s="8"/>
+        <tr r="K39" s="8"/>
+        <tr r="G32" s="8"/>
+        <tr r="H32" s="8"/>
+        <tr r="H31" s="8"/>
+        <tr r="J40" s="8"/>
+        <tr r="J34" s="8"/>
+        <tr r="K46" s="8"/>
+        <tr r="K38" s="8"/>
+        <tr r="E32" s="8"/>
+        <tr r="L36" s="8"/>
+        <tr r="K31" s="8"/>
+        <tr r="H44" s="8"/>
+        <tr r="H39" s="8"/>
+        <tr r="I36" s="8"/>
+        <tr r="K36" s="8"/>
+        <tr r="K35" s="8"/>
+        <tr r="J32" s="8"/>
+        <tr r="E44" s="8"/>
+        <tr r="L46" s="8"/>
+        <tr r="I38" s="8"/>
+        <tr r="L38" s="8"/>
+        <tr r="I39" s="8"/>
+        <tr r="L35" s="8"/>
+        <tr r="G38" s="8"/>
+        <tr r="G44" s="8"/>
+        <tr r="G34" s="8"/>
+        <tr r="F35" s="8"/>
+        <tr r="J45" s="8"/>
+        <tr r="H36" s="8"/>
+        <tr r="G49" s="8"/>
+        <tr r="H46" s="8"/>
+        <tr r="I45" s="8"/>
+        <tr r="F42" s="8"/>
+        <tr r="G31" s="8"/>
+        <tr r="J49" s="8"/>
+        <tr r="J39" s="8"/>
+        <tr r="I37" s="8"/>
+        <tr r="K44" s="8"/>
+        <tr r="J38" s="8"/>
+        <tr r="H51" s="8"/>
+        <tr r="E34" s="8"/>
+        <tr r="I34" s="8"/>
+        <tr r="I49" s="8"/>
+        <tr r="J35" s="8"/>
+        <tr r="L37" s="8"/>
+        <tr r="H45" s="8"/>
+        <tr r="E41" s="8"/>
+        <tr r="G41" s="8"/>
+        <tr r="F37" s="8"/>
+        <tr r="F32" s="8"/>
+        <tr r="F41" s="8"/>
+        <tr r="H41" s="8"/>
+        <tr r="G47" s="8"/>
+        <tr r="E47" s="8"/>
+        <tr r="J41" s="8"/>
+        <tr r="G37" s="8"/>
+        <tr r="F47" s="8"/>
+        <tr r="J43" s="8"/>
+        <tr r="K50" s="8"/>
+        <tr r="H38" s="8"/>
+        <tr r="G40" s="8"/>
+        <tr r="L44" s="8"/>
+        <tr r="J44" s="8"/>
+        <tr r="I46" s="8"/>
+        <tr r="L51" s="8"/>
+        <tr r="L39" s="8"/>
+        <tr r="F36" s="8"/>
+        <tr r="I44" s="8"/>
+        <tr r="E45" s="8"/>
+        <tr r="L50" s="8"/>
+        <tr r="E39" s="8"/>
+        <tr r="G36" s="8"/>
+        <tr r="E38" s="8"/>
+        <tr r="F51" s="8"/>
+        <tr r="J51" s="8"/>
+        <tr r="F45" s="8"/>
+        <tr r="H34" s="8"/>
+        <tr r="E36" s="8"/>
+        <tr r="K32" s="8"/>
+        <tr r="L48" s="8"/>
+        <tr r="J31" s="8"/>
+        <tr r="F44" s="8"/>
+        <tr r="G48" s="8"/>
+        <tr r="I31" s="8"/>
+        <tr r="K33" s="8"/>
+        <tr r="I50" s="8"/>
+        <tr r="K51" s="8"/>
+        <tr r="F48" s="8"/>
+        <tr r="G50" s="8"/>
+        <tr r="L45" s="8"/>
+        <tr r="E49" s="8"/>
+        <tr r="I43" s="8"/>
+        <tr r="H50" s="8"/>
+        <tr r="E50" s="8"/>
+        <tr r="F40" s="8"/>
+        <tr r="F50" s="8"/>
+        <tr r="K34" s="8"/>
+        <tr r="L32" s="8"/>
+        <tr r="E43" s="8"/>
+        <tr r="L33" s="8"/>
+        <tr r="E37" s="8"/>
+        <tr r="F34" s="8"/>
+        <tr r="J37" s="8"/>
+        <tr r="I47" s="8"/>
+        <tr r="K47" s="8"/>
+        <tr r="L31" s="8"/>
+        <tr r="L41" s="8"/>
+        <tr r="K49" s="8"/>
+        <tr r="J50" s="8"/>
+        <tr r="J33" s="8"/>
+        <tr r="L47" s="8"/>
+        <tr r="F49" s="8"/>
+        <tr r="K42" s="8"/>
+        <tr r="I48" s="8"/>
+        <tr r="H40" s="8"/>
+        <tr r="L40" s="8"/>
+        <tr r="I40" s="8"/>
+        <tr r="G33" s="8"/>
+        <tr r="E33" s="8"/>
+        <tr r="G42" s="8"/>
+        <tr r="E48" s="8"/>
+        <tr r="J47" s="8"/>
+        <tr r="K43" s="8"/>
+        <tr r="E46" s="8"/>
+        <tr r="I35" s="8"/>
+        <tr r="E42" s="8"/>
+        <tr r="H47" s="8"/>
+        <tr r="H48" s="8"/>
+        <tr r="K41" s="8"/>
+        <tr r="G35" s="8"/>
+        <tr r="E35" s="8"/>
+        <tr r="G45" s="8"/>
+        <tr r="I42" s="8"/>
+        <tr r="I41" s="8"/>
+        <tr r="F31" s="8"/>
+        <tr r="G43" s="8"/>
+        <tr r="K48" s="8"/>
+        <tr r="F43" s="8"/>
+        <tr r="H33" s="8"/>
+        <tr r="L49" s="8"/>
+        <tr r="E51" s="8"/>
+        <tr r="G39" s="8"/>
+        <tr r="F38" s="8"/>
+        <tr r="E31" s="8"/>
+        <tr r="J36" s="8"/>
+        <tr r="E40" s="8"/>
+        <tr r="I32" s="8"/>
+        <tr r="G51" s="8"/>
+        <tr r="H37" s="8"/>
+        <tr r="J48" s="8"/>
+        <tr r="K40" s="8"/>
+        <tr r="J42" s="8"/>
+        <tr r="H49" s="8"/>
+        <tr r="K45" s="8"/>
+        <tr r="I51" s="8"/>
+        <tr r="F33" s="8"/>
+        <tr r="F39" s="8"/>
+        <tr r="H43" s="8"/>
+        <tr r="J46" s="8"/>
+        <tr r="L34" s="8"/>
+        <tr r="F46" s="8"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>2a6b2658-410f-4dba-a903-c7d17865390c</stp>
+        <stp>be204d21-5288-4369-83fd-5732a4ce920e</stp>
+        <tr r="M32" s="5"/>
+        <tr r="G34" s="5"/>
+        <tr r="F33" s="5"/>
+        <tr r="I33" s="5"/>
+        <tr r="I29" s="5"/>
+        <tr r="M35" s="5"/>
+        <tr r="H32" s="5"/>
+        <tr r="K32" s="5"/>
+        <tr r="E30" s="5"/>
+        <tr r="K30" s="5"/>
+        <tr r="L35" s="5"/>
+        <tr r="I32" s="5"/>
+        <tr r="G29" s="5"/>
+        <tr r="G33" s="5"/>
+        <tr r="E33" s="5"/>
+        <tr r="L29" s="5"/>
+        <tr r="I31" s="5"/>
+        <tr r="F32" s="5"/>
+        <tr r="L31" s="5"/>
+        <tr r="F34" s="5"/>
+        <tr r="H33" s="5"/>
+        <tr r="K31" s="5"/>
+        <tr r="F35" s="5"/>
+        <tr r="E31" s="5"/>
+        <tr r="H29" s="5"/>
+        <tr r="H31" s="5"/>
+        <tr r="L33" s="5"/>
+        <tr r="H30" s="5"/>
+        <tr r="G31" s="5"/>
+        <tr r="E34" s="5"/>
+        <tr r="M33" s="5"/>
+        <tr r="M31" s="5"/>
+        <tr r="M34" s="5"/>
+        <tr r="J33" s="5"/>
+        <tr r="E29" s="5"/>
+        <tr r="E35" s="5"/>
+        <tr r="G32" s="5"/>
+        <tr r="F31" s="5"/>
+        <tr r="I34" s="5"/>
         <tr r="I30" s="5"/>
-        <tr r="H34" s="5"/>
-        <tr r="E30" s="5"/>
-        <tr r="L35" s="5"/>
-        <tr r="L32" s="5"/>
-        <tr r="M35" s="5"/>
-        <tr r="H30" s="5"/>
-        <tr r="I31" s="5"/>
-        <tr r="E35" s="5"/>
-        <tr r="H29" s="5"/>
-        <tr r="F34" s="5"/>
-        <tr r="I35" s="5"/>
-        <tr r="K34" s="5"/>
-        <tr r="J34" s="5"/>
-        <tr r="E33" s="5"/>
-        <tr r="J32" s="5"/>
-        <tr r="K35" s="5"/>
-        <tr r="M33" s="5"/>
-        <tr r="M32" s="5"/>
-        <tr r="G35" s="5"/>
-        <tr r="G29" s="5"/>
-        <tr r="L31" s="5"/>
-        <tr r="F32" s="5"/>
-        <tr r="M34" s="5"/>
-        <tr r="I34" s="5"/>
-        <tr r="L33" s="5"/>
-        <tr r="H33" s="5"/>
-        <tr r="M29" s="5"/>
-        <tr r="F29" s="5"/>
-        <tr r="K30" s="5"/>
-        <tr r="J30" s="5"/>
-        <tr r="I33" s="5"/>
-        <tr r="H32" s="5"/>
-        <tr r="J33" s="5"/>
-        <tr r="F30" s="5"/>
-        <tr r="K31" s="5"/>
-        <tr r="H31" s="5"/>
-        <tr r="M31" s="5"/>
-        <tr r="M30" s="5"/>
-        <tr r="L34" s="5"/>
-        <tr r="L29" s="5"/>
-        <tr r="J29" s="5"/>
-        <tr r="H35" s="5"/>
-        <tr r="F33" s="5"/>
-        <tr r="G33" s="5"/>
-        <tr r="E32" s="5"/>
-        <tr r="F35" s="5"/>
-        <tr r="G30" s="5"/>
-        <tr r="I29" s="5"/>
-        <tr r="E34" s="5"/>
-        <tr r="E29" s="5"/>
-        <tr r="I32" s="5"/>
-        <tr r="K32" s="5"/>
-        <tr r="G32" s="5"/>
         <tr r="K33" s="5"/>
         <tr r="L30" s="5"/>
-        <tr r="F31" s="5"/>
+        <tr r="I35" s="5"/>
+        <tr r="J31" s="5"/>
+        <tr r="K34" s="5"/>
+        <tr r="M30" s="5"/>
+        <tr r="J34" s="5"/>
+        <tr r="L34" s="5"/>
+        <tr r="K35" s="5"/>
+        <tr r="F29" s="5"/>
+        <tr r="J30" s="5"/>
+        <tr r="M29" s="5"/>
+        <tr r="G30" s="5"/>
+        <tr r="H34" s="5"/>
+        <tr r="J32" s="5"/>
+        <tr r="J29" s="5"/>
+        <tr r="L32" s="5"/>
+        <tr r="G35" s="5"/>
+        <tr r="E32" s="5"/>
+        <tr r="K29" s="5"/>
+        <tr r="H35" s="5"/>
         <tr r="J35" s="5"/>
-        <tr r="G34" s="5"/>
-        <tr r="K29" s="5"/>
-        <tr r="E31" s="5"/>
-        <tr r="J31" s="5"/>
-        <tr r="G31" s="5"/>
+        <tr r="F30" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>bee37476-a266-4bc8-a0cc-6d7e84123c46</stp>
+        <tr r="L40" s="13"/>
+        <tr r="E47" s="13"/>
+        <tr r="I49" s="13"/>
+        <tr r="G45" s="13"/>
+        <tr r="N47" s="13"/>
+        <tr r="J45" s="13"/>
+        <tr r="H42" s="13"/>
+        <tr r="J42" s="13"/>
+        <tr r="F40" s="13"/>
+        <tr r="M41" s="13"/>
+        <tr r="J44" s="13"/>
+        <tr r="N49" s="13"/>
+        <tr r="E48" s="13"/>
+        <tr r="F43" s="13"/>
+        <tr r="N42" s="13"/>
+        <tr r="O44" s="13"/>
+        <tr r="J41" s="13"/>
+        <tr r="K42" s="13"/>
+        <tr r="K39" s="13"/>
+        <tr r="E46" s="13"/>
+        <tr r="L45" s="13"/>
+        <tr r="F45" s="13"/>
+        <tr r="E39" s="13"/>
+        <tr r="I40" s="13"/>
+        <tr r="I47" s="13"/>
+        <tr r="J39" s="13"/>
+        <tr r="G42" s="13"/>
+        <tr r="N43" s="13"/>
+        <tr r="G49" s="13"/>
+        <tr r="M40" s="13"/>
+        <tr r="F48" s="13"/>
+        <tr r="J43" s="13"/>
+        <tr r="H39" s="13"/>
+        <tr r="K49" s="13"/>
+        <tr r="F39" s="13"/>
+        <tr r="G41" s="13"/>
+        <tr r="L46" s="13"/>
+        <tr r="E40" s="13"/>
+        <tr r="J48" s="13"/>
+        <tr r="N44" s="13"/>
+        <tr r="O48" s="13"/>
+        <tr r="K44" s="13"/>
+        <tr r="E45" s="13"/>
+        <tr r="G48" s="13"/>
+        <tr r="J47" s="13"/>
+        <tr r="L41" s="13"/>
+        <tr r="O40" s="13"/>
+        <tr r="F44" s="13"/>
+        <tr r="L43" s="13"/>
+        <tr r="F42" s="13"/>
+        <tr r="O49" s="13"/>
+        <tr r="M46" s="13"/>
+        <tr r="K43" s="13"/>
+        <tr r="G46" s="13"/>
+        <tr r="L44" s="13"/>
+        <tr r="F49" s="13"/>
+        <tr r="N46" s="13"/>
+        <tr r="H46" s="13"/>
+        <tr r="I39" s="13"/>
+        <tr r="M49" s="13"/>
+        <tr r="M43" s="13"/>
+        <tr r="L39" s="13"/>
+        <tr r="N45" s="13"/>
+        <tr r="N48" s="13"/>
+        <tr r="H49" s="13"/>
+        <tr r="N41" s="13"/>
+        <tr r="I45" s="13"/>
+        <tr r="I48" s="13"/>
+        <tr r="G44" s="13"/>
+        <tr r="N39" s="13"/>
+        <tr r="J46" s="13"/>
+        <tr r="L42" s="13"/>
+        <tr r="H45" s="13"/>
+        <tr r="O46" s="13"/>
+        <tr r="K46" s="13"/>
+        <tr r="G43" s="13"/>
+        <tr r="O39" s="13"/>
+        <tr r="J49" s="13"/>
+        <tr r="H43" s="13"/>
+        <tr r="H41" s="13"/>
+        <tr r="I43" s="13"/>
+        <tr r="H48" s="13"/>
+        <tr r="H40" s="13"/>
+        <tr r="K40" s="13"/>
+        <tr r="M47" s="13"/>
+        <tr r="I44" s="13"/>
+        <tr r="K45" s="13"/>
+        <tr r="M42" s="13"/>
+        <tr r="K47" s="13"/>
+        <tr r="I42" s="13"/>
+        <tr r="E44" s="13"/>
+        <tr r="H47" s="13"/>
+        <tr r="N40" s="13"/>
+        <tr r="G47" s="13"/>
+        <tr r="O45" s="13"/>
+        <tr r="L48" s="13"/>
+        <tr r="H44" s="13"/>
+        <tr r="L47" s="13"/>
+        <tr r="I41" s="13"/>
+        <tr r="M44" s="13"/>
+        <tr r="K48" s="13"/>
+        <tr r="M45" s="13"/>
+        <tr r="E41" s="13"/>
+        <tr r="G39" s="13"/>
+        <tr r="O42" s="13"/>
+        <tr r="E43" s="13"/>
+        <tr r="E42" s="13"/>
+        <tr r="J40" s="13"/>
+        <tr r="O47" s="13"/>
+        <tr r="O41" s="13"/>
+        <tr r="M39" s="13"/>
+        <tr r="L49" s="13"/>
+        <tr r="E49" s="13"/>
+        <tr r="K41" s="13"/>
+        <tr r="M48" s="13"/>
+        <tr r="F46" s="13"/>
+        <tr r="F47" s="13"/>
+        <tr r="O43" s="13"/>
+        <tr r="I46" s="13"/>
+        <tr r="F41" s="13"/>
+        <tr r="G40" s="13"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.5c3b0217e56b442aa347c26aae01a01e">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>4efa2d5a-daf9-46a2-ac77-af5d0b85d95a</stp>
+        <tr r="G37" s="9"/>
+        <tr r="F31" s="9"/>
+        <tr r="E31" s="9"/>
+        <tr r="E30" s="9"/>
+        <tr r="F34" s="9"/>
+        <tr r="G33" s="9"/>
+        <tr r="E32" s="9"/>
+        <tr r="E35" s="9"/>
+        <tr r="E28" s="9"/>
+        <tr r="G39" s="9"/>
+        <tr r="F33" s="9"/>
+        <tr r="E33" s="9"/>
+        <tr r="F39" s="9"/>
+        <tr r="G31" s="9"/>
+        <tr r="F32" s="9"/>
+        <tr r="G36" s="9"/>
+        <tr r="E39" s="9"/>
+        <tr r="E34" s="9"/>
+        <tr r="E36" s="9"/>
+        <tr r="G30" s="9"/>
+        <tr r="G28" s="9"/>
+        <tr r="F37" s="9"/>
+        <tr r="F29" s="9"/>
+        <tr r="F36" s="9"/>
+        <tr r="G35" s="9"/>
+        <tr r="F28" s="9"/>
+        <tr r="G29" s="9"/>
+        <tr r="E29" s="9"/>
+        <tr r="E37" s="9"/>
+        <tr r="G34" s="9"/>
+        <tr r="F30" s="9"/>
+        <tr r="E38" s="9"/>
+        <tr r="G38" s="9"/>
+        <tr r="G32" s="9"/>
+        <tr r="F38" s="9"/>
+        <tr r="F35" s="9"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>48dde97a-3006-4fd3-85a5-47391d61148a</stp>
-        <tr r="X36" s="6"/>
-        <tr r="AH35" s="6"/>
-        <tr r="O43" s="6"/>
-        <tr r="O33" s="6"/>
-        <tr r="V40" s="6"/>
-        <tr r="K45" s="6"/>
-        <tr r="AC42" s="6"/>
-        <tr r="G45" s="6"/>
-        <tr r="H42" s="6"/>
-        <tr r="AF42" s="6"/>
-        <tr r="AF49" s="6"/>
-        <tr r="G49" s="6"/>
-        <tr r="AA40" s="6"/>
-        <tr r="I47" s="6"/>
-        <tr r="J52" s="6"/>
-        <tr r="AE37" s="6"/>
-        <tr r="AE42" s="6"/>
-        <tr r="AG45" s="6"/>
-        <tr r="E52" s="6"/>
-        <tr r="AH33" s="6"/>
-        <tr r="AG34" s="6"/>
-        <tr r="AH50" s="6"/>
-        <tr r="N33" s="6"/>
-        <tr r="R47" s="6"/>
-        <tr r="AC41" s="6"/>
-        <tr r="Z34" s="6"/>
-        <tr r="Y51" s="6"/>
-        <tr r="T43" s="6"/>
-        <tr r="E40" s="6"/>
-        <tr r="G51" s="6"/>
-        <tr r="AD36" s="6"/>
-        <tr r="AE50" s="6"/>
-        <tr r="X48" s="6"/>
-        <tr r="X42" s="6"/>
-        <tr r="E37" s="6"/>
-        <tr r="AH41" s="6"/>
-        <tr r="AA33" s="6"/>
-        <tr r="K48" s="6"/>
-        <tr r="F36" s="6"/>
-        <tr r="AD42" s="6"/>
-        <tr r="Y39" s="6"/>
-        <tr r="L35" s="6"/>
-        <tr r="AE47" s="6"/>
-        <tr r="AB37" s="6"/>
-        <tr r="AG52" s="6"/>
-        <tr r="N51" s="6"/>
-        <tr r="R37" s="6"/>
-        <tr r="X51" s="6"/>
-        <tr r="J47" s="6"/>
-        <tr r="O34" s="6"/>
-        <tr r="X39" s="6"/>
-        <tr r="AD50" s="6"/>
-        <tr r="AD43" s="6"/>
-        <tr r="I48" s="6"/>
-        <tr r="U41" s="6"/>
-        <tr r="AF47" s="6"/>
-        <tr r="Q38" s="6"/>
-        <tr r="K47" s="6"/>
-        <tr r="G50" s="6"/>
-        <tr r="P39" s="6"/>
-        <tr r="AC39" s="6"/>
-        <tr r="AB33" s="6"/>
-        <tr r="AC44" s="6"/>
-        <tr r="AB52" s="6"/>
-        <tr r="V46" s="6"/>
-        <tr r="H46" s="6"/>
-        <tr r="AH43" s="6"/>
-        <tr r="R46" s="6"/>
-        <tr r="E33" s="6"/>
-        <tr r="M40" s="6"/>
-        <tr r="L50" s="6"/>
-        <tr r="H50" s="6"/>
-        <tr r="P50" s="6"/>
-        <tr r="E39" s="6"/>
-        <tr r="AA34" s="6"/>
-        <tr r="E43" s="6"/>
-        <tr r="J45" s="6"/>
-        <tr r="S46" s="6"/>
-        <tr r="P44" s="6"/>
-        <tr r="W50" s="6"/>
-        <tr r="AC40" s="6"/>
-        <tr r="X46" s="6"/>
-        <tr r="Q33" s="6"/>
-        <tr r="V35" s="6"/>
-        <tr r="AC36" s="6"/>
-        <tr r="R49" s="6"/>
-        <tr r="AF51" s="6"/>
-        <tr r="R38" s="6"/>
-        <tr r="F35" s="6"/>
-        <tr r="AF45" s="6"/>
-        <tr r="AH36" s="6"/>
-        <tr r="F48" s="6"/>
-        <tr r="K36" s="6"/>
-        <tr r="H43" s="6"/>
-        <tr r="AE43" s="6"/>
-        <tr r="U34" s="6"/>
-        <tr r="K50" s="6"/>
-        <tr r="I33" s="6"/>
-        <tr r="U42" s="6"/>
-        <tr r="N44" s="6"/>
-        <tr r="Y45" s="6"/>
-        <tr r="R40" s="6"/>
-        <tr r="U51" s="6"/>
-        <tr r="AA42" s="6"/>
-        <tr r="N47" s="6"/>
-        <tr r="AH44" s="6"/>
-        <tr r="Y47" s="6"/>
-        <tr r="T33" s="6"/>
-        <tr r="W52" s="6"/>
-        <tr r="AA43" s="6"/>
-        <tr r="L43" s="6"/>
-        <tr r="P51" s="6"/>
-        <tr r="J46" s="6"/>
-        <tr r="L45" s="6"/>
-        <tr r="P33" s="6"/>
-        <tr r="H38" s="6"/>
-        <tr r="N38" s="6"/>
-        <tr r="X37" s="6"/>
-        <tr r="N37" s="6"/>
-        <tr r="N48" s="6"/>
-        <tr r="Y38" s="6"/>
-        <tr r="T44" s="6"/>
-        <tr r="K40" s="6"/>
-        <tr r="G38" s="6"/>
-        <tr r="T39" s="6"/>
-        <tr r="I41" s="6"/>
-        <tr r="M47" s="6"/>
-        <tr r="AE39" s="6"/>
-        <tr r="U40" s="6"/>
-        <tr r="Q43" s="6"/>
-        <tr r="M48" s="6"/>
-        <tr r="S35" s="6"/>
-        <tr r="H47" s="6"/>
-        <tr r="W51" s="6"/>
-        <tr r="AB34" s="6"/>
-        <tr r="AF41" s="6"/>
-        <tr r="AH46" s="6"/>
-        <tr r="AB45" s="6"/>
-        <tr r="K37" s="6"/>
-        <tr r="Q46" s="6"/>
-        <tr r="Y44" s="6"/>
-        <tr r="K43" s="6"/>
-        <tr r="AH49" s="6"/>
-        <tr r="Z44" s="6"/>
-        <tr r="Z41" s="6"/>
-        <tr r="H48" s="6"/>
-        <tr r="S33" s="6"/>
-        <tr r="W40" s="6"/>
-        <tr r="U39" s="6"/>
-        <tr r="O36" s="6"/>
-        <tr r="J44" s="6"/>
-        <tr r="R33" s="6"/>
-        <tr r="AC38" s="6"/>
-        <tr r="S52" s="6"/>
-        <tr r="AF37" s="6"/>
-        <tr r="AC52" s="6"/>
-        <tr r="Z35" s="6"/>
-        <tr r="AH34" s="6"/>
-        <tr r="Z38" s="6"/>
-        <tr r="AE48" s="6"/>
-        <tr r="W45" s="6"/>
-        <tr r="X52" s="6"/>
-        <tr r="V47" s="6"/>
-        <tr r="J49" s="6"/>
-        <tr r="H36" s="6"/>
-        <tr r="V37" s="6"/>
-        <tr r="N40" s="6"/>
-        <tr r="P38" s="6"/>
-        <tr r="F40" s="6"/>
-        <tr r="K52" s="6"/>
-        <tr r="J51" s="6"/>
-        <tr r="E49" s="6"/>
-        <tr r="AC48" s="6"/>
-        <tr r="AH42" s="6"/>
-        <tr r="G37" s="6"/>
-        <tr r="S40" s="6"/>
-        <tr r="AA44" s="6"/>
-        <tr r="M41" s="6"/>
-        <tr r="AF36" s="6"/>
-        <tr r="E48" s="6"/>
-        <tr r="H34" s="6"/>
-        <tr r="AC33" s="6"/>
-        <tr r="AG41" s="6"/>
-        <tr r="X45" s="6"/>
-        <tr r="H33" s="6"/>
-        <tr r="AA39" s="6"/>
-        <tr r="AA50" s="6"/>
-        <tr r="G42" s="6"/>
-        <tr r="AE36" s="6"/>
-        <tr r="G39" s="6"/>
-        <tr r="AD38" s="6"/>
-        <tr r="F37" s="6"/>
-        <tr r="G52" s="6"/>
-        <tr r="U45" s="6"/>
-        <tr r="S50" s="6"/>
-        <tr r="Y40" s="6"/>
-        <tr r="H41" s="6"/>
-        <tr r="R43" s="6"/>
-        <tr r="AC50" s="6"/>
-        <tr r="F42" s="6"/>
-        <tr r="I43" s="6"/>
-        <tr r="AC49" s="6"/>
-        <tr r="Z40" s="6"/>
-        <tr r="Z52" s="6"/>
-        <tr r="E35" s="6"/>
-        <tr r="AG48" s="6"/>
-        <tr r="T46" s="6"/>
-        <tr r="L36" s="6"/>
-        <tr r="AG35" s="6"/>
-        <tr r="I50" s="6"/>
-        <tr r="X34" s="6"/>
-        <tr r="X50" s="6"/>
-        <tr r="AD33" s="6"/>
-        <tr r="U44" s="6"/>
-        <tr r="AF33" s="6"/>
-        <tr r="T37" s="6"/>
-        <tr r="F41" s="6"/>
-        <tr r="E45" s="6"/>
-        <tr r="N50" s="6"/>
-        <tr r="Q41" s="6"/>
-        <tr r="AG50" s="6"/>
-        <tr r="W41" s="6"/>
-        <tr r="Q51" s="6"/>
-        <tr r="W34" s="6"/>
-        <tr r="AC45" s="6"/>
-        <tr r="AA45" s="6"/>
-        <tr r="AB36" s="6"/>
-        <tr r="X38" s="6"/>
-        <tr r="AG49" s="6"/>
-        <tr r="J50" s="6"/>
-        <tr r="AF40" s="6"/>
-        <tr r="N35" s="6"/>
-        <tr r="AF50" s="6"/>
-        <tr r="O44" s="6"/>
-        <tr r="L44" s="6"/>
-        <tr r="O47" s="6"/>
-        <tr r="P35" s="6"/>
-        <tr r="I35" s="6"/>
-        <tr r="P37" s="6"/>
-        <tr r="X41" s="6"/>
-        <tr r="AE38" s="6"/>
-        <tr r="J41" s="6"/>
-        <tr r="V48" s="6"/>
-        <tr r="F33" s="6"/>
-        <tr r="R42" s="6"/>
-        <tr r="AC35" s="6"/>
-        <tr r="W39" s="6"/>
-        <tr r="E38" s="6"/>
-        <tr r="V34" s="6"/>
-        <tr r="AE35" s="6"/>
-        <tr r="I42" s="6"/>
-        <tr r="AC47" s="6"/>
-        <tr r="H40" s="6"/>
-        <tr r="Y48" s="6"/>
-        <tr r="AG33" s="6"/>
-        <tr r="I37" s="6"/>
-        <tr r="T51" s="6"/>
-        <tr r="I49" s="6"/>
-        <tr r="S42" s="6"/>
-        <tr r="L47" s="6"/>
-        <tr r="Z47" s="6"/>
-        <tr r="AD39" s="6"/>
-        <tr r="G41" s="6"/>
-        <tr r="H37" s="6"/>
-        <tr r="Q36" s="6"/>
-        <tr r="AD35" s="6"/>
-        <tr r="AE34" s="6"/>
-        <tr r="M37" s="6"/>
-        <tr r="X47" s="6"/>
-        <tr r="AA38" s="6"/>
-        <tr r="AG36" s="6"/>
-        <tr r="K46" s="6"/>
-        <tr r="AC37" s="6"/>
-        <tr r="Y43" s="6"/>
-        <tr r="AE33" s="6"/>
-        <tr r="F47" s="6"/>
-        <tr r="I46" s="6"/>
-        <tr r="H44" s="6"/>
-        <tr r="O45" s="6"/>
-        <tr r="U33" s="6"/>
-        <tr r="P46" s="6"/>
-        <tr r="U49" s="6"/>
-        <tr r="T34" s="6"/>
-        <tr r="U36" s="6"/>
-        <tr r="P42" s="6"/>
-        <tr r="P48" s="6"/>
-        <tr r="Q50" s="6"/>
-        <tr r="O50" s="6"/>
-        <tr r="K34" s="6"/>
-        <tr r="R48" s="6"/>
-        <tr r="F34" s="6"/>
-        <tr r="J42" s="6"/>
-        <tr r="AH37" s="6"/>
-        <tr r="AD46" s="6"/>
-        <tr r="S41" s="6"/>
-        <tr r="W48" s="6"/>
-        <tr r="AC34" s="6"/>
-        <tr r="S37" s="6"/>
-        <tr r="Y50" s="6"/>
-        <tr r="T52" s="6"/>
-        <tr r="L46" s="6"/>
-        <tr r="V51" s="6"/>
-        <tr r="Y42" s="6"/>
-        <tr r="AA46" s="6"/>
-        <tr r="Q44" s="6"/>
-        <tr r="W43" s="6"/>
-        <tr r="V36" s="6"/>
-        <tr r="W49" s="6"/>
-        <tr r="AE40" s="6"/>
-        <tr r="K51" s="6"/>
-        <tr r="M50" s="6"/>
-        <tr r="V49" s="6"/>
-        <tr r="X44" s="6"/>
-        <tr r="AC51" s="6"/>
-        <tr r="AD48" s="6"/>
-        <tr r="U52" s="6"/>
-        <tr r="AF43" s="6"/>
-        <tr r="AE46" s="6"/>
-        <tr r="M36" s="6"/>
-        <tr r="Q49" s="6"/>
-        <tr r="Z51" s="6"/>
-        <tr r="M45" s="6"/>
-        <tr r="T48" s="6"/>
-        <tr r="AD51" s="6"/>
-        <tr r="V43" s="6"/>
-        <tr r="E41" s="6"/>
-        <tr r="Q47" s="6"/>
-        <tr r="R52" s="6"/>
-        <tr r="H52" s="6"/>
-        <tr r="R34" s="6"/>
-        <tr r="N46" s="6"/>
-        <tr r="K49" s="6"/>
-        <tr r="P36" s="6"/>
-        <tr r="AG46" s="6"/>
-        <tr r="O42" s="6"/>
-        <tr r="AA37" s="6"/>
-        <tr r="Q40" s="6"/>
-        <tr r="Q39" s="6"/>
-        <tr r="S36" s="6"/>
-        <tr r="Y41" s="6"/>
-        <tr r="AH39" s="6"/>
-        <tr r="AH48" s="6"/>
-        <tr r="E42" s="6"/>
-        <tr r="R44" s="6"/>
-        <tr r="L51" s="6"/>
-        <tr r="T41" s="6"/>
-        <tr r="G35" s="6"/>
-        <tr r="AG44" s="6"/>
-        <tr r="T47" s="6"/>
-        <tr r="G47" s="6"/>
-        <tr r="M38" s="6"/>
-        <tr r="AB47" s="6"/>
-        <tr r="Q48" s="6"/>
-        <tr r="AH40" s="6"/>
-        <tr r="N39" s="6"/>
-        <tr r="Y37" s="6"/>
-        <tr r="AB38" s="6"/>
-        <tr r="I40" s="6"/>
-        <tr r="Z49" s="6"/>
-        <tr r="AA48" s="6"/>
-        <tr r="G36" s="6"/>
-        <tr r="Y34" s="6"/>
-        <tr r="O41" s="6"/>
-        <tr r="AA52" s="6"/>
-        <tr r="O52" s="6"/>
-        <tr r="AF35" s="6"/>
-        <tr r="R36" s="6"/>
-        <tr r="AB44" s="6"/>
-        <tr r="AA47" s="6"/>
-        <tr r="L49" s="6"/>
-        <tr r="K38" s="6"/>
-        <tr r="W44" s="6"/>
-        <tr r="AB50" s="6"/>
-        <tr r="W33" s="6"/>
-        <tr r="N45" s="6"/>
-        <tr r="AH45" s="6"/>
-        <tr r="U48" s="6"/>
-        <tr r="I36" s="6"/>
-        <tr r="AB51" s="6"/>
-        <tr r="P49" s="6"/>
-        <tr r="R39" s="6"/>
-        <tr r="X49" s="6"/>
-        <tr r="AG42" s="6"/>
-        <tr r="AB48" s="6"/>
-        <tr r="O37" s="6"/>
-        <tr r="AA41" s="6"/>
-        <tr r="V39" s="6"/>
-        <tr r="M52" s="6"/>
-        <tr r="P41" s="6"/>
-        <tr r="Z36" s="6"/>
-        <tr r="AE44" s="6"/>
-        <tr r="E44" s="6"/>
-        <tr r="T38" s="6"/>
-        <tr r="F39" s="6"/>
-        <tr r="AH38" s="6"/>
-        <tr r="J35" s="6"/>
-        <tr r="U50" s="6"/>
-        <tr r="M35" s="6"/>
-        <tr r="O39" s="6"/>
-        <tr r="Q42" s="6"/>
-        <tr r="AH47" s="6"/>
-        <tr r="Z50" s="6"/>
-        <tr r="S47" s="6"/>
-        <tr r="Q52" s="6"/>
-        <tr r="N34" s="6"/>
-        <tr r="AB39" s="6"/>
-        <tr r="AC43" s="6"/>
-        <tr r="J37" s="6"/>
-        <tr r="E34" s="6"/>
-        <tr r="W37" s="6"/>
-        <tr r="J43" s="6"/>
-        <tr r="F38" s="6"/>
-        <tr r="W46" s="6"/>
-        <tr r="H51" s="6"/>
-        <tr r="V38" s="6"/>
-        <tr r="G40" s="6"/>
-        <tr r="M34" s="6"/>
-        <tr r="AB42" s="6"/>
-        <tr r="S45" s="6"/>
-        <tr r="F46" s="6"/>
-        <tr r="F51" s="6"/>
-        <tr r="AD52" s="6"/>
-        <tr r="T45" s="6"/>
-        <tr r="N36" s="6"/>
-        <tr r="W47" s="6"/>
-        <tr r="E46" s="6"/>
-        <tr r="K41" s="6"/>
-        <tr r="V42" s="6"/>
-        <tr r="AB41" s="6"/>
-        <tr r="Z43" s="6"/>
-        <tr r="S43" s="6"/>
-        <tr r="AE45" s="6"/>
-        <tr r="I34" s="6"/>
-        <tr r="W38" s="6"/>
-        <tr r="E36" s="6"/>
-        <tr r="O38" s="6"/>
-        <tr r="AB35" s="6"/>
-        <tr r="L34" s="6"/>
-        <tr r="I51" s="6"/>
-        <tr r="F49" s="6"/>
-        <tr r="R51" s="6"/>
-        <tr r="Z39" s="6"/>
-        <tr r="E50" s="6"/>
-        <tr r="S38" s="6"/>
-        <tr r="P43" s="6"/>
-        <tr r="AB49" s="6"/>
-        <tr r="K35" s="6"/>
-        <tr r="G34" s="6"/>
-        <tr r="AG51" s="6"/>
-        <tr r="P34" s="6"/>
-        <tr r="W42" s="6"/>
-        <tr r="AD41" s="6"/>
-        <tr r="U47" s="6"/>
-        <tr r="Y33" s="6"/>
-        <tr r="Y49" s="6"/>
-        <tr r="AB40" s="6"/>
-        <tr r="H39" s="6"/>
-        <tr r="U46" s="6"/>
-        <tr r="G48" s="6"/>
-        <tr r="AE41" s="6"/>
-        <tr r="H45" s="6"/>
-        <tr r="T40" s="6"/>
-        <tr r="G46" s="6"/>
-        <tr r="F52" s="6"/>
-        <tr r="K42" s="6"/>
-        <tr r="AF38" s="6"/>
-        <tr r="AF39" s="6"/>
-        <tr r="N42" s="6"/>
-        <tr r="I45" s="6"/>
-        <tr r="AF34" s="6"/>
-        <tr r="Y36" s="6"/>
-        <tr r="V44" s="6"/>
-        <tr r="F43" s="6"/>
-        <tr r="Z48" s="6"/>
-        <tr r="J38" s="6"/>
-        <tr r="S34" s="6"/>
-        <tr r="AD34" s="6"/>
-        <tr r="R45" s="6"/>
-        <tr r="AC46" s="6"/>
-        <tr r="G43" s="6"/>
-        <tr r="J39" s="6"/>
-        <tr r="AA49" s="6"/>
-        <tr r="L41" s="6"/>
-        <tr r="AH51" s="6"/>
-        <tr r="W36" s="6"/>
-        <tr r="J48" s="6"/>
-        <tr r="T35" s="6"/>
-        <tr r="R41" s="6"/>
-        <tr r="AD44" s="6"/>
-        <tr r="AF52" s="6"/>
-        <tr r="AG37" s="6"/>
-        <tr r="Y46" s="6"/>
-        <tr r="I39" s="6"/>
-        <tr r="Q37" s="6"/>
-        <tr r="T36" s="6"/>
-        <tr r="U37" s="6"/>
-        <tr r="V33" s="6"/>
-        <tr r="AA36" s="6"/>
-        <tr r="P45" s="6"/>
-        <tr r="L37" s="6"/>
-        <tr r="Y52" s="6"/>
-        <tr r="AG43" s="6"/>
-        <tr r="F50" s="6"/>
-        <tr r="L33" s="6"/>
-        <tr r="W35" s="6"/>
-        <tr r="L39" s="6"/>
-        <tr r="X33" s="6"/>
-        <tr r="Q45" s="6"/>
-        <tr r="O48" s="6"/>
-        <tr r="K33" s="6"/>
-        <tr r="AD40" s="6"/>
-        <tr r="M49" s="6"/>
-        <tr r="X40" s="6"/>
-        <tr r="G33" s="6"/>
-        <tr r="S39" s="6"/>
-        <tr r="AD37" s="6"/>
-        <tr r="E51" s="6"/>
-        <tr r="O40" s="6"/>
-        <tr r="Z42" s="6"/>
-        <tr r="S51" s="6"/>
-        <tr r="AF48" s="6"/>
-        <tr r="V52" s="6"/>
-        <tr r="P47" s="6"/>
-        <tr r="Z46" s="6"/>
-        <tr r="P52" s="6"/>
-        <tr r="M39" s="6"/>
-        <tr r="T49" s="6"/>
-        <tr r="G44" s="6"/>
-        <tr r="R50" s="6"/>
-        <tr r="N43" s="6"/>
-        <tr r="U35" s="6"/>
-        <tr r="F45" s="6"/>
-        <tr r="V45" s="6"/>
-        <tr r="J40" s="6"/>
-        <tr r="M42" s="6"/>
-        <tr r="AA35" s="6"/>
-        <tr r="O35" s="6"/>
-        <tr r="H49" s="6"/>
-        <tr r="M44" s="6"/>
-        <tr r="N49" s="6"/>
-        <tr r="AG47" s="6"/>
-        <tr r="S48" s="6"/>
-        <tr r="M43" s="6"/>
-        <tr r="AE52" s="6"/>
-        <tr r="N41" s="6"/>
-        <tr r="Z33" s="6"/>
-        <tr r="P40" s="6"/>
-        <tr r="AD49" s="6"/>
-        <tr r="AD47" s="6"/>
-        <tr r="AH52" s="6"/>
-        <tr r="AA51" s="6"/>
-        <tr r="U43" s="6"/>
-        <tr r="AB46" s="6"/>
-        <tr r="K44" s="6"/>
-        <tr r="E47" s="6"/>
-        <tr r="Q34" s="6"/>
-        <tr r="M46" s="6"/>
-        <tr r="N52" s="6"/>
-        <tr r="L42" s="6"/>
-        <tr r="U38" s="6"/>
-        <tr r="H35" s="6"/>
-        <tr r="S49" s="6"/>
-        <tr r="O51" s="6"/>
-        <tr r="L40" s="6"/>
-        <tr r="AF46" s="6"/>
-        <tr r="Y35" s="6"/>
-        <tr r="K39" s="6"/>
-        <tr r="I38" s="6"/>
-        <tr r="L52" s="6"/>
-        <tr r="X35" s="6"/>
-        <tr r="O49" s="6"/>
-        <tr r="F44" s="6"/>
-        <tr r="AB43" s="6"/>
-        <tr r="AG39" s="6"/>
-        <tr r="L38" s="6"/>
-        <tr r="V50" s="6"/>
-        <tr r="I52" s="6"/>
-        <tr r="Q35" s="6"/>
-        <tr r="S44" s="6"/>
-        <tr r="O46" s="6"/>
-        <tr r="V41" s="6"/>
-        <tr r="AG40" s="6"/>
-        <tr r="AE49" s="6"/>
-        <tr r="J34" s="6"/>
-        <tr r="M33" s="6"/>
-        <tr r="Z45" s="6"/>
-        <tr r="I44" s="6"/>
-        <tr r="AD45" s="6"/>
-        <tr r="Z37" s="6"/>
-        <tr r="AG38" s="6"/>
-        <tr r="AE51" s="6"/>
-        <tr r="T42" s="6"/>
-        <tr r="AF44" s="6"/>
-        <tr r="J33" s="6"/>
-        <tr r="M51" s="6"/>
-        <tr r="J36" s="6"/>
-        <tr r="R35" s="6"/>
-        <tr r="X43" s="6"/>
-        <tr r="T50" s="6"/>
-        <tr r="L48" s="6"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.45f29de5428d4e99882dfebacb0ed41d">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>ecfe3379-a858-4a76-8c7a-cdada848b15e</stp>
+        <stp>1aa3071f-32df-4618-96c7-f7e8977e8cd4</stp>
+        <tr r="D15" s="7"/>
+        <tr r="D20" s="7"/>
+        <tr r="D25" s="7"/>
+        <tr r="D17" s="7"/>
+        <tr r="D22" s="7"/>
+        <tr r="D19" s="7"/>
+        <tr r="D16" s="7"/>
+        <tr r="D18" s="7"/>
         <tr r="D24" s="7"/>
-        <tr r="D15" s="7"/>
         <tr r="D23" s="7"/>
         <tr r="D21" s="7"/>
-        <tr r="D20" s="7"/>
-        <tr r="D22" s="7"/>
-        <tr r="D16" s="7"/>
-        <tr r="D18" s="7"/>
-        <tr r="D19" s="7"/>
-        <tr r="D25" s="7"/>
-        <tr r="D17" s="7"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.45f29de5428d4e99882dfebacb0ed41d">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>d2c43cf1-7535-453c-9743-cf98a9b8c267</stp>
-        <tr r="E38" s="9"/>
-        <tr r="G32" s="9"/>
-        <tr r="E34" s="9"/>
-        <tr r="G37" s="9"/>
-        <tr r="G28" s="9"/>
-        <tr r="F30" s="9"/>
-        <tr r="E35" s="9"/>
-        <tr r="F33" s="9"/>
-        <tr r="E36" s="9"/>
-        <tr r="E39" s="9"/>
-        <tr r="G31" s="9"/>
-        <tr r="G30" s="9"/>
-        <tr r="E33" s="9"/>
-        <tr r="E29" s="9"/>
-        <tr r="E30" s="9"/>
-        <tr r="G29" s="9"/>
-        <tr r="G33" s="9"/>
-        <tr r="G39" s="9"/>
-        <tr r="E32" s="9"/>
-        <tr r="E37" s="9"/>
-        <tr r="F31" s="9"/>
-        <tr r="G35" s="9"/>
-        <tr r="G36" s="9"/>
-        <tr r="G34" s="9"/>
-        <tr r="F38" s="9"/>
-        <tr r="F32" s="9"/>
-        <tr r="F34" s="9"/>
-        <tr r="F29" s="9"/>
-        <tr r="E31" s="9"/>
-        <tr r="F36" s="9"/>
-        <tr r="F39" s="9"/>
-        <tr r="E28" s="9"/>
-        <tr r="F37" s="9"/>
-        <tr r="F35" s="9"/>
-        <tr r="G38" s="9"/>
-        <tr r="F28" s="9"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.45f29de5428d4e99882dfebacb0ed41d">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>5bdea107-be5d-4701-b1f4-052530db2353</stp>
-        <tr r="E39" s="13"/>
-        <tr r="F48" s="13"/>
-        <tr r="K43" s="13"/>
-        <tr r="M43" s="13"/>
-        <tr r="L44" s="13"/>
-        <tr r="K46" s="13"/>
-        <tr r="G43" s="13"/>
-        <tr r="E48" s="13"/>
-        <tr r="J47" s="13"/>
-        <tr r="K42" s="13"/>
-        <tr r="I39" s="13"/>
-        <tr r="E44" s="13"/>
-        <tr r="N49" s="13"/>
-        <tr r="G42" s="13"/>
-        <tr r="O40" s="13"/>
-        <tr r="I40" s="13"/>
-        <tr r="E41" s="13"/>
-        <tr r="I44" s="13"/>
-        <tr r="H48" s="13"/>
-        <tr r="E46" s="13"/>
-        <tr r="K47" s="13"/>
-        <tr r="J45" s="13"/>
-        <tr r="N45" s="13"/>
-        <tr r="J48" s="13"/>
-        <tr r="G49" s="13"/>
-        <tr r="O39" s="13"/>
-        <tr r="J40" s="13"/>
-        <tr r="O42" s="13"/>
-        <tr r="G45" s="13"/>
-        <tr r="O48" s="13"/>
-        <tr r="K44" s="13"/>
-        <tr r="N48" s="13"/>
-        <tr r="F49" s="13"/>
-        <tr r="F44" s="13"/>
-        <tr r="K39" s="13"/>
-        <tr r="H49" s="13"/>
-        <tr r="G47" s="13"/>
-        <tr r="N41" s="13"/>
-        <tr r="E40" s="13"/>
-        <tr r="E49" s="13"/>
-        <tr r="O41" s="13"/>
-        <tr r="L40" s="13"/>
-        <tr r="K49" s="13"/>
-        <tr r="H39" s="13"/>
-        <tr r="F40" s="13"/>
-        <tr r="L48" s="13"/>
-        <tr r="M42" s="13"/>
-        <tr r="O43" s="13"/>
-        <tr r="M48" s="13"/>
-        <tr r="I47" s="13"/>
-        <tr r="I43" s="13"/>
-        <tr r="N40" s="13"/>
-        <tr r="H41" s="13"/>
-        <tr r="F41" s="13"/>
-        <tr r="J44" s="13"/>
-        <tr r="G44" s="13"/>
-        <tr r="M40" s="13"/>
-        <tr r="F45" s="13"/>
-        <tr r="J49" s="13"/>
-        <tr r="M47" s="13"/>
-        <tr r="O45" s="13"/>
-        <tr r="E47" s="13"/>
-        <tr r="H45" s="13"/>
-        <tr r="M45" s="13"/>
-        <tr r="N44" s="13"/>
-        <tr r="M46" s="13"/>
-        <tr r="G41" s="13"/>
-        <tr r="L39" s="13"/>
-        <tr r="N43" s="13"/>
-        <tr r="N39" s="13"/>
-        <tr r="H46" s="13"/>
-        <tr r="K40" s="13"/>
-        <tr r="G48" s="13"/>
-        <tr r="E42" s="13"/>
-        <tr r="G39" s="13"/>
-        <tr r="J46" s="13"/>
-        <tr r="M49" s="13"/>
-        <tr r="H47" s="13"/>
-        <tr r="O49" s="13"/>
-        <tr r="J39" s="13"/>
-        <tr r="F39" s="13"/>
-        <tr r="L49" s="13"/>
-        <tr r="O47" s="13"/>
-        <tr r="E43" s="13"/>
-        <tr r="I42" s="13"/>
-        <tr r="H42" s="13"/>
-        <tr r="J42" s="13"/>
-        <tr r="M39" s="13"/>
-        <tr r="N47" s="13"/>
-        <tr r="H40" s="13"/>
-        <tr r="F47" s="13"/>
-        <tr r="K41" s="13"/>
-        <tr r="F46" s="13"/>
-        <tr r="L42" s="13"/>
-        <tr r="J41" s="13"/>
-        <tr r="M41" s="13"/>
-        <tr r="H43" s="13"/>
-        <tr r="K45" s="13"/>
-        <tr r="I41" s="13"/>
-        <tr r="I46" s="13"/>
-        <tr r="G40" s="13"/>
-        <tr r="J43" s="13"/>
-        <tr r="E45" s="13"/>
-        <tr r="N46" s="13"/>
-        <tr r="K48" s="13"/>
-        <tr r="L41" s="13"/>
-        <tr r="I45" s="13"/>
-        <tr r="F43" s="13"/>
-        <tr r="M44" s="13"/>
-        <tr r="O44" s="13"/>
-        <tr r="L43" s="13"/>
-        <tr r="L45" s="13"/>
-        <tr r="I48" s="13"/>
-        <tr r="F42" s="13"/>
-        <tr r="H44" s="13"/>
-        <tr r="I49" s="13"/>
-        <tr r="N42" s="13"/>
-        <tr r="O46" s="13"/>
-        <tr r="G46" s="13"/>
-        <tr r="L46" s="13"/>
-        <tr r="L47" s="13"/>
       </tp>
     </main>
   </volType>
@@ -3402,7 +3411,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>705972</xdr:colOff>
+      <xdr:colOff>705973</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>6562</xdr:rowOff>
     </xdr:to>
@@ -4401,7 +4410,7 @@
   <dimension ref="B1:N37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4726,7 +4735,7 @@
       <c r="J19" s="18"/>
       <c r="K19" s="31"/>
       <c r="L19" s="16"/>
-      <c r="M19" s="29" t="str">
+      <c r="M19" s="98" t="str">
         <f>_xll.flPortfoliosAdd(F15,E18:L19)</f>
         <v>Error creating portfolio with id Global-Equity in scope Finbourne-Examples effective at 2019-04-10T00:00:00.0000000+00:00 because it already exists.</v>
       </c>
@@ -6343,7 +6352,7 @@
   <dimension ref="B1:S92"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6852,10 +6861,10 @@
         <v>Finbourne-Examples</v>
       </c>
       <c r="G30" s="29" t="str">
-        <v>US-Corporate-Bond</v>
+        <v>US-Treasury-Bond</v>
       </c>
       <c r="H30" s="29" t="str">
-        <v>US Corporate Bond Fund</v>
+        <v>US$ Treasury Bond Fund</v>
       </c>
       <c r="I30" s="30">
         <v>0</v>
@@ -6888,10 +6897,10 @@
         <v>Finbourne-Examples</v>
       </c>
       <c r="G31" s="29" t="str">
-        <v>US-Treasury-Bond</v>
+        <v>Global-Equity</v>
       </c>
       <c r="H31" s="29" t="str">
-        <v>US$ Treasury Bond Fund</v>
+        <v>Global Equity Fund</v>
       </c>
       <c r="I31" s="30">
         <v>0</v>
@@ -6960,10 +6969,10 @@
         <v>Finbourne-Examples</v>
       </c>
       <c r="G33" s="29" t="str">
-        <v>Global-Equity</v>
+        <v>US-Corporate-Bond</v>
       </c>
       <c r="H33" s="29" t="str">
-        <v>Global Equity Fund</v>
+        <v>US Corporate Bond Fund</v>
       </c>
       <c r="I33" s="30">
         <v>0</v>
@@ -7220,7 +7229,7 @@
         <v>Transaction</v>
       </c>
       <c r="F46" s="29" t="str">
-        <v>Global Equity Fund</v>
+        <v>UK Equity Fund</v>
       </c>
       <c r="G46" s="69">
         <v>43466</v>
@@ -7246,7 +7255,7 @@
         <v>Transaction</v>
       </c>
       <c r="F47" s="29" t="str">
-        <v>US Corporate Bond Fund</v>
+        <v>Global Equity Fund</v>
       </c>
       <c r="G47" s="69">
         <v>43466</v>
@@ -7272,7 +7281,7 @@
         <v>Transaction</v>
       </c>
       <c r="F48" s="29" t="str">
-        <v>UK Equity Fund</v>
+        <v>US Corporate Bond Fund</v>
       </c>
       <c r="G48" s="69">
         <v>43466</v>
@@ -8059,13 +8068,13 @@
         <v>P</v>
       </c>
       <c r="G32" s="50">
-        <v>12001081</v>
+        <v>12000750</v>
       </c>
       <c r="H32" s="52">
-        <v>12001081</v>
+        <v>12000750</v>
       </c>
       <c r="I32" s="52">
-        <v>2390924402.77</v>
+        <v>2390874062.98</v>
       </c>
       <c r="J32" s="28" t="str">
         <v>USD</v>
@@ -8596,13 +8605,13 @@
         <v>B</v>
       </c>
       <c r="G48" s="86">
-        <v>-106707520.57117647</v>
+        <v>-106641575.44117647</v>
       </c>
       <c r="H48" s="52">
-        <v>-106707520.57117647</v>
+        <v>-106641575.44117647</v>
       </c>
       <c r="I48" s="52">
-        <v>-106707520.56999999</v>
+        <v>-106641575.44</v>
       </c>
       <c r="J48" s="83" t="str">
         <v>USD</v>
@@ -8740,7 +8749,7 @@
   <dimension ref="B1:P79"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10063,15 +10072,15 @@
       </c>
       <c r="G69" s="58">
         <f>'View Holdings'!G32</f>
-        <v>12001081</v>
+        <v>12000750</v>
       </c>
       <c r="H69" s="77">
         <f>'View Holdings'!H32</f>
-        <v>12001081</v>
+        <v>12000750</v>
       </c>
       <c r="I69" s="77">
         <f>'View Holdings'!I32</f>
-        <v>2390924402.77</v>
+        <v>2390874062.98</v>
       </c>
       <c r="J69" s="78" t="str">
         <f>'View Holdings'!J32</f>
@@ -10616,7 +10625,7 @@
   <dimension ref="B1:AJ110"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11412,22 +11421,22 @@
         <v>CancelDateTime</v>
       </c>
       <c r="Y33" s="10" t="str">
-        <v>Original Settlement Date</v>
+        <v>Net holding as a result of the transaction</v>
       </c>
       <c r="Z33" s="10" t="str">
         <v>Exchange rate from the transaction currency to the portfolio currency.</v>
       </c>
       <c r="AA33" s="10" t="str">
+        <v>SourcePortfolioScope</v>
+      </c>
+      <c r="AB33" s="10" t="str">
         <v>SourcePortfolioId</v>
       </c>
-      <c r="AB33" s="10" t="str">
-        <v>SourcePortfolioScope</v>
-      </c>
       <c r="AC33" s="10" t="str">
-        <v>Net holding as a result of the transaction</v>
+        <v>Original Transaction Date</v>
       </c>
       <c r="AD33" s="10" t="str">
-        <v>Original Transaction Date</v>
+        <v>Original Settlement Date</v>
       </c>
       <c r="AE33" s="10" t="str">
         <v>CostPortfolioCcy Amount</v>
@@ -11510,23 +11519,23 @@
       <c r="X34" s="90">
         <v>0</v>
       </c>
-      <c r="Y34" s="88" t="str">
+      <c r="Y34" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD34" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z34" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA34" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB34" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD34" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE34" s="86">
         <v>0</v>
@@ -11609,23 +11618,23 @@
       <c r="X35" s="90">
         <v>0</v>
       </c>
-      <c r="Y35" s="88" t="str">
+      <c r="Y35" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD35" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z35" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA35" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB35" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC35" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD35" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE35" s="86">
         <v>0</v>
@@ -11708,23 +11717,23 @@
       <c r="X36" s="90">
         <v>0</v>
       </c>
-      <c r="Y36" s="88" t="str">
+      <c r="Y36" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD36" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z36" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE36" s="86">
         <v>0</v>
@@ -11807,23 +11816,23 @@
       <c r="X37" s="90">
         <v>0</v>
       </c>
-      <c r="Y37" s="88" t="str">
+      <c r="Y37" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD37" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z37" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA37" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB37" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE37" s="86">
         <v>0</v>
@@ -11906,23 +11915,23 @@
       <c r="X38" s="90">
         <v>0</v>
       </c>
-      <c r="Y38" s="88" t="str">
+      <c r="Y38" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD38" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z38" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB38" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD38" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE38" s="86">
         <v>0</v>
@@ -12005,23 +12014,23 @@
       <c r="X39" s="90">
         <v>0</v>
       </c>
-      <c r="Y39" s="88" t="str">
+      <c r="Y39" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD39" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z39" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA39" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB39" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD39" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE39" s="86">
         <v>0</v>
@@ -12104,23 +12113,23 @@
       <c r="X40" s="90">
         <v>0</v>
       </c>
-      <c r="Y40" s="88" t="str">
+      <c r="Y40" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD40" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z40" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB40" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD40" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE40" s="86">
         <v>0</v>
@@ -12203,23 +12212,23 @@
       <c r="X41" s="90">
         <v>0</v>
       </c>
-      <c r="Y41" s="88" t="str">
+      <c r="Y41" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD41" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z41" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA41" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB41" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD41" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE41" s="86">
         <v>0</v>
@@ -12302,23 +12311,23 @@
       <c r="X42" s="90">
         <v>0</v>
       </c>
-      <c r="Y42" s="88" t="str">
+      <c r="Y42" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD42" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z42" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA42" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB42" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD42" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE42" s="86">
         <v>0</v>
@@ -12401,23 +12410,23 @@
       <c r="X43" s="90">
         <v>0</v>
       </c>
-      <c r="Y43" s="88" t="str">
+      <c r="Y43" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="88">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="91">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="91" t="str">
+        <v>2019-04-15T00:00:00.0000000+00:00</v>
+      </c>
+      <c r="AD43" s="86" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="Z43" s="88">
-        <v>0</v>
-      </c>
-      <c r="AA43" s="88">
-        <v>0</v>
-      </c>
-      <c r="AB43" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="91">
-        <v>0</v>
-      </c>
-      <c r="AD43" s="86" t="str">
-        <v>2019-04-15T00:00:00.0000000+00:00</v>
       </c>
       <c r="AE43" s="86">
         <v>0</v>
@@ -12495,7 +12504,7 @@
         <v>0</v>
       </c>
       <c r="W44" s="90">
-        <v>43711.463611423613</v>
+        <v>43712.479699837961</v>
       </c>
       <c r="X44" s="90">
         <v>0</v>
@@ -12507,10 +12516,10 @@
         <v>0</v>
       </c>
       <c r="AA44" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB44" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB44" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC44" s="91">
         <v>0</v>
@@ -12606,10 +12615,10 @@
         <v>0</v>
       </c>
       <c r="AA45" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB45" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB45" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC45" s="91">
         <v>0</v>
@@ -12705,10 +12714,10 @@
         <v>0</v>
       </c>
       <c r="AA46" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB46" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB46" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC46" s="91">
         <v>0</v>
@@ -12804,10 +12813,10 @@
         <v>0</v>
       </c>
       <c r="AA47" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB47" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB47" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC47" s="91">
         <v>0</v>
@@ -12903,10 +12912,10 @@
         <v>0</v>
       </c>
       <c r="AA48" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB48" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB48" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC48" s="91">
         <v>0</v>
@@ -13002,10 +13011,10 @@
         <v>0</v>
       </c>
       <c r="AA49" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB49" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB49" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC49" s="91">
         <v>0</v>
@@ -13101,10 +13110,10 @@
         <v>0</v>
       </c>
       <c r="AA50" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB50" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB50" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC50" s="91">
         <v>0</v>
@@ -13188,7 +13197,7 @@
         <v>0</v>
       </c>
       <c r="W51" s="90">
-        <v>43711.463611423613</v>
+        <v>43712.479699837961</v>
       </c>
       <c r="X51" s="90">
         <v>0</v>
@@ -13200,10 +13209,10 @@
         <v>0</v>
       </c>
       <c r="AA51" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB51" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB51" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC51" s="91">
         <v>0</v>
@@ -13299,10 +13308,10 @@
         <v>0</v>
       </c>
       <c r="AA52" s="88" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="AB52" s="91" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
-      </c>
-      <c r="AB52" s="91" t="str">
-        <v>Finbourne-Examples</v>
       </c>
       <c r="AC52" s="91">
         <v>0</v>
@@ -13784,8 +13793,8 @@
   </sheetPr>
   <dimension ref="B1:S54"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14221,7 +14230,7 @@
       </c>
       <c r="F27" s="92">
         <f ca="1">NOW()-1/24</f>
-        <v>43711.669038773151</v>
+        <v>43712.658282060191</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -14303,7 +14312,7 @@
       </c>
       <c r="F31" s="92">
         <f ca="1">F27-2/1440</f>
-        <v>43711.667649884264</v>
+        <v>43712.656893171305</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -15011,7 +15020,7 @@
   <dimension ref="B1:R32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15020,7 +15029,7 @@
     <col min="2" max="2" width="2.5703125" customWidth="1"/>
     <col min="3" max="3" width="1" customWidth="1"/>
     <col min="4" max="4" width="3.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -15530,14 +15539,14 @@
         <v>43649</v>
       </c>
       <c r="K22" s="52">
-        <v>331</v>
+        <v>0</v>
       </c>
       <c r="L22" s="87">
         <v>199.23</v>
       </c>
       <c r="M22" s="59">
         <f>L22*K22</f>
-        <v>65945.12999999999</v>
+        <v>0</v>
       </c>
       <c r="N22" s="62">
         <v>1.31</v>
@@ -15719,7 +15728,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="21" t="str">
+      <c r="E31" s="98" t="str">
         <f>_xll.flTransactionsAdd(F15,F17,E19:Q22)</f>
         <v>Transactions added</v>
       </c>
@@ -15803,7 +15812,7 @@
   <dimension ref="B1:M36"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16512,11 +16521,11 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="12" t="str">
+      <c r="E34" s="98" t="str">
         <f>_xll.flHoldingsAdjust(F15,F17,F19,E22:M32)</f>
         <v>Holdings set for portfolio code Global-Equity</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="98"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -16852,17 +16861,17 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F07F7B26-A8FB-44CC-BC1A-494CF9683469}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
     <ds:schemaRef ds:uri="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added portfolio subgroups (#11)
</commit_message>
<xml_diff>
--- a/LUSID Excel - Setting up your IBOR template Global Equity Fund.xlsx
+++ b/LUSID Excel - Setting up your IBOR template Global Equity Fund.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusSekhon\Dev\sample-excel\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1FEAE3-6BBD-4A96-8C62-71FB18CEE56E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13BAC2E-436E-4661-AB1B-7E5EF5FEC2D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="255" windowWidth="29040" windowHeight="15840" tabRatio="798" firstSheet="1" activeTab="6" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" firstSheet="1" activeTab="10" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Datetime format" sheetId="11" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="372">
   <si>
     <t>Code</t>
   </si>
@@ -1248,30 +1248,12 @@
     <t>Step 1: Create a portfolio group</t>
   </si>
   <si>
-    <t>Investment group 1</t>
-  </si>
-  <si>
-    <t>Group1</t>
-  </si>
-  <si>
-    <t>Step 2: Add a portfolio to the group</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Group scope: </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Group code:</t>
-  </si>
-  <si>
     <t>Portfolio scope:</t>
   </si>
   <si>
     <t xml:space="preserve">Group scope: </t>
   </si>
   <si>
-    <t>Contains LUSID example portfolios</t>
-  </si>
-  <si>
     <t>Step 3: View results</t>
   </si>
   <si>
@@ -1288,6 +1270,54 @@
   </si>
   <si>
     <t>The edit was made seconds ago, so the reconciliation shows an edit to an historic transaction which is only visible in AsAt space. In effective date space, you have overwritten what was there previously.</t>
+  </si>
+  <si>
+    <t>US-FI</t>
+  </si>
+  <si>
+    <t>Finbourne-Examples-Fund</t>
+  </si>
+  <si>
+    <t>US Fixed Income group</t>
+  </si>
+  <si>
+    <t>Contains Finbourne US Fixed Income portfolios</t>
+  </si>
+  <si>
+    <t>Finbourne Examples group</t>
+  </si>
+  <si>
+    <t>Contains Finbourne Examples portfolios</t>
+  </si>
+  <si>
+    <t>US-Treasury-Bond</t>
+  </si>
+  <si>
+    <t>Step 2: Add portfolios to groups</t>
+  </si>
+  <si>
+    <t>US-Corporate-Bond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub-group/portfolio codeGroup scope: </t>
+  </si>
+  <si>
+    <t>Group code:</t>
+  </si>
+  <si>
+    <t>UK-Equities</t>
+  </si>
+  <si>
+    <t>Hierarchy</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Sub-group</t>
+  </si>
+  <si>
+    <t>Portfolios</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1735,6 +1765,9 @@
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1763,1201 +1796,1184 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
+    <main first="rtdsrv.deac2096b1a04d65a4cbf75486327008">
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>83d29c96-f659-4f6c-99cb-9d569ac13fe1</stp>
-        <tr r="G47" s="14"/>
-        <tr r="G51" s="14"/>
-        <tr r="H47" s="14"/>
-        <tr r="H52" s="14"/>
-        <tr r="F52" s="14"/>
-        <tr r="F47" s="14"/>
-        <tr r="F48" s="14"/>
-        <tr r="H49" s="14"/>
-        <tr r="J50" s="14"/>
-        <tr r="E51" s="14"/>
-        <tr r="E50" s="14"/>
-        <tr r="G49" s="14"/>
-        <tr r="E52" s="14"/>
-        <tr r="G52" s="14"/>
-        <tr r="I51" s="14"/>
-        <tr r="K47" s="14"/>
-        <tr r="K49" s="14"/>
-        <tr r="I52" s="14"/>
-        <tr r="K48" s="14"/>
-        <tr r="G48" s="14"/>
-        <tr r="I50" s="14"/>
-        <tr r="G50" s="14"/>
-        <tr r="J52" s="14"/>
-        <tr r="J48" s="14"/>
-        <tr r="E47" s="14"/>
-        <tr r="I49" s="14"/>
-        <tr r="H50" s="14"/>
-        <tr r="H48" s="14"/>
-        <tr r="F51" s="14"/>
-        <tr r="E49" s="14"/>
-        <tr r="J47" s="14"/>
-        <tr r="H51" s="14"/>
-        <tr r="F50" s="14"/>
-        <tr r="I48" s="14"/>
-        <tr r="I47" s="14"/>
-        <tr r="K51" s="14"/>
-        <tr r="E48" s="14"/>
-        <tr r="K50" s="14"/>
-        <tr r="K52" s="14"/>
-        <tr r="J51" s="14"/>
-        <tr r="F49" s="14"/>
-        <tr r="J49" s="14"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>8f209322-45c9-44bc-8101-3a573886412a</stp>
-        <tr r="F54" s="5"/>
-        <tr r="G46" s="5"/>
-        <tr r="H49" s="5"/>
-        <tr r="F55" s="5"/>
-        <tr r="E52" s="5"/>
-        <tr r="G48" s="5"/>
-        <tr r="E53" s="5"/>
-        <tr r="H48" s="5"/>
-        <tr r="F48" s="5"/>
-        <tr r="G55" s="5"/>
-        <tr r="F47" s="5"/>
-        <tr r="H54" s="5"/>
-        <tr r="G50" s="5"/>
-        <tr r="E49" s="5"/>
-        <tr r="F51" s="5"/>
-        <tr r="E54" s="5"/>
-        <tr r="H50" s="5"/>
-        <tr r="E55" s="5"/>
-        <tr r="G52" s="5"/>
-        <tr r="H52" s="5"/>
-        <tr r="H46" s="5"/>
-        <tr r="F50" s="5"/>
-        <tr r="F52" s="5"/>
-        <tr r="G47" s="5"/>
-        <tr r="H51" s="5"/>
-        <tr r="G51" s="5"/>
-        <tr r="F46" s="5"/>
-        <tr r="E48" s="5"/>
-        <tr r="E47" s="5"/>
-        <tr r="E50" s="5"/>
-        <tr r="F49" s="5"/>
-        <tr r="H55" s="5"/>
-        <tr r="F53" s="5"/>
-        <tr r="E51" s="5"/>
-        <tr r="H47" s="5"/>
-        <tr r="H53" s="5"/>
-        <tr r="G54" s="5"/>
-        <tr r="E46" s="5"/>
-        <tr r="G49" s="5"/>
-        <tr r="G53" s="5"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>1dbed206-49bd-45a4-bd3d-cc8448825b13</stp>
-        <tr r="T37" s="6"/>
-        <tr r="N49" s="6"/>
-        <tr r="S43" s="6"/>
-        <tr r="F48" s="6"/>
-        <tr r="L44" s="6"/>
-        <tr r="M36" s="6"/>
-        <tr r="AC35" s="6"/>
-        <tr r="N44" s="6"/>
-        <tr r="M47" s="6"/>
-        <tr r="J34" s="6"/>
-        <tr r="M50" s="6"/>
-        <tr r="AG34" s="6"/>
-        <tr r="G41" s="6"/>
-        <tr r="R47" s="6"/>
-        <tr r="AC48" s="6"/>
-        <tr r="Q45" s="6"/>
-        <tr r="Y46" s="6"/>
-        <tr r="H50" s="6"/>
-        <tr r="V36" s="6"/>
-        <tr r="K42" s="6"/>
-        <tr r="AC37" s="6"/>
-        <tr r="AE47" s="6"/>
-        <tr r="AB50" s="6"/>
-        <tr r="AF38" s="6"/>
-        <tr r="W33" s="6"/>
-        <tr r="S42" s="6"/>
-        <tr r="AD37" s="6"/>
-        <tr r="W37" s="6"/>
-        <tr r="W43" s="6"/>
-        <tr r="R52" s="6"/>
-        <tr r="K36" s="6"/>
-        <tr r="P46" s="6"/>
-        <tr r="U34" s="6"/>
-        <tr r="S41" s="6"/>
-        <tr r="S48" s="6"/>
-        <tr r="AC50" s="6"/>
-        <tr r="P45" s="6"/>
-        <tr r="N46" s="6"/>
-        <tr r="W36" s="6"/>
-        <tr r="O45" s="6"/>
-        <tr r="M48" s="6"/>
-        <tr r="AB52" s="6"/>
-        <tr r="F52" s="6"/>
-        <tr r="X33" s="6"/>
-        <tr r="AH33" s="6"/>
-        <tr r="O49" s="6"/>
-        <tr r="G47" s="6"/>
-        <tr r="K40" s="6"/>
-        <tr r="N38" s="6"/>
-        <tr r="E52" s="6"/>
-        <tr r="V45" s="6"/>
-        <tr r="K43" s="6"/>
-        <tr r="AC49" s="6"/>
-        <tr r="Q39" s="6"/>
-        <tr r="R49" s="6"/>
-        <tr r="J44" s="6"/>
-        <tr r="AD40" s="6"/>
-        <tr r="G42" s="6"/>
-        <tr r="AA48" s="6"/>
-        <tr r="AH50" s="6"/>
-        <tr r="I42" s="6"/>
-        <tr r="J43" s="6"/>
-        <tr r="AG37" s="6"/>
-        <tr r="P39" s="6"/>
-        <tr r="AA34" s="6"/>
-        <tr r="Y44" s="6"/>
-        <tr r="Y43" s="6"/>
-        <tr r="AE35" s="6"/>
-        <tr r="T48" s="6"/>
-        <tr r="AE44" s="6"/>
-        <tr r="AH52" s="6"/>
-        <tr r="Z41" s="6"/>
-        <tr r="AC47" s="6"/>
-        <tr r="X37" s="6"/>
-        <tr r="K38" s="6"/>
-        <tr r="N33" s="6"/>
-        <tr r="N41" s="6"/>
-        <tr r="V52" s="6"/>
-        <tr r="AH43" s="6"/>
-        <tr r="X51" s="6"/>
-        <tr r="I44" s="6"/>
-        <tr r="H42" s="6"/>
-        <tr r="R51" s="6"/>
-        <tr r="U43" s="6"/>
-        <tr r="Y41" s="6"/>
-        <tr r="AG51" s="6"/>
-        <tr r="M52" s="6"/>
-        <tr r="R33" s="6"/>
-        <tr r="AE40" s="6"/>
-        <tr r="M42" s="6"/>
-        <tr r="Z47" s="6"/>
-        <tr r="R36" s="6"/>
-        <tr r="X36" s="6"/>
-        <tr r="X35" s="6"/>
-        <tr r="F45" s="6"/>
-        <tr r="N48" s="6"/>
-        <tr r="S34" s="6"/>
-        <tr r="AG39" s="6"/>
-        <tr r="Q50" s="6"/>
-        <tr r="S46" s="6"/>
-        <tr r="J46" s="6"/>
-        <tr r="I48" s="6"/>
-        <tr r="AE43" s="6"/>
-        <tr r="Z38" s="6"/>
-        <tr r="Y48" s="6"/>
-        <tr r="AD50" s="6"/>
-        <tr r="Q38" s="6"/>
-        <tr r="E40" s="6"/>
-        <tr r="O33" s="6"/>
-        <tr r="I49" s="6"/>
-        <tr r="L52" s="6"/>
-        <tr r="AA41" s="6"/>
-        <tr r="AG47" s="6"/>
-        <tr r="AA33" s="6"/>
-        <tr r="X38" s="6"/>
-        <tr r="L50" s="6"/>
-        <tr r="AB35" s="6"/>
-        <tr r="AA36" s="6"/>
-        <tr r="H47" s="6"/>
-        <tr r="AG45" s="6"/>
-        <tr r="Q34" s="6"/>
-        <tr r="W50" s="6"/>
-        <tr r="S33" s="6"/>
-        <tr r="AG43" s="6"/>
-        <tr r="M43" s="6"/>
-        <tr r="Z33" s="6"/>
-        <tr r="H52" s="6"/>
-        <tr r="F39" s="6"/>
-        <tr r="AB36" s="6"/>
-        <tr r="U47" s="6"/>
-        <tr r="H36" s="6"/>
-        <tr r="N39" s="6"/>
-        <tr r="E41" s="6"/>
-        <tr r="L42" s="6"/>
-        <tr r="AC40" s="6"/>
-        <tr r="AA46" s="6"/>
-        <tr r="L37" s="6"/>
-        <tr r="K51" s="6"/>
-        <tr r="X50" s="6"/>
-        <tr r="E46" s="6"/>
-        <tr r="T50" s="6"/>
-        <tr r="I34" s="6"/>
-        <tr r="K33" s="6"/>
-        <tr r="O34" s="6"/>
-        <tr r="L45" s="6"/>
-        <tr r="AG36" s="6"/>
-        <tr r="J33" s="6"/>
-        <tr r="R43" s="6"/>
-        <tr r="F37" s="6"/>
-        <tr r="E35" s="6"/>
-        <tr r="AD41" s="6"/>
-        <tr r="K34" s="6"/>
-        <tr r="Z34" s="6"/>
-        <tr r="AB48" s="6"/>
-        <tr r="O47" s="6"/>
-        <tr r="AH47" s="6"/>
-        <tr r="AE38" s="6"/>
-        <tr r="H48" s="6"/>
-        <tr r="G38" s="6"/>
-        <tr r="AE36" s="6"/>
-        <tr r="G33" s="6"/>
-        <tr r="P35" s="6"/>
-        <tr r="Q33" s="6"/>
-        <tr r="AB43" s="6"/>
-        <tr r="S44" s="6"/>
-        <tr r="L39" s="6"/>
-        <tr r="H38" s="6"/>
-        <tr r="L38" s="6"/>
-        <tr r="K47" s="6"/>
-        <tr r="Q43" s="6"/>
-        <tr r="X42" s="6"/>
-        <tr r="W47" s="6"/>
-        <tr r="AB47" s="6"/>
-        <tr r="F42" s="6"/>
-        <tr r="L46" s="6"/>
-        <tr r="J52" s="6"/>
-        <tr r="T46" s="6"/>
-        <tr r="W42" s="6"/>
-        <tr r="S51" s="6"/>
-        <tr r="M46" s="6"/>
-        <tr r="I39" s="6"/>
-        <tr r="V46" s="6"/>
-        <tr r="G52" s="6"/>
-        <tr r="J37" s="6"/>
-        <tr r="O51" s="6"/>
-        <tr r="E45" s="6"/>
-        <tr r="J40" s="6"/>
-        <tr r="AE39" s="6"/>
-        <tr r="R37" s="6"/>
-        <tr r="K52" s="6"/>
-        <tr r="F38" s="6"/>
-        <tr r="I37" s="6"/>
-        <tr r="W41" s="6"/>
-        <tr r="F33" s="6"/>
-        <tr r="X41" s="6"/>
-        <tr r="V50" s="6"/>
-        <tr r="R34" s="6"/>
-        <tr r="W45" s="6"/>
-        <tr r="S52" s="6"/>
-        <tr r="I45" s="6"/>
-        <tr r="AG49" s="6"/>
-        <tr r="Q42" s="6"/>
-        <tr r="Y38" s="6"/>
-        <tr r="Z44" s="6"/>
-        <tr r="Y50" s="6"/>
-        <tr r="P52" s="6"/>
-        <tr r="K41" s="6"/>
-        <tr r="P44" s="6"/>
-        <tr r="Q40" s="6"/>
-        <tr r="R42" s="6"/>
-        <tr r="X40" s="6"/>
-        <tr r="X49" s="6"/>
-        <tr r="K37" s="6"/>
-        <tr r="R40" s="6"/>
-        <tr r="AE51" s="6"/>
-        <tr r="T35" s="6"/>
-        <tr r="Q48" s="6"/>
-        <tr r="AC43" s="6"/>
-        <tr r="AH37" s="6"/>
-        <tr r="Z48" s="6"/>
-        <tr r="T42" s="6"/>
-        <tr r="AF41" s="6"/>
-        <tr r="N50" s="6"/>
-        <tr r="H37" s="6"/>
-        <tr r="AH35" s="6"/>
-        <tr r="H49" s="6"/>
-        <tr r="T44" s="6"/>
-        <tr r="U48" s="6"/>
-        <tr r="E42" s="6"/>
-        <tr r="AH34" s="6"/>
-        <tr r="H43" s="6"/>
-        <tr r="G51" s="6"/>
-        <tr r="O48" s="6"/>
-        <tr r="AD39" s="6"/>
-        <tr r="AF52" s="6"/>
-        <tr r="AF51" s="6"/>
-        <tr r="W34" s="6"/>
-        <tr r="Y35" s="6"/>
-        <tr r="F44" s="6"/>
-        <tr r="AA47" s="6"/>
-        <tr r="H35" s="6"/>
-        <tr r="P38" s="6"/>
-        <tr r="M37" s="6"/>
-        <tr r="AD46" s="6"/>
-        <tr r="S45" s="6"/>
-        <tr r="U49" s="6"/>
-        <tr r="U50" s="6"/>
-        <tr r="F41" s="6"/>
-        <tr r="N51" s="6"/>
-        <tr r="U38" s="6"/>
-        <tr r="L51" s="6"/>
-        <tr r="E49" s="6"/>
-        <tr r="Z35" s="6"/>
-        <tr r="F47" s="6"/>
-        <tr r="Z50" s="6"/>
-        <tr r="Z52" s="6"/>
-        <tr r="AF35" s="6"/>
-        <tr r="Z43" s="6"/>
-        <tr r="K49" s="6"/>
-        <tr r="Z45" s="6"/>
-        <tr r="AE48" s="6"/>
-        <tr r="S49" s="6"/>
-        <tr r="AB44" s="6"/>
-        <tr r="F36" s="6"/>
-        <tr r="G37" s="6"/>
-        <tr r="P37" s="6"/>
-        <tr r="Y40" s="6"/>
-        <tr r="AE52" s="6"/>
-        <tr r="P33" s="6"/>
-        <tr r="P43" s="6"/>
-        <tr r="AC36" s="6"/>
-        <tr r="AF37" s="6"/>
-        <tr r="N37" s="6"/>
-        <tr r="H51" s="6"/>
-        <tr r="E50" s="6"/>
-        <tr r="AE46" s="6"/>
-        <tr r="Y45" s="6"/>
-        <tr r="AB49" s="6"/>
-        <tr r="AD35" s="6"/>
-        <tr r="AH40" s="6"/>
-        <tr r="AG48" s="6"/>
-        <tr r="I41" s="6"/>
-        <tr r="Y52" s="6"/>
-        <tr r="AF46" s="6"/>
-        <tr r="U39" s="6"/>
-        <tr r="M45" s="6"/>
-        <tr r="K50" s="6"/>
-        <tr r="AB51" s="6"/>
-        <tr r="X44" s="6"/>
-        <tr r="O36" s="6"/>
-        <tr r="AF47" s="6"/>
-        <tr r="AB39" s="6"/>
-        <tr r="AG46" s="6"/>
-        <tr r="AD52" s="6"/>
-        <tr r="J48" s="6"/>
-        <tr r="J39" s="6"/>
-        <tr r="T45" s="6"/>
-        <tr r="H41" s="6"/>
-        <tr r="AH41" s="6"/>
-        <tr r="R45" s="6"/>
-        <tr r="E37" s="6"/>
-        <tr r="T40" s="6"/>
-        <tr r="W44" s="6"/>
-        <tr r="Z42" s="6"/>
-        <tr r="G39" s="6"/>
-        <tr r="X45" s="6"/>
-        <tr r="F49" s="6"/>
-        <tr r="N36" s="6"/>
-        <tr r="J51" s="6"/>
-        <tr r="M39" s="6"/>
-        <tr r="K48" s="6"/>
-        <tr r="AB41" s="6"/>
-        <tr r="K45" s="6"/>
-        <tr r="AG44" s="6"/>
-        <tr r="E38" s="6"/>
-        <tr r="AE33" s="6"/>
-        <tr r="S36" s="6"/>
-        <tr r="O46" s="6"/>
-        <tr r="AB34" s="6"/>
-        <tr r="AH38" s="6"/>
-        <tr r="G48" s="6"/>
-        <tr r="U45" s="6"/>
-        <tr r="AG40" s="6"/>
-        <tr r="K46" s="6"/>
-        <tr r="Q52" s="6"/>
-        <tr r="AC34" s="6"/>
-        <tr r="V39" s="6"/>
-        <tr r="O37" s="6"/>
-        <tr r="Z46" s="6"/>
-        <tr r="AC33" s="6"/>
-        <tr r="W49" s="6"/>
-        <tr r="AD48" s="6"/>
-        <tr r="R50" s="6"/>
-        <tr r="P50" s="6"/>
-        <tr r="E33" s="6"/>
-        <tr r="AD44" s="6"/>
-        <tr r="N42" s="6"/>
-        <tr r="O39" s="6"/>
-        <tr r="J41" s="6"/>
-        <tr r="Y42" s="6"/>
-        <tr r="Y36" s="6"/>
-        <tr r="AH45" s="6"/>
-        <tr r="AE45" s="6"/>
-        <tr r="U37" s="6"/>
-        <tr r="K35" s="6"/>
-        <tr r="AA40" s="6"/>
-        <tr r="I33" s="6"/>
-        <tr r="M35" s="6"/>
-        <tr r="N52" s="6"/>
-        <tr r="R44" s="6"/>
-        <tr r="AD51" s="6"/>
-        <tr r="AF33" s="6"/>
-        <tr r="T52" s="6"/>
-        <tr r="X34" s="6"/>
-        <tr r="AA49" s="6"/>
-        <tr r="Z49" s="6"/>
-        <tr r="J47" s="6"/>
-        <tr r="AC52" s="6"/>
-        <tr r="Z36" s="6"/>
-        <tr r="AH51" s="6"/>
-        <tr r="E43" s="6"/>
-        <tr r="N35" s="6"/>
-        <tr r="AF39" s="6"/>
-        <tr r="U35" s="6"/>
-        <tr r="U46" s="6"/>
-        <tr r="P42" s="6"/>
-        <tr r="AA35" s="6"/>
-        <tr r="W46" s="6"/>
-        <tr r="AD42" s="6"/>
-        <tr r="J42" s="6"/>
-        <tr r="T43" s="6"/>
-        <tr r="Y37" s="6"/>
-        <tr r="AF44" s="6"/>
-        <tr r="U52" s="6"/>
-        <tr r="J36" s="6"/>
-        <tr r="L36" s="6"/>
-        <tr r="F34" s="6"/>
-        <tr r="M38" s="6"/>
-        <tr r="AA37" s="6"/>
-        <tr r="M51" s="6"/>
-        <tr r="R46" s="6"/>
-        <tr r="AF49" s="6"/>
-        <tr r="F46" s="6"/>
-        <tr r="V43" s="6"/>
-        <tr r="U42" s="6"/>
-        <tr r="J49" s="6"/>
-        <tr r="Y51" s="6"/>
-        <tr r="AD34" s="6"/>
-        <tr r="H46" s="6"/>
-        <tr r="Q51" s="6"/>
-        <tr r="V38" s="6"/>
-        <tr r="O43" s="6"/>
-        <tr r="N34" s="6"/>
-        <tr r="W52" s="6"/>
-        <tr r="L49" s="6"/>
-        <tr r="L34" s="6"/>
-        <tr r="E34" s="6"/>
-        <tr r="Q36" s="6"/>
-        <tr r="I47" s="6"/>
-        <tr r="L33" s="6"/>
-        <tr r="I38" s="6"/>
-        <tr r="X39" s="6"/>
-        <tr r="I46" s="6"/>
-        <tr r="U40" s="6"/>
-        <tr r="AF36" s="6"/>
-        <tr r="M40" s="6"/>
-        <tr r="AA42" s="6"/>
-        <tr r="E44" s="6"/>
-        <tr r="AF48" s="6"/>
-        <tr r="AB42" s="6"/>
-        <tr r="AD47" s="6"/>
-        <tr r="I52" s="6"/>
-        <tr r="V48" s="6"/>
-        <tr r="L41" s="6"/>
-        <tr r="AA50" s="6"/>
-        <tr r="V40" s="6"/>
-        <tr r="AG33" s="6"/>
-        <tr r="AF50" s="6"/>
-        <tr r="O44" s="6"/>
-        <tr r="V35" s="6"/>
-        <tr r="AC42" s="6"/>
-        <tr r="P40" s="6"/>
-        <tr r="P41" s="6"/>
-        <tr r="AH46" s="6"/>
-        <tr r="E51" s="6"/>
-        <tr r="AD45" s="6"/>
-        <tr r="T39" s="6"/>
-        <tr r="P48" s="6"/>
-        <tr r="E36" s="6"/>
-        <tr r="V44" s="6"/>
-        <tr r="J50" s="6"/>
-        <tr r="L48" s="6"/>
-        <tr r="F35" s="6"/>
-        <tr r="O52" s="6"/>
-        <tr r="V47" s="6"/>
-        <tr r="W35" s="6"/>
-        <tr r="V49" s="6"/>
-        <tr r="AB46" s="6"/>
-        <tr r="P49" s="6"/>
-        <tr r="U33" s="6"/>
-        <tr r="P47" s="6"/>
-        <tr r="H33" s="6"/>
-        <tr r="AB37" s="6"/>
-        <tr r="Q44" s="6"/>
-        <tr r="AD49" s="6"/>
-        <tr r="X52" s="6"/>
-        <tr r="L35" s="6"/>
-        <tr r="T38" s="6"/>
-        <tr r="H39" s="6"/>
-        <tr r="AG38" s="6"/>
-        <tr r="X46" s="6"/>
-        <tr r="Q41" s="6"/>
-        <tr r="T36" s="6"/>
-        <tr r="I50" s="6"/>
-        <tr r="P34" s="6"/>
-        <tr r="AF34" s="6"/>
-        <tr r="AE50" s="6"/>
-        <tr r="AA51" s="6"/>
-        <tr r="AH44" s="6"/>
-        <tr r="Y47" s="6"/>
-        <tr r="AA45" s="6"/>
-        <tr r="R48" s="6"/>
-        <tr r="AC38" s="6"/>
-        <tr r="AD33" s="6"/>
-        <tr r="AC44" s="6"/>
-        <tr r="AH39" s="6"/>
-        <tr r="O50" s="6"/>
-        <tr r="T51" s="6"/>
-        <tr r="N45" s="6"/>
-        <tr r="W40" s="6"/>
-        <tr r="F50" s="6"/>
-        <tr r="G36" s="6"/>
-        <tr r="G40" s="6"/>
-        <tr r="Z40" s="6"/>
-        <tr r="H40" s="6"/>
-        <tr r="AF43" s="6"/>
-        <tr r="O42" s="6"/>
-        <tr r="E39" s="6"/>
-        <tr r="G46" s="6"/>
-        <tr r="S39" s="6"/>
-        <tr r="AA52" s="6"/>
-        <tr r="J35" s="6"/>
-        <tr r="L43" s="6"/>
-        <tr r="V33" s="6"/>
-        <tr r="Y49" s="6"/>
-        <tr r="R35" s="6"/>
-        <tr r="V37" s="6"/>
-        <tr r="E47" s="6"/>
-        <tr r="AE49" s="6"/>
-        <tr r="AA39" s="6"/>
-        <tr r="AC51" s="6"/>
-        <tr r="AB33" s="6"/>
-        <tr r="AB40" s="6"/>
-        <tr r="P36" s="6"/>
-        <tr r="G35" s="6"/>
-        <tr r="H44" s="6"/>
-        <tr r="S37" s="6"/>
-        <tr r="Y34" s="6"/>
-        <tr r="M34" s="6"/>
-        <tr r="Q47" s="6"/>
-        <tr r="R38" s="6"/>
-        <tr r="U36" s="6"/>
-        <tr r="I40" s="6"/>
-        <tr r="V41" s="6"/>
-        <tr r="AG41" s="6"/>
-        <tr r="N43" s="6"/>
-        <tr r="R39" s="6"/>
-        <tr r="T34" s="6"/>
-        <tr r="U44" s="6"/>
-        <tr r="Q46" s="6"/>
-        <tr r="Q49" s="6"/>
-        <tr r="V34" s="6"/>
-        <tr r="U51" s="6"/>
-        <tr r="AE37" s="6"/>
-        <tr r="W39" s="6"/>
-        <tr r="G50" s="6"/>
-        <tr r="I35" s="6"/>
-        <tr r="N47" s="6"/>
-        <tr r="S35" s="6"/>
-        <tr r="AH36" s="6"/>
-        <tr r="H34" s="6"/>
-        <tr r="Q37" s="6"/>
-        <tr r="W38" s="6"/>
-        <tr r="I36" s="6"/>
-        <tr r="S50" s="6"/>
-        <tr r="N40" s="6"/>
-        <tr r="AF40" s="6"/>
-        <tr r="O40" s="6"/>
-        <tr r="AF42" s="6"/>
-        <tr r="O41" s="6"/>
-        <tr r="P51" s="6"/>
-        <tr r="AB45" s="6"/>
-        <tr r="M49" s="6"/>
-        <tr r="W48" s="6"/>
-        <tr r="F51" s="6"/>
-        <tr r="T47" s="6"/>
-        <tr r="AE42" s="6"/>
-        <tr r="R41" s="6"/>
-        <tr r="Z51" s="6"/>
-        <tr r="T49" s="6"/>
-        <tr r="AE34" s="6"/>
-        <tr r="AA43" s="6"/>
-        <tr r="M33" s="6"/>
-        <tr r="AH48" s="6"/>
-        <tr r="O38" s="6"/>
-        <tr r="O35" s="6"/>
-        <tr r="W51" s="6"/>
-        <tr r="AC39" s="6"/>
-        <tr r="J38" s="6"/>
-        <tr r="M44" s="6"/>
-        <tr r="G43" s="6"/>
-        <tr r="I43" s="6"/>
-        <tr r="V42" s="6"/>
-        <tr r="AH49" s="6"/>
-        <tr r="T33" s="6"/>
-        <tr r="Y33" s="6"/>
-        <tr r="AA44" s="6"/>
-        <tr r="J45" s="6"/>
-        <tr r="AC45" s="6"/>
-        <tr r="G34" s="6"/>
-        <tr r="G49" s="6"/>
-        <tr r="H45" s="6"/>
-        <tr r="AG35" s="6"/>
-        <tr r="Z37" s="6"/>
-        <tr r="AG42" s="6"/>
-        <tr r="S40" s="6"/>
-        <tr r="X43" s="6"/>
-        <tr r="AD43" s="6"/>
-        <tr r="S38" s="6"/>
-        <tr r="Z39" s="6"/>
-        <tr r="AG50" s="6"/>
-        <tr r="Y39" s="6"/>
-        <tr r="V51" s="6"/>
-        <tr r="F40" s="6"/>
-        <tr r="Q35" s="6"/>
-        <tr r="S47" s="6"/>
-        <tr r="X47" s="6"/>
-        <tr r="M41" s="6"/>
-        <tr r="E48" s="6"/>
-        <tr r="U41" s="6"/>
-        <tr r="AE41" s="6"/>
-        <tr r="AG52" s="6"/>
-        <tr r="AF45" s="6"/>
-        <tr r="AH42" s="6"/>
-        <tr r="T41" s="6"/>
-        <tr r="G44" s="6"/>
-        <tr r="AD38" s="6"/>
-        <tr r="I51" s="6"/>
-        <tr r="L40" s="6"/>
-        <tr r="K39" s="6"/>
-        <tr r="F43" s="6"/>
-        <tr r="K44" s="6"/>
-        <tr r="AC41" s="6"/>
-        <tr r="AD36" s="6"/>
-        <tr r="AB38" s="6"/>
-        <tr r="AC46" s="6"/>
-        <tr r="G45" s="6"/>
-        <tr r="L47" s="6"/>
-        <tr r="X48" s="6"/>
-        <tr r="AA38" s="6"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>b85ad992-fc00-4b44-8c7a-65f645574e43</stp>
+        <stp>aaba2f8a-4cec-4ab5-a4c0-f8c360bb0690</stp>
+        <tr r="G35" s="9"/>
+        <tr r="G38" s="9"/>
+        <tr r="F36" s="9"/>
+        <tr r="F35" s="9"/>
+        <tr r="E36" s="9"/>
+        <tr r="G30" s="9"/>
+        <tr r="F31" s="9"/>
         <tr r="F33" s="9"/>
+        <tr r="E33" s="9"/>
+        <tr r="F34" s="9"/>
+        <tr r="G33" s="9"/>
+        <tr r="F37" s="9"/>
+        <tr r="G34" s="9"/>
+        <tr r="G29" s="9"/>
+        <tr r="E37" s="9"/>
+        <tr r="E28" s="9"/>
+        <tr r="F39" s="9"/>
+        <tr r="E32" s="9"/>
         <tr r="G39" s="9"/>
-        <tr r="F29" s="9"/>
+        <tr r="E38" s="9"/>
+        <tr r="E29" s="9"/>
+        <tr r="G36" s="9"/>
         <tr r="E34" s="9"/>
-        <tr r="G35" s="9"/>
-        <tr r="F31" s="9"/>
         <tr r="F28" s="9"/>
         <tr r="G28" s="9"/>
-        <tr r="G38" s="9"/>
-        <tr r="F37" s="9"/>
         <tr r="G31" s="9"/>
         <tr r="E31" s="9"/>
-        <tr r="F34" s="9"/>
-        <tr r="E36" s="9"/>
+        <tr r="G32" s="9"/>
+        <tr r="F32" s="9"/>
+        <tr r="F29" s="9"/>
         <tr r="G37" s="9"/>
-        <tr r="G34" s="9"/>
-        <tr r="F36" s="9"/>
+        <tr r="E39" s="9"/>
         <tr r="F38" s="9"/>
-        <tr r="G29" s="9"/>
-        <tr r="E28" s="9"/>
-        <tr r="F39" s="9"/>
-        <tr r="E33" s="9"/>
-        <tr r="G32" s="9"/>
-        <tr r="E38" s="9"/>
-        <tr r="E39" s="9"/>
-        <tr r="G30" s="9"/>
         <tr r="E30" s="9"/>
         <tr r="F30" s="9"/>
-        <tr r="E29" s="9"/>
-        <tr r="E32" s="9"/>
-        <tr r="F35" s="9"/>
         <tr r="E35" s="9"/>
-        <tr r="G33" s="9"/>
-        <tr r="E37" s="9"/>
-        <tr r="F32" s="9"/>
-        <tr r="G36" s="9"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>234c73c9-5f95-4856-b8d1-9f5085bbe1e6</stp>
-        <tr r="H53" s="9"/>
-        <tr r="F52" s="9"/>
-        <tr r="H60" s="9"/>
-        <tr r="F53" s="9"/>
-        <tr r="F59" s="9"/>
-        <tr r="F58" s="9"/>
-        <tr r="I54" s="9"/>
-        <tr r="H54" s="9"/>
-        <tr r="J52" s="9"/>
-        <tr r="J59" s="9"/>
-        <tr r="F54" s="9"/>
-        <tr r="H57" s="9"/>
-        <tr r="I60" s="9"/>
-        <tr r="G57" s="9"/>
-        <tr r="H51" s="9"/>
-        <tr r="G61" s="9"/>
-        <tr r="F56" s="9"/>
-        <tr r="G59" s="9"/>
-        <tr r="I58" s="9"/>
-        <tr r="H56" s="9"/>
-        <tr r="G55" s="9"/>
-        <tr r="I55" s="9"/>
-        <tr r="F57" s="9"/>
-        <tr r="I52" s="9"/>
-        <tr r="G53" s="9"/>
-        <tr r="F60" s="9"/>
-        <tr r="G51" s="9"/>
-        <tr r="F55" s="9"/>
-        <tr r="G56" s="9"/>
-        <tr r="G52" s="9"/>
-        <tr r="G54" s="9"/>
-        <tr r="H59" s="9"/>
-        <tr r="J57" s="9"/>
-        <tr r="I59" s="9"/>
-        <tr r="J51" s="9"/>
-        <tr r="F51" s="9"/>
-        <tr r="I56" s="9"/>
-        <tr r="H52" s="9"/>
-        <tr r="I57" s="9"/>
-        <tr r="I53" s="9"/>
-        <tr r="F61" s="9"/>
-        <tr r="J61" s="9"/>
-        <tr r="H61" s="9"/>
-        <tr r="G60" s="9"/>
-        <tr r="J55" s="9"/>
-        <tr r="I61" s="9"/>
-        <tr r="J56" s="9"/>
-        <tr r="I51" s="9"/>
-        <tr r="J53" s="9"/>
-        <tr r="J58" s="9"/>
-        <tr r="J60" s="9"/>
-        <tr r="G58" s="9"/>
-        <tr r="J54" s="9"/>
-        <tr r="H55" s="9"/>
-        <tr r="H58" s="9"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>acf96de3-4be4-4a58-806d-7f82fca9e0df</stp>
-        <tr r="K42" s="8"/>
-        <tr r="F47" s="8"/>
-        <tr r="H48" s="8"/>
-        <tr r="L50" s="8"/>
-        <tr r="J47" s="8"/>
-        <tr r="G47" s="8"/>
-        <tr r="I38" s="8"/>
-        <tr r="L35" s="8"/>
-        <tr r="H51" s="8"/>
-        <tr r="F32" s="8"/>
-        <tr r="L48" s="8"/>
-        <tr r="F50" s="8"/>
-        <tr r="F38" s="8"/>
-        <tr r="G38" s="8"/>
-        <tr r="E45" s="8"/>
-        <tr r="E43" s="8"/>
-        <tr r="G45" s="8"/>
-        <tr r="K49" s="8"/>
-        <tr r="F43" s="8"/>
-        <tr r="I40" s="8"/>
-        <tr r="G36" s="8"/>
-        <tr r="E42" s="8"/>
-        <tr r="G32" s="8"/>
-        <tr r="L36" s="8"/>
-        <tr r="F33" s="8"/>
-        <tr r="F42" s="8"/>
-        <tr r="J50" s="8"/>
-        <tr r="H45" s="8"/>
-        <tr r="H36" s="8"/>
-        <tr r="E51" s="8"/>
-        <tr r="K35" s="8"/>
-        <tr r="H34" s="8"/>
-        <tr r="E49" s="8"/>
-        <tr r="G31" s="8"/>
-        <tr r="K43" s="8"/>
-        <tr r="I37" s="8"/>
-        <tr r="L42" s="8"/>
-        <tr r="E46" s="8"/>
-        <tr r="I45" s="8"/>
-        <tr r="L40" s="8"/>
-        <tr r="K37" s="8"/>
-        <tr r="K31" s="8"/>
-        <tr r="I31" s="8"/>
-        <tr r="J40" s="8"/>
-        <tr r="I32" s="8"/>
-        <tr r="J43" s="8"/>
-        <tr r="E41" s="8"/>
-        <tr r="K38" s="8"/>
-        <tr r="L31" s="8"/>
-        <tr r="E44" s="8"/>
-        <tr r="F31" s="8"/>
-        <tr r="I34" s="8"/>
-        <tr r="G40" s="8"/>
-        <tr r="J46" s="8"/>
-        <tr r="F35" s="8"/>
-        <tr r="J42" s="8"/>
-        <tr r="E47" s="8"/>
-        <tr r="I47" s="8"/>
-        <tr r="I33" s="8"/>
-        <tr r="I36" s="8"/>
-        <tr r="L45" s="8"/>
-        <tr r="I42" s="8"/>
-        <tr r="E40" s="8"/>
-        <tr r="H41" s="8"/>
-        <tr r="G49" s="8"/>
-        <tr r="H31" s="8"/>
-        <tr r="J37" s="8"/>
-        <tr r="K39" s="8"/>
-        <tr r="E34" s="8"/>
-        <tr r="J49" s="8"/>
-        <tr r="J35" s="8"/>
-        <tr r="J38" s="8"/>
-        <tr r="G42" s="8"/>
-        <tr r="I46" s="8"/>
-        <tr r="K44" s="8"/>
-        <tr r="J44" s="8"/>
-        <tr r="L43" s="8"/>
-        <tr r="J45" s="8"/>
-        <tr r="I50" s="8"/>
-        <tr r="K45" s="8"/>
-        <tr r="K41" s="8"/>
-        <tr r="K50" s="8"/>
-        <tr r="L37" s="8"/>
-        <tr r="E37" s="8"/>
-        <tr r="I44" s="8"/>
-        <tr r="F41" s="8"/>
-        <tr r="E35" s="8"/>
-        <tr r="H47" s="8"/>
-        <tr r="F36" s="8"/>
-        <tr r="L46" s="8"/>
-        <tr r="K33" s="8"/>
-        <tr r="J34" s="8"/>
-        <tr r="F49" s="8"/>
-        <tr r="G44" s="8"/>
-        <tr r="I41" s="8"/>
-        <tr r="H32" s="8"/>
-        <tr r="E39" s="8"/>
-        <tr r="J31" s="8"/>
-        <tr r="G41" s="8"/>
-        <tr r="I43" s="8"/>
-        <tr r="F46" s="8"/>
-        <tr r="L51" s="8"/>
-        <tr r="J39" s="8"/>
-        <tr r="I48" s="8"/>
-        <tr r="J48" s="8"/>
-        <tr r="K48" s="8"/>
-        <tr r="G51" s="8"/>
-        <tr r="H44" s="8"/>
-        <tr r="G33" s="8"/>
-        <tr r="G50" s="8"/>
-        <tr r="E31" s="8"/>
-        <tr r="J33" s="8"/>
-        <tr r="I51" s="8"/>
-        <tr r="G43" s="8"/>
-        <tr r="H49" s="8"/>
-        <tr r="F45" s="8"/>
-        <tr r="L34" s="8"/>
-        <tr r="E33" s="8"/>
-        <tr r="G46" s="8"/>
-        <tr r="H38" s="8"/>
-        <tr r="I35" s="8"/>
-        <tr r="E36" s="8"/>
-        <tr r="K32" s="8"/>
-        <tr r="F39" s="8"/>
-        <tr r="L47" s="8"/>
-        <tr r="K34" s="8"/>
-        <tr r="J41" s="8"/>
-        <tr r="K36" s="8"/>
-        <tr r="E48" s="8"/>
-        <tr r="L38" s="8"/>
-        <tr r="F40" s="8"/>
-        <tr r="H46" s="8"/>
-        <tr r="K47" s="8"/>
-        <tr r="L39" s="8"/>
-        <tr r="L33" s="8"/>
-        <tr r="F34" s="8"/>
-        <tr r="F51" s="8"/>
-        <tr r="H33" s="8"/>
-        <tr r="H39" s="8"/>
-        <tr r="G34" s="8"/>
-        <tr r="I39" s="8"/>
-        <tr r="H37" s="8"/>
-        <tr r="L44" s="8"/>
-        <tr r="E50" s="8"/>
-        <tr r="E32" s="8"/>
-        <tr r="K46" s="8"/>
-        <tr r="L49" s="8"/>
-        <tr r="F48" s="8"/>
-        <tr r="E38" s="8"/>
-        <tr r="K51" s="8"/>
-        <tr r="F44" s="8"/>
-        <tr r="H35" s="8"/>
-        <tr r="L41" s="8"/>
-        <tr r="I49" s="8"/>
-        <tr r="G37" s="8"/>
-        <tr r="K40" s="8"/>
-        <tr r="J32" s="8"/>
-        <tr r="H43" s="8"/>
-        <tr r="L32" s="8"/>
-        <tr r="H50" s="8"/>
-        <tr r="F37" s="8"/>
-        <tr r="J51" s="8"/>
-        <tr r="J36" s="8"/>
-        <tr r="H42" s="8"/>
-        <tr r="H40" s="8"/>
-        <tr r="G35" s="8"/>
-        <tr r="G48" s="8"/>
-        <tr r="G39" s="8"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>ef9a34d9-4ee5-4009-a4ed-241240564747</stp>
-        <tr r="O42" s="13"/>
-        <tr r="J45" s="13"/>
-        <tr r="J49" s="13"/>
-        <tr r="H44" s="13"/>
-        <tr r="L42" s="13"/>
-        <tr r="F46" s="13"/>
-        <tr r="G46" s="13"/>
-        <tr r="F44" s="13"/>
-        <tr r="N42" s="13"/>
-        <tr r="G47" s="13"/>
-        <tr r="J39" s="13"/>
-        <tr r="E39" s="13"/>
-        <tr r="J42" s="13"/>
-        <tr r="E44" s="13"/>
-        <tr r="E40" s="13"/>
-        <tr r="F47" s="13"/>
-        <tr r="O46" s="13"/>
-        <tr r="I42" s="13"/>
-        <tr r="O39" s="13"/>
-        <tr r="J46" s="13"/>
-        <tr r="M41" s="13"/>
-        <tr r="L48" s="13"/>
-        <tr r="F39" s="13"/>
-        <tr r="O48" s="13"/>
-        <tr r="O47" s="13"/>
-        <tr r="N46" s="13"/>
-        <tr r="G40" s="13"/>
-        <tr r="M49" s="13"/>
-        <tr r="N49" s="13"/>
-        <tr r="J41" s="13"/>
-        <tr r="I45" s="13"/>
-        <tr r="F42" s="13"/>
-        <tr r="M44" s="13"/>
-        <tr r="F40" s="13"/>
-        <tr r="N45" s="13"/>
-        <tr r="K43" s="13"/>
-        <tr r="G42" s="13"/>
-        <tr r="G43" s="13"/>
-        <tr r="J43" s="13"/>
-        <tr r="M40" s="13"/>
-        <tr r="I46" s="13"/>
-        <tr r="F45" s="13"/>
-        <tr r="M39" s="13"/>
-        <tr r="K48" s="13"/>
-        <tr r="L39" s="13"/>
-        <tr r="J40" s="13"/>
-        <tr r="M48" s="13"/>
-        <tr r="J47" s="13"/>
-        <tr r="K44" s="13"/>
-        <tr r="K47" s="13"/>
-        <tr r="H40" s="13"/>
-        <tr r="F48" s="13"/>
-        <tr r="E49" s="13"/>
-        <tr r="O45" s="13"/>
-        <tr r="L41" s="13"/>
-        <tr r="E46" s="13"/>
-        <tr r="N48" s="13"/>
-        <tr r="N44" s="13"/>
-        <tr r="L44" s="13"/>
-        <tr r="E42" s="13"/>
-        <tr r="J48" s="13"/>
-        <tr r="I49" s="13"/>
-        <tr r="O44" s="13"/>
-        <tr r="O49" s="13"/>
-        <tr r="K42" s="13"/>
-        <tr r="H48" s="13"/>
-        <tr r="I41" s="13"/>
-        <tr r="G45" s="13"/>
-        <tr r="G44" s="13"/>
-        <tr r="M43" s="13"/>
-        <tr r="L47" s="13"/>
-        <tr r="O40" s="13"/>
-        <tr r="G41" s="13"/>
-        <tr r="K40" s="13"/>
-        <tr r="H49" s="13"/>
-        <tr r="K49" s="13"/>
-        <tr r="N47" s="13"/>
-        <tr r="N39" s="13"/>
-        <tr r="E48" s="13"/>
-        <tr r="H47" s="13"/>
-        <tr r="L43" s="13"/>
-        <tr r="I48" s="13"/>
-        <tr r="I43" s="13"/>
-        <tr r="E47" s="13"/>
-        <tr r="I47" s="13"/>
-        <tr r="N41" s="13"/>
-        <tr r="H46" s="13"/>
-        <tr r="M47" s="13"/>
-        <tr r="N43" s="13"/>
-        <tr r="F49" s="13"/>
-        <tr r="O41" s="13"/>
-        <tr r="K46" s="13"/>
-        <tr r="G39" s="13"/>
-        <tr r="L46" s="13"/>
-        <tr r="E41" s="13"/>
-        <tr r="K39" s="13"/>
-        <tr r="M45" s="13"/>
-        <tr r="J44" s="13"/>
-        <tr r="E43" s="13"/>
-        <tr r="H39" s="13"/>
-        <tr r="L49" s="13"/>
-        <tr r="G48" s="13"/>
-        <tr r="N40" s="13"/>
-        <tr r="O43" s="13"/>
-        <tr r="F43" s="13"/>
-        <tr r="M46" s="13"/>
-        <tr r="H43" s="13"/>
-        <tr r="H42" s="13"/>
-        <tr r="K45" s="13"/>
-        <tr r="F41" s="13"/>
-        <tr r="H41" s="13"/>
-        <tr r="M42" s="13"/>
-        <tr r="H45" s="13"/>
-        <tr r="I40" s="13"/>
-        <tr r="I39" s="13"/>
-        <tr r="K41" s="13"/>
-        <tr r="G49" s="13"/>
-        <tr r="E45" s="13"/>
-        <tr r="L40" s="13"/>
-        <tr r="L45" s="13"/>
-        <tr r="I44" s="13"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.ed82164b9a8c4523a70d33f583fe4783">
-      <tp>
-        <v>-1</v>
-        <stp/>
-        <stp>e694aaf1-9578-4073-9845-9a6b32a6d04f</stp>
-        <tr r="D20" s="7"/>
-        <tr r="D22" s="7"/>
-        <tr r="D19" s="7"/>
-        <tr r="D25" s="7"/>
-        <tr r="D18" s="7"/>
-        <tr r="D17" s="7"/>
-        <tr r="D24" s="7"/>
-        <tr r="D15" s="7"/>
-        <tr r="D16" s="7"/>
-        <tr r="D21" s="7"/>
-        <tr r="D23" s="7"/>
       </tp>
       <tp>
         <v>-1</v>
         <stp/>
-        <stp>d68b5658-c437-4513-ab49-72e14e1a49a4</stp>
+        <stp>fbe99989-f4e2-4d7d-a2d4-c343a5755d19</stp>
+        <tr r="I42" s="8"/>
+        <tr r="F47" s="8"/>
+        <tr r="F50" s="8"/>
+        <tr r="G36" s="8"/>
+        <tr r="H38" s="8"/>
+        <tr r="K46" s="8"/>
+        <tr r="L32" s="8"/>
+        <tr r="I40" s="8"/>
+        <tr r="H48" s="8"/>
+        <tr r="F43" s="8"/>
+        <tr r="I41" s="8"/>
+        <tr r="I35" s="8"/>
+        <tr r="F48" s="8"/>
+        <tr r="E46" s="8"/>
+        <tr r="H32" s="8"/>
+        <tr r="G50" s="8"/>
+        <tr r="E36" s="8"/>
+        <tr r="J34" s="8"/>
+        <tr r="E39" s="8"/>
+        <tr r="J36" s="8"/>
+        <tr r="J47" s="8"/>
+        <tr r="I51" s="8"/>
+        <tr r="G45" s="8"/>
+        <tr r="J50" s="8"/>
+        <tr r="G31" s="8"/>
+        <tr r="F35" s="8"/>
+        <tr r="I46" s="8"/>
+        <tr r="J31" s="8"/>
+        <tr r="K48" s="8"/>
+        <tr r="H40" s="8"/>
+        <tr r="H36" s="8"/>
+        <tr r="K37" s="8"/>
+        <tr r="K39" s="8"/>
+        <tr r="L43" s="8"/>
+        <tr r="K41" s="8"/>
+        <tr r="I49" s="8"/>
+        <tr r="H51" s="8"/>
+        <tr r="L31" s="8"/>
+        <tr r="E47" s="8"/>
+        <tr r="F45" s="8"/>
+        <tr r="L44" s="8"/>
+        <tr r="K42" s="8"/>
+        <tr r="F36" s="8"/>
+        <tr r="J41" s="8"/>
+        <tr r="H44" s="8"/>
+        <tr r="H49" s="8"/>
+        <tr r="K47" s="8"/>
+        <tr r="F51" s="8"/>
+        <tr r="G34" s="8"/>
+        <tr r="K40" s="8"/>
+        <tr r="J32" s="8"/>
+        <tr r="F37" s="8"/>
+        <tr r="I38" s="8"/>
+        <tr r="F38" s="8"/>
+        <tr r="K49" s="8"/>
+        <tr r="E42" s="8"/>
+        <tr r="L36" s="8"/>
+        <tr r="K43" s="8"/>
+        <tr r="J42" s="8"/>
+        <tr r="J49" s="8"/>
+        <tr r="H47" s="8"/>
+        <tr r="E33" s="8"/>
+        <tr r="F39" s="8"/>
+        <tr r="K36" s="8"/>
+        <tr r="L39" s="8"/>
+        <tr r="H33" s="8"/>
+        <tr r="E32" s="8"/>
+        <tr r="F44" s="8"/>
+        <tr r="H50" s="8"/>
+        <tr r="J51" s="8"/>
+        <tr r="L35" s="8"/>
+        <tr r="F33" s="8"/>
+        <tr r="H45" s="8"/>
+        <tr r="E44" s="8"/>
+        <tr r="I34" s="8"/>
+        <tr r="J46" s="8"/>
+        <tr r="I36" s="8"/>
+        <tr r="G49" s="8"/>
+        <tr r="J37" s="8"/>
+        <tr r="J35" s="8"/>
+        <tr r="G51" s="8"/>
+        <tr r="J33" s="8"/>
+        <tr r="L47" s="8"/>
+        <tr r="E48" s="8"/>
+        <tr r="H37" s="8"/>
+        <tr r="H35" s="8"/>
+        <tr r="H43" s="8"/>
+        <tr r="L50" s="8"/>
+        <tr r="E45" s="8"/>
+        <tr r="H34" s="8"/>
+        <tr r="L42" s="8"/>
+        <tr r="E41" s="8"/>
+        <tr r="F31" s="8"/>
+        <tr r="G40" s="8"/>
+        <tr r="L45" s="8"/>
+        <tr r="K44" s="8"/>
+        <tr r="I44" s="8"/>
+        <tr r="F41" s="8"/>
+        <tr r="K33" s="8"/>
+        <tr r="G41" s="8"/>
+        <tr r="F46" s="8"/>
+        <tr r="I48" s="8"/>
+        <tr r="J48" s="8"/>
+        <tr r="G33" s="8"/>
+        <tr r="G46" s="8"/>
+        <tr r="K34" s="8"/>
+        <tr r="L38" s="8"/>
+        <tr r="L33" s="8"/>
+        <tr r="E50" s="8"/>
+        <tr r="E38" s="8"/>
+        <tr r="L41" s="8"/>
+        <tr r="H42" s="8"/>
+        <tr r="G35" s="8"/>
+        <tr r="G39" s="8"/>
+        <tr r="G47" s="8"/>
+        <tr r="F42" s="8"/>
+        <tr r="E51" s="8"/>
+        <tr r="E49" s="8"/>
+        <tr r="I37" s="8"/>
+        <tr r="K38" s="8"/>
+        <tr r="I47" s="8"/>
+        <tr r="E40" s="8"/>
+        <tr r="H31" s="8"/>
+        <tr r="E34" s="8"/>
+        <tr r="J44" s="8"/>
+        <tr r="I50" s="8"/>
+        <tr r="K50" s="8"/>
+        <tr r="E37" s="8"/>
+        <tr r="L46" s="8"/>
+        <tr r="G44" s="8"/>
+        <tr r="L51" s="8"/>
+        <tr r="E31" s="8"/>
+        <tr r="G43" s="8"/>
+        <tr r="K32" s="8"/>
+        <tr r="F34" s="8"/>
+        <tr r="H39" s="8"/>
+        <tr r="L49" s="8"/>
+        <tr r="K51" s="8"/>
+        <tr r="G48" s="8"/>
+        <tr r="K35" s="8"/>
+        <tr r="I45" s="8"/>
+        <tr r="K31" s="8"/>
+        <tr r="J40" s="8"/>
+        <tr r="I33" s="8"/>
+        <tr r="H41" s="8"/>
+        <tr r="J38" s="8"/>
+        <tr r="K45" s="8"/>
+        <tr r="F49" s="8"/>
+        <tr r="I43" s="8"/>
+        <tr r="F40" s="8"/>
+        <tr r="I39" s="8"/>
+        <tr r="G37" s="8"/>
+        <tr r="F32" s="8"/>
+        <tr r="L48" s="8"/>
+        <tr r="G38" s="8"/>
+        <tr r="E43" s="8"/>
+        <tr r="G32" s="8"/>
+        <tr r="L40" s="8"/>
+        <tr r="I31" s="8"/>
+        <tr r="I32" s="8"/>
+        <tr r="J43" s="8"/>
+        <tr r="G42" s="8"/>
+        <tr r="J45" s="8"/>
+        <tr r="L37" s="8"/>
+        <tr r="E35" s="8"/>
+        <tr r="J39" s="8"/>
+        <tr r="L34" s="8"/>
+        <tr r="H46" s="8"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>ae32f7ed-b2e4-4e7a-8396-d316badc6d2c</stp>
+        <tr r="D22" s="7"/>
+        <tr r="D18" s="7"/>
+        <tr r="D20" s="7"/>
+        <tr r="D19" s="7"/>
+        <tr r="D25" s="7"/>
+        <tr r="D15" s="7"/>
+        <tr r="D17" s="7"/>
+        <tr r="D24" s="7"/>
+        <tr r="D21" s="7"/>
+        <tr r="D23" s="7"/>
+        <tr r="D16" s="7"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.deac2096b1a04d65a4cbf75486327008">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>06614704-0993-41a3-b446-bc10c2e345d1</stp>
+        <tr r="K29" s="5"/>
+        <tr r="M34" s="5"/>
+        <tr r="M33" s="5"/>
+        <tr r="H33" s="5"/>
+        <tr r="L29" s="5"/>
+        <tr r="M35" s="5"/>
+        <tr r="L35" s="5"/>
+        <tr r="J35" s="5"/>
+        <tr r="M30" s="5"/>
+        <tr r="G30" s="5"/>
+        <tr r="K31" s="5"/>
+        <tr r="G34" s="5"/>
+        <tr r="E30" s="5"/>
+        <tr r="J29" s="5"/>
+        <tr r="J30" s="5"/>
+        <tr r="J33" s="5"/>
+        <tr r="K33" s="5"/>
+        <tr r="I34" s="5"/>
+        <tr r="G35" s="5"/>
+        <tr r="M29" s="5"/>
+        <tr r="H30" s="5"/>
+        <tr r="L34" s="5"/>
+        <tr r="M31" s="5"/>
+        <tr r="F34" s="5"/>
+        <tr r="E34" s="5"/>
+        <tr r="I29" s="5"/>
+        <tr r="E29" s="5"/>
+        <tr r="M32" s="5"/>
+        <tr r="F33" s="5"/>
+        <tr r="G31" s="5"/>
         <tr r="H34" s="5"/>
-        <tr r="H30" s="5"/>
+        <tr r="H32" s="5"/>
+        <tr r="I35" s="5"/>
+        <tr r="I33" s="5"/>
+        <tr r="E33" s="5"/>
+        <tr r="G33" s="5"/>
+        <tr r="E35" s="5"/>
+        <tr r="H31" s="5"/>
+        <tr r="K34" s="5"/>
+        <tr r="H29" s="5"/>
+        <tr r="L31" s="5"/>
+        <tr r="G29" s="5"/>
+        <tr r="K30" s="5"/>
+        <tr r="J34" s="5"/>
+        <tr r="L32" s="5"/>
         <tr r="F32" s="5"/>
-        <tr r="L34" s="5"/>
-        <tr r="E35" s="5"/>
-        <tr r="K33" s="5"/>
+        <tr r="J31" s="5"/>
+        <tr r="I32" s="5"/>
+        <tr r="F31" s="5"/>
+        <tr r="K35" s="5"/>
+        <tr r="L33" s="5"/>
+        <tr r="F29" s="5"/>
+        <tr r="K32" s="5"/>
         <tr r="E32" s="5"/>
         <tr r="F35" s="5"/>
-        <tr r="M34" s="5"/>
         <tr r="L30" s="5"/>
-        <tr r="J31" s="5"/>
         <tr r="J32" s="5"/>
-        <tr r="H32" s="5"/>
-        <tr r="K30" s="5"/>
         <tr r="I30" s="5"/>
-        <tr r="H31" s="5"/>
-        <tr r="M31" s="5"/>
-        <tr r="M33" s="5"/>
-        <tr r="F29" s="5"/>
-        <tr r="I35" s="5"/>
-        <tr r="F34" s="5"/>
-        <tr r="H33" s="5"/>
-        <tr r="K31" s="5"/>
-        <tr r="K34" s="5"/>
-        <tr r="I34" s="5"/>
-        <tr r="L29" s="5"/>
-        <tr r="J34" s="5"/>
-        <tr r="G34" s="5"/>
-        <tr r="E34" s="5"/>
-        <tr r="I32" s="5"/>
-        <tr r="M35" s="5"/>
         <tr r="G32" s="5"/>
-        <tr r="L35" s="5"/>
-        <tr r="G35" s="5"/>
-        <tr r="I29" s="5"/>
-        <tr r="E29" s="5"/>
-        <tr r="E30" s="5"/>
-        <tr r="I33" s="5"/>
-        <tr r="K29" s="5"/>
-        <tr r="M32" s="5"/>
-        <tr r="H29" s="5"/>
         <tr r="E31" s="5"/>
-        <tr r="G30" s="5"/>
-        <tr r="J29" s="5"/>
         <tr r="H35" s="5"/>
-        <tr r="J35" s="5"/>
-        <tr r="K32" s="5"/>
-        <tr r="F33" s="5"/>
-        <tr r="E33" s="5"/>
-        <tr r="F31" s="5"/>
-        <tr r="G33" s="5"/>
-        <tr r="M30" s="5"/>
-        <tr r="M29" s="5"/>
-        <tr r="K35" s="5"/>
-        <tr r="L32" s="5"/>
-        <tr r="L31" s="5"/>
         <tr r="F30" s="5"/>
-        <tr r="G29" s="5"/>
-        <tr r="L33" s="5"/>
-        <tr r="J30" s="5"/>
-        <tr r="G31" s="5"/>
-        <tr r="J33" s="5"/>
         <tr r="I31" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.deac2096b1a04d65a4cbf75486327008">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>4d13e5dc-435c-45aa-996e-a1d53500589a</stp>
+        <tr r="I60" s="9"/>
+        <tr r="J57" s="9"/>
+        <tr r="J61" s="9"/>
+        <tr r="J52" s="9"/>
+        <tr r="G53" s="9"/>
+        <tr r="H53" s="9"/>
+        <tr r="G57" s="9"/>
+        <tr r="I58" s="9"/>
+        <tr r="J55" s="9"/>
+        <tr r="H51" s="9"/>
+        <tr r="I55" s="9"/>
+        <tr r="H56" s="9"/>
+        <tr r="F52" s="9"/>
+        <tr r="F56" s="9"/>
+        <tr r="H52" s="9"/>
+        <tr r="F61" s="9"/>
+        <tr r="J56" s="9"/>
+        <tr r="G54" s="9"/>
+        <tr r="F51" s="9"/>
+        <tr r="I53" s="9"/>
+        <tr r="J60" s="9"/>
+        <tr r="J54" s="9"/>
+        <tr r="H58" s="9"/>
+        <tr r="H60" s="9"/>
+        <tr r="H57" s="9"/>
+        <tr r="G55" s="9"/>
+        <tr r="F57" s="9"/>
+        <tr r="F55" s="9"/>
+        <tr r="H59" s="9"/>
+        <tr r="I59" s="9"/>
+        <tr r="J51" s="9"/>
+        <tr r="I56" s="9"/>
+        <tr r="H55" s="9"/>
+        <tr r="F59" s="9"/>
+        <tr r="F58" s="9"/>
+        <tr r="G51" s="9"/>
+        <tr r="G52" s="9"/>
+        <tr r="H61" s="9"/>
+        <tr r="J53" s="9"/>
+        <tr r="J59" s="9"/>
+        <tr r="G59" s="9"/>
+        <tr r="F54" s="9"/>
+        <tr r="G61" s="9"/>
+        <tr r="F60" s="9"/>
+        <tr r="I57" s="9"/>
+        <tr r="I51" s="9"/>
+        <tr r="F53" s="9"/>
+        <tr r="I54" s="9"/>
+        <tr r="H54" s="9"/>
+        <tr r="I52" s="9"/>
+        <tr r="G56" s="9"/>
+        <tr r="G60" s="9"/>
+        <tr r="I61" s="9"/>
+        <tr r="J58" s="9"/>
+        <tr r="G58" s="9"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.deac2096b1a04d65a4cbf75486327008">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>a33c7af0-21c3-4b36-8c13-4f9deb8faa38</stp>
+        <tr r="G46" s="5"/>
+        <tr r="F48" s="5"/>
+        <tr r="H54" s="5"/>
+        <tr r="E51" s="5"/>
+        <tr r="F47" s="5"/>
+        <tr r="G50" s="5"/>
+        <tr r="G52" s="5"/>
+        <tr r="F52" s="5"/>
+        <tr r="G47" s="5"/>
+        <tr r="G53" s="5"/>
+        <tr r="G54" s="5"/>
+        <tr r="H51" s="5"/>
+        <tr r="G55" s="5"/>
+        <tr r="H46" s="5"/>
+        <tr r="F46" s="5"/>
+        <tr r="E48" s="5"/>
+        <tr r="E47" s="5"/>
+        <tr r="G49" s="5"/>
+        <tr r="E53" s="5"/>
+        <tr r="F51" s="5"/>
+        <tr r="E54" s="5"/>
+        <tr r="F50" s="5"/>
+        <tr r="H55" s="5"/>
+        <tr r="F53" s="5"/>
+        <tr r="H53" s="5"/>
+        <tr r="H52" s="5"/>
+        <tr r="G51" s="5"/>
+        <tr r="E50" s="5"/>
+        <tr r="F55" s="5"/>
+        <tr r="E52" s="5"/>
+        <tr r="E55" s="5"/>
+        <tr r="H48" s="5"/>
+        <tr r="H50" s="5"/>
+        <tr r="F54" s="5"/>
+        <tr r="H49" s="5"/>
+        <tr r="G48" s="5"/>
+        <tr r="E49" s="5"/>
+        <tr r="F49" s="5"/>
+        <tr r="H47" s="5"/>
+        <tr r="E46" s="5"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.deac2096b1a04d65a4cbf75486327008">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>c154f083-50c3-4496-8135-59d398dab137</stp>
+        <tr r="F51" s="14"/>
+        <tr r="E51" s="14"/>
+        <tr r="J50" s="14"/>
+        <tr r="J51" s="14"/>
+        <tr r="H51" s="14"/>
+        <tr r="I50" s="14"/>
+        <tr r="F50" s="14"/>
+        <tr r="H50" s="14"/>
+        <tr r="I51" s="14"/>
+        <tr r="G51" s="14"/>
+        <tr r="E50" s="14"/>
+        <tr r="G50" s="14"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.deac2096b1a04d65a4cbf75486327008">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>ae2faab2-ba96-4c64-81e5-1b3aed01172b</stp>
+        <tr r="F47" s="14"/>
+        <tr r="I47" s="14"/>
+        <tr r="E47" s="14"/>
+        <tr r="J47" s="14"/>
+        <tr r="F48" s="14"/>
+        <tr r="H47" s="14"/>
+        <tr r="E48" s="14"/>
+        <tr r="I48" s="14"/>
+        <tr r="G47" s="14"/>
+        <tr r="H48" s="14"/>
+        <tr r="J48" s="14"/>
+        <tr r="G48" s="14"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>5661f1cb-5139-4edb-81cb-5a8ded3db303</stp>
+        <tr r="AC50" s="6"/>
+        <tr r="Y44" s="6"/>
+        <tr r="N48" s="6"/>
+        <tr r="V52" s="6"/>
+        <tr r="S46" s="6"/>
+        <tr r="I34" s="6"/>
+        <tr r="S44" s="6"/>
+        <tr r="J40" s="6"/>
+        <tr r="Q40" s="6"/>
+        <tr r="E42" s="6"/>
+        <tr r="F47" s="6"/>
+        <tr r="AD35" s="6"/>
+        <tr r="E37" s="6"/>
+        <tr r="U45" s="6"/>
+        <tr r="AE47" s="6"/>
+        <tr r="K42" s="6"/>
+        <tr r="Z33" s="6"/>
+        <tr r="O34" s="6"/>
+        <tr r="K47" s="6"/>
+        <tr r="X40" s="6"/>
+        <tr r="G51" s="6"/>
+        <tr r="Z43" s="6"/>
+        <tr r="AE45" s="6"/>
+        <tr r="AF49" s="6"/>
+        <tr r="O42" s="6"/>
+        <tr r="AG34" s="6"/>
+        <tr r="R51" s="6"/>
+        <tr r="F39" s="6"/>
+        <tr r="R43" s="6"/>
+        <tr r="X42" s="6"/>
+        <tr r="F33" s="6"/>
+        <tr r="AF52" s="6"/>
+        <tr r="U39" s="6"/>
+        <tr r="G39" s="6"/>
+        <tr r="AA40" s="6"/>
+        <tr r="S50" s="6"/>
+        <tr r="AD43" s="6"/>
+        <tr r="M52" s="6"/>
+        <tr r="AB47" s="6"/>
+        <tr r="Y35" s="6"/>
+        <tr r="K50" s="6"/>
+        <tr r="N52" s="6"/>
+        <tr r="H33" s="6"/>
+        <tr r="V37" s="6"/>
+        <tr r="M49" s="6"/>
+        <tr r="AE51" s="6"/>
+        <tr r="F36" s="6"/>
+        <tr r="M36" s="6"/>
+        <tr r="S42" s="6"/>
+        <tr r="I49" s="6"/>
+        <tr r="J52" s="6"/>
+        <tr r="H35" s="6"/>
+        <tr r="AE52" s="6"/>
+        <tr r="O36" s="6"/>
+        <tr r="N36" s="6"/>
+        <tr r="I38" s="6"/>
+        <tr r="AG38" s="6"/>
+        <tr r="T49" s="6"/>
+        <tr r="AH52" s="6"/>
+        <tr r="V50" s="6"/>
+        <tr r="N44" s="6"/>
+        <tr r="R52" s="6"/>
+        <tr r="M48" s="6"/>
+        <tr r="E52" s="6"/>
+        <tr r="AH50" s="6"/>
+        <tr r="R36" s="6"/>
+        <tr r="O47" s="6"/>
+        <tr r="S51" s="6"/>
+        <tr r="AG46" s="6"/>
+        <tr r="K48" s="6"/>
+        <tr r="P50" s="6"/>
+        <tr r="E43" s="6"/>
+        <tr r="E44" s="6"/>
+        <tr r="G35" s="6"/>
+        <tr r="AE41" s="6"/>
+        <tr r="N39" s="6"/>
+        <tr r="J34" s="6"/>
+        <tr r="U34" s="6"/>
+        <tr r="AH33" s="6"/>
+        <tr r="AC49" s="6"/>
+        <tr r="L50" s="6"/>
+        <tr r="V46" s="6"/>
+        <tr r="U50" s="6"/>
+        <tr r="AF37" s="6"/>
+        <tr r="J39" s="6"/>
+        <tr r="AG44" s="6"/>
+        <tr r="N42" s="6"/>
+        <tr r="AD42" s="6"/>
+        <tr r="AC44" s="6"/>
+        <tr r="AC39" s="6"/>
+        <tr r="I51" s="6"/>
+        <tr r="AG45" s="6"/>
+        <tr r="P35" s="6"/>
+        <tr r="P52" s="6"/>
+        <tr r="L51" s="6"/>
+        <tr r="AE46" s="6"/>
+        <tr r="O46" s="6"/>
+        <tr r="Y42" s="6"/>
+        <tr r="P40" s="6"/>
+        <tr r="N43" s="6"/>
+        <tr r="AH49" s="6"/>
+        <tr r="AD36" s="6"/>
+        <tr r="T52" s="6"/>
+        <tr r="J47" s="6"/>
+        <tr r="U46" s="6"/>
+        <tr r="Y37" s="6"/>
+        <tr r="M38" s="6"/>
+        <tr r="J49" s="6"/>
+        <tr r="V38" s="6"/>
+        <tr r="E34" s="6"/>
+        <tr r="U40" s="6"/>
+        <tr r="AF50" s="6"/>
+        <tr r="E51" s="6"/>
+        <tr r="E36" s="6"/>
+        <tr r="O52" s="6"/>
+        <tr r="P49" s="6"/>
+        <tr r="X52" s="6"/>
+        <tr r="I50" s="6"/>
+        <tr r="AA45" s="6"/>
+        <tr r="G40" s="6"/>
+        <tr r="Z40" s="6"/>
+        <tr r="V33" s="6"/>
+        <tr r="Y34" s="6"/>
+        <tr r="I40" s="6"/>
+        <tr r="Q46" s="6"/>
+        <tr r="W39" s="6"/>
+        <tr r="Q37" s="6"/>
+        <tr r="AF42" s="6"/>
+        <tr r="AA43" s="6"/>
+        <tr r="AH48" s="6"/>
+        <tr r="G34" s="6"/>
+        <tr r="Z37" s="6"/>
+        <tr r="U41" s="6"/>
+        <tr r="AH42" s="6"/>
+        <tr r="F43" s="6"/>
+        <tr r="L47" s="6"/>
+        <tr r="S43" s="6"/>
+        <tr r="AC35" s="6"/>
+        <tr r="G41" s="6"/>
+        <tr r="R47" s="6"/>
+        <tr r="AD37" s="6"/>
+        <tr r="W36" s="6"/>
+        <tr r="Q39" s="6"/>
+        <tr r="AC47" s="6"/>
+        <tr r="AH43" s="6"/>
+        <tr r="U43" s="6"/>
+        <tr r="X35" s="6"/>
+        <tr r="J46" s="6"/>
+        <tr r="AD50" s="6"/>
+        <tr r="L52" s="6"/>
+        <tr r="AB35" s="6"/>
+        <tr r="S33" s="6"/>
+        <tr r="AB36" s="6"/>
+        <tr r="AC40" s="6"/>
+        <tr r="K51" s="6"/>
+        <tr r="K33" s="6"/>
+        <tr r="F37" s="6"/>
+        <tr r="G38" s="6"/>
+        <tr r="L39" s="6"/>
+        <tr r="T46" s="6"/>
+        <tr r="G52" s="6"/>
+        <tr r="AE39" s="6"/>
+        <tr r="S52" s="6"/>
+        <tr r="Y38" s="6"/>
+        <tr r="X49" s="6"/>
+        <tr r="AH37" s="6"/>
+        <tr r="H37" s="6"/>
+        <tr r="AH34" s="6"/>
+        <tr r="AF51" s="6"/>
+        <tr r="P38" s="6"/>
+        <tr r="F41" s="6"/>
+        <tr r="Z50" s="6"/>
+        <tr r="AE48" s="6"/>
+        <tr r="P33" s="6"/>
+        <tr r="N37" s="6"/>
+        <tr r="AH40" s="6"/>
+        <tr r="AF47" s="6"/>
+        <tr r="X45" s="6"/>
+        <tr r="J51" s="6"/>
+        <tr r="E38" s="6"/>
+        <tr r="AG40" s="6"/>
+        <tr r="AD48" s="6"/>
+        <tr r="O39" s="6"/>
+        <tr r="AH45" s="6"/>
+        <tr r="I33" s="6"/>
+        <tr r="AC52" s="6"/>
+        <tr r="P42" s="6"/>
+        <tr r="AA37" s="6"/>
+        <tr r="M51" s="6"/>
+        <tr r="Y51" s="6"/>
+        <tr r="O43" s="6"/>
+        <tr r="Q36" s="6"/>
+        <tr r="AF36" s="6"/>
+        <tr r="I52" s="6"/>
+        <tr r="O44" s="6"/>
+        <tr r="V47" s="6"/>
+        <tr r="L35" s="6"/>
+        <tr r="P34" s="6"/>
+        <tr r="R48" s="6"/>
+        <tr r="N45" s="6"/>
+        <tr r="H40" s="6"/>
+        <tr r="Y49" s="6"/>
+        <tr r="AB33" s="6"/>
+        <tr r="M34" s="6"/>
+        <tr r="V41" s="6"/>
+        <tr r="G50" s="6"/>
+        <tr r="W38" s="6"/>
+        <tr r="O41" s="6"/>
+        <tr r="AE42" s="6"/>
+        <tr r="O38" s="6"/>
+        <tr r="I43" s="6"/>
+        <tr r="AG42" s="6"/>
+        <tr r="T41" s="6"/>
+        <tr r="K44" s="6"/>
+        <tr r="H50" s="6"/>
+        <tr r="W37" s="6"/>
+        <tr r="O45" s="6"/>
+        <tr r="K40" s="6"/>
+        <tr r="R49" s="6"/>
+        <tr r="AA48" s="6"/>
+        <tr r="P39" s="6"/>
+        <tr r="X51" s="6"/>
+        <tr r="Y41" s="6"/>
+        <tr r="M42" s="6"/>
+        <tr r="I48" s="6"/>
+        <tr r="Q38" s="6"/>
+        <tr r="AA41" s="6"/>
+        <tr r="AA36" s="6"/>
+        <tr r="AG43" s="6"/>
+        <tr r="U47" s="6"/>
+        <tr r="AA46" s="6"/>
+        <tr r="Z34" s="6"/>
+        <tr r="AE36" s="6"/>
+        <tr r="H38" s="6"/>
+        <tr r="W42" s="6"/>
+        <tr r="J37" s="6"/>
+        <tr r="R37" s="6"/>
+        <tr r="Z44" s="6"/>
+        <tr r="K37" s="6"/>
+        <tr r="AH35" s="6"/>
+        <tr r="W34" s="6"/>
+        <tr r="M37" s="6"/>
+        <tr r="N51" s="6"/>
+        <tr r="Z52" s="6"/>
+        <tr r="S49" s="6"/>
+        <tr r="P43" s="6"/>
+        <tr r="H51" s="6"/>
+        <tr r="AG48" s="6"/>
+        <tr r="M45" s="6"/>
+        <tr r="T45" s="6"/>
+        <tr r="T40" s="6"/>
+        <tr r="M39" s="6"/>
+        <tr r="AE33" s="6"/>
+        <tr r="K46" s="6"/>
+        <tr r="R50" s="6"/>
+        <tr r="J41" s="6"/>
+        <tr r="Z36" s="6"/>
+        <tr r="AA35" s="6"/>
+        <tr r="AF44" s="6"/>
+        <tr r="R46" s="6"/>
+        <tr r="AD34" s="6"/>
+        <tr r="I47" s="6"/>
+        <tr r="M40" s="6"/>
+        <tr r="V48" s="6"/>
+        <tr r="V35" s="6"/>
+        <tr r="W35" s="6"/>
+        <tr r="U33" s="6"/>
+        <tr r="T38" s="6"/>
+        <tr r="AF34" s="6"/>
+        <tr r="AC38" s="6"/>
+        <tr r="AF43" s="6"/>
+        <tr r="S39" s="6"/>
+        <tr r="R35" s="6"/>
+        <tr r="AE49" s="6"/>
+        <tr r="AB40" s="6"/>
+        <tr r="AG41" s="6"/>
+        <tr r="Q49" s="6"/>
+        <tr r="I35" s="6"/>
+        <tr r="I36" s="6"/>
+        <tr r="P51" s="6"/>
+        <tr r="R41" s="6"/>
+        <tr r="O35" s="6"/>
+        <tr r="V42" s="6"/>
+        <tr r="S40" s="6"/>
+        <tr r="AG50" s="6"/>
+        <tr r="S47" s="6"/>
+        <tr r="G44" s="6"/>
+        <tr r="AC41" s="6"/>
+        <tr r="X48" s="6"/>
+        <tr r="AC48" s="6"/>
+        <tr r="M47" s="6"/>
+        <tr r="Q45" s="6"/>
+        <tr r="V36" s="6"/>
+        <tr r="W43" s="6"/>
+        <tr r="O49" s="6"/>
+        <tr r="N38" s="6"/>
+        <tr r="AA34" s="6"/>
+        <tr r="X37" s="6"/>
+        <tr r="AG51" s="6"/>
+        <tr r="Z47" s="6"/>
+        <tr r="F45" s="6"/>
+        <tr r="E40" s="6"/>
+        <tr r="AG47" s="6"/>
+        <tr r="H47" s="6"/>
+        <tr r="M43" s="6"/>
+        <tr r="H36" s="6"/>
+        <tr r="E35" s="6"/>
+        <tr r="AB48" s="6"/>
+        <tr r="G33" s="6"/>
+        <tr r="L38" s="6"/>
+        <tr r="W47" s="6"/>
+        <tr r="O51" s="6"/>
+        <tr r="K52" s="6"/>
+        <tr r="X41" s="6"/>
+        <tr r="I45" s="6"/>
+        <tr r="Y50" s="6"/>
+        <tr r="R42" s="6"/>
+        <tr r="R40" s="6"/>
+        <tr r="Z48" s="6"/>
+        <tr r="H43" s="6"/>
+        <tr r="AD46" s="6"/>
+        <tr r="U38" s="6"/>
+        <tr r="AF35" s="6"/>
+        <tr r="AB44" s="6"/>
+        <tr r="AC36" s="6"/>
+        <tr r="E50" s="6"/>
+        <tr r="AB39" s="6"/>
+        <tr r="S36" s="6"/>
+        <tr r="Q52" s="6"/>
+        <tr r="Z46" s="6"/>
+        <tr r="M35" s="6"/>
+        <tr r="AH51" s="6"/>
+        <tr r="W46" s="6"/>
+        <tr r="U52" s="6"/>
+        <tr r="H46" s="6"/>
+        <tr r="N34" s="6"/>
+        <tr r="L33" s="6"/>
+        <tr r="AA42" s="6"/>
+        <tr r="L41" s="6"/>
+        <tr r="AC42" s="6"/>
+        <tr r="V44" s="6"/>
+        <tr r="V49" s="6"/>
+        <tr r="P47" s="6"/>
+        <tr r="H39" s="6"/>
+        <tr r="AE50" s="6"/>
+        <tr r="AD33" s="6"/>
+        <tr r="AA39" s="6"/>
+        <tr r="P36" s="6"/>
+        <tr r="Q47" s="6"/>
+        <tr r="V34" s="6"/>
+        <tr r="N47" s="6"/>
+        <tr r="AB45" s="6"/>
+        <tr r="Z51" s="6"/>
+        <tr r="W51" s="6"/>
+        <tr r="G49" s="6"/>
+        <tr r="X43" s="6"/>
+        <tr r="Y39" s="6"/>
+        <tr r="AD38" s="6"/>
+        <tr r="AA38" s="6"/>
+        <tr r="F48" s="6"/>
+        <tr r="Y46" s="6"/>
+        <tr r="AB50" s="6"/>
+        <tr r="S41" s="6"/>
+        <tr r="P45" s="6"/>
+        <tr r="AB52" s="6"/>
+        <tr r="V45" s="6"/>
+        <tr r="J44" s="6"/>
+        <tr r="I42" s="6"/>
+        <tr r="Y43" s="6"/>
+        <tr r="T48" s="6"/>
+        <tr r="K38" s="6"/>
+        <tr r="S34" s="6"/>
+        <tr r="AE43" s="6"/>
+        <tr r="O33" s="6"/>
+        <tr r="AA33" s="6"/>
+        <tr r="Q34" s="6"/>
+        <tr r="H52" s="6"/>
+        <tr r="E41" s="6"/>
+        <tr r="X50" s="6"/>
+        <tr r="L45" s="6"/>
+        <tr r="AH47" s="6"/>
+        <tr r="F38" s="6"/>
+        <tr r="T35" s="6"/>
+        <tr r="T42" s="6"/>
+        <tr r="H49" s="6"/>
+        <tr r="O48" s="6"/>
+        <tr r="S45" s="6"/>
+        <tr r="K49" s="6"/>
+        <tr r="G37" s="6"/>
+        <tr r="I41" s="6"/>
+        <tr r="AB51" s="6"/>
+        <tr r="AD52" s="6"/>
+        <tr r="H41" s="6"/>
+        <tr r="F49" s="6"/>
+        <tr r="AB34" s="6"/>
+        <tr r="AC34" s="6"/>
+        <tr r="AC33" s="6"/>
+        <tr r="E33" s="6"/>
+        <tr r="U37" s="6"/>
+        <tr r="R44" s="6"/>
+        <tr r="X34" s="6"/>
+        <tr r="N35" s="6"/>
+        <tr r="J36" s="6"/>
+        <tr r="F46" s="6"/>
+        <tr r="W52" s="6"/>
+        <tr r="AF48" s="6"/>
+        <tr r="AA50" s="6"/>
+        <tr r="P41" s="6"/>
+        <tr r="AD45" s="6"/>
+        <tr r="J50" s="6"/>
+        <tr r="AB37" s="6"/>
+        <tr r="X46" s="6"/>
+        <tr r="AA51" s="6"/>
+        <tr r="AH39" s="6"/>
+        <tr r="W40" s="6"/>
+        <tr r="E39" s="6"/>
+        <tr r="AA52" s="6"/>
+        <tr r="H44" s="6"/>
+        <tr r="R38" s="6"/>
+        <tr r="R39" s="6"/>
+        <tr r="S35" s="6"/>
+        <tr r="N40" s="6"/>
+        <tr r="W48" s="6"/>
+        <tr r="M33" s="6"/>
+        <tr r="J38" s="6"/>
+        <tr r="T33" s="6"/>
+        <tr r="AA44" s="6"/>
+        <tr r="H45" s="6"/>
+        <tr r="S38" s="6"/>
+        <tr r="V51" s="6"/>
+        <tr r="X47" s="6"/>
+        <tr r="AB38" s="6"/>
+        <tr r="AC37" s="6"/>
+        <tr r="AF38" s="6"/>
+        <tr r="S48" s="6"/>
+        <tr r="N46" s="6"/>
+        <tr r="F52" s="6"/>
+        <tr r="G47" s="6"/>
+        <tr r="AD40" s="6"/>
+        <tr r="J43" s="6"/>
+        <tr r="AE35" s="6"/>
+        <tr r="AE44" s="6"/>
+        <tr r="Z41" s="6"/>
+        <tr r="N33" s="6"/>
+        <tr r="I44" s="6"/>
+        <tr r="R33" s="6"/>
+        <tr r="AG39" s="6"/>
+        <tr r="Z38" s="6"/>
+        <tr r="W50" s="6"/>
+        <tr r="L42" s="6"/>
+        <tr r="E46" s="6"/>
+        <tr r="AG36" s="6"/>
+        <tr r="AD41" s="6"/>
+        <tr r="AE38" s="6"/>
+        <tr r="Q33" s="6"/>
+        <tr r="F42" s="6"/>
+        <tr r="M46" s="6"/>
+        <tr r="I37" s="6"/>
+        <tr r="R34" s="6"/>
+        <tr r="AG49" s="6"/>
+        <tr r="K41" s="6"/>
+        <tr r="Q48" s="6"/>
+        <tr r="AF41" s="6"/>
+        <tr r="T44" s="6"/>
+        <tr r="AD39" s="6"/>
+        <tr r="F44" s="6"/>
+        <tr r="U49" s="6"/>
+        <tr r="E49" s="6"/>
+        <tr r="P37" s="6"/>
+        <tr r="Y45" s="6"/>
+        <tr r="Y52" s="6"/>
+        <tr r="J48" s="6"/>
+        <tr r="AH41" s="6"/>
+        <tr r="W44" s="6"/>
+        <tr r="AB41" s="6"/>
+        <tr r="AH38" s="6"/>
+        <tr r="V39" s="6"/>
+        <tr r="W49" s="6"/>
+        <tr r="Y36" s="6"/>
+        <tr r="K35" s="6"/>
+        <tr r="AD51" s="6"/>
+        <tr r="AA49" s="6"/>
+        <tr r="AF39" s="6"/>
+        <tr r="J42" s="6"/>
+        <tr r="L36" s="6"/>
+        <tr r="V43" s="6"/>
+        <tr r="L49" s="6"/>
+        <tr r="X39" s="6"/>
+        <tr r="AB42" s="6"/>
+        <tr r="V40" s="6"/>
+        <tr r="AH46" s="6"/>
+        <tr r="T39" s="6"/>
+        <tr r="L48" s="6"/>
+        <tr r="Q44" s="6"/>
+        <tr r="Q41" s="6"/>
+        <tr r="AH44" s="6"/>
+        <tr r="O50" s="6"/>
+        <tr r="F50" s="6"/>
+        <tr r="J35" s="6"/>
+        <tr r="E47" s="6"/>
+        <tr r="AC51" s="6"/>
+        <tr r="U36" s="6"/>
+        <tr r="T34" s="6"/>
+        <tr r="U51" s="6"/>
+        <tr r="AH36" s="6"/>
+        <tr r="AF40" s="6"/>
+        <tr r="F51" s="6"/>
+        <tr r="M44" s="6"/>
+        <tr r="Y33" s="6"/>
+        <tr r="J45" s="6"/>
+        <tr r="AG35" s="6"/>
+        <tr r="Z39" s="6"/>
+        <tr r="F40" s="6"/>
+        <tr r="M41" s="6"/>
+        <tr r="AG52" s="6"/>
+        <tr r="L40" s="6"/>
+        <tr r="AC46" s="6"/>
+        <tr r="K36" s="6"/>
+        <tr r="T37" s="6"/>
+        <tr r="N49" s="6"/>
+        <tr r="L44" s="6"/>
+        <tr r="M50" s="6"/>
+        <tr r="W33" s="6"/>
+        <tr r="P46" s="6"/>
+        <tr r="X33" s="6"/>
+        <tr r="K43" s="6"/>
+        <tr r="G42" s="6"/>
+        <tr r="AG37" s="6"/>
+        <tr r="N41" s="6"/>
+        <tr r="H42" s="6"/>
+        <tr r="AE40" s="6"/>
+        <tr r="X36" s="6"/>
+        <tr r="Q50" s="6"/>
+        <tr r="Y48" s="6"/>
+        <tr r="X38" s="6"/>
+        <tr r="L37" s="6"/>
+        <tr r="T50" s="6"/>
+        <tr r="J33" s="6"/>
+        <tr r="K34" s="6"/>
+        <tr r="H48" s="6"/>
+        <tr r="AB43" s="6"/>
+        <tr r="Q43" s="6"/>
+        <tr r="L46" s="6"/>
+        <tr r="I39" s="6"/>
+        <tr r="E45" s="6"/>
+        <tr r="W41" s="6"/>
+        <tr r="W45" s="6"/>
+        <tr r="Q42" s="6"/>
+        <tr r="P44" s="6"/>
+        <tr r="AC43" s="6"/>
+        <tr r="N50" s="6"/>
+        <tr r="U48" s="6"/>
+        <tr r="AA47" s="6"/>
+        <tr r="Z35" s="6"/>
+        <tr r="Z45" s="6"/>
+        <tr r="Y40" s="6"/>
+        <tr r="AB49" s="6"/>
+        <tr r="AF46" s="6"/>
+        <tr r="X44" s="6"/>
+        <tr r="R45" s="6"/>
+        <tr r="Z42" s="6"/>
+        <tr r="K45" s="6"/>
+        <tr r="G48" s="6"/>
+        <tr r="O37" s="6"/>
+        <tr r="AD44" s="6"/>
+        <tr r="AF33" s="6"/>
+        <tr r="Z49" s="6"/>
+        <tr r="U35" s="6"/>
+        <tr r="T43" s="6"/>
+        <tr r="F34" s="6"/>
+        <tr r="U42" s="6"/>
+        <tr r="Q51" s="6"/>
+        <tr r="L34" s="6"/>
+        <tr r="I46" s="6"/>
+        <tr r="AD47" s="6"/>
+        <tr r="AG33" s="6"/>
+        <tr r="P48" s="6"/>
+        <tr r="F35" s="6"/>
+        <tr r="AB46" s="6"/>
+        <tr r="AD49" s="6"/>
+        <tr r="T36" s="6"/>
+        <tr r="Y47" s="6"/>
+        <tr r="T51" s="6"/>
+        <tr r="G36" s="6"/>
+        <tr r="G46" s="6"/>
+        <tr r="L43" s="6"/>
+        <tr r="S37" s="6"/>
+        <tr r="U44" s="6"/>
+        <tr r="AE37" s="6"/>
+        <tr r="H34" s="6"/>
+        <tr r="O40" s="6"/>
+        <tr r="T47" s="6"/>
+        <tr r="AE34" s="6"/>
+        <tr r="G43" s="6"/>
+        <tr r="AC45" s="6"/>
+        <tr r="Q35" s="6"/>
+        <tr r="E48" s="6"/>
+        <tr r="AF45" s="6"/>
+        <tr r="K39" s="6"/>
+        <tr r="G45" s="6"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>6cea516a-fb5d-4566-8bca-5bdb926b6593</stp>
+        <tr r="E39" s="13"/>
+        <tr r="F39" s="13"/>
+        <tr r="F48" s="13"/>
+        <tr r="H44" s="13"/>
+        <tr r="J42" s="13"/>
+        <tr r="O47" s="13"/>
+        <tr r="O45" s="13"/>
+        <tr r="G45" s="13"/>
+        <tr r="E45" s="13"/>
+        <tr r="L48" s="13"/>
+        <tr r="F46" s="13"/>
+        <tr r="E44" s="13"/>
+        <tr r="G40" s="13"/>
+        <tr r="N44" s="13"/>
+        <tr r="H46" s="13"/>
+        <tr r="G48" s="13"/>
+        <tr r="G46" s="13"/>
+        <tr r="F47" s="13"/>
+        <tr r="L39" s="13"/>
+        <tr r="I49" s="13"/>
+        <tr r="H49" s="13"/>
+        <tr r="F49" s="13"/>
+        <tr r="N40" s="13"/>
+        <tr r="E48" s="13"/>
+        <tr r="L46" s="13"/>
+        <tr r="H45" s="13"/>
+        <tr r="I42" s="13"/>
+        <tr r="K43" s="13"/>
+        <tr r="I43" s="13"/>
+        <tr r="J44" s="13"/>
+        <tr r="F44" s="13"/>
+        <tr r="O42" s="13"/>
+        <tr r="N42" s="13"/>
+        <tr r="J46" s="13"/>
+        <tr r="M40" s="13"/>
+        <tr r="F42" s="13"/>
+        <tr r="J49" s="13"/>
+        <tr r="G47" s="13"/>
+        <tr r="M41" s="13"/>
+        <tr r="H42" s="13"/>
+        <tr r="O46" s="13"/>
+        <tr r="H48" s="13"/>
+        <tr r="M42" s="13"/>
+        <tr r="K41" s="13"/>
+        <tr r="G42" s="13"/>
+        <tr r="J40" s="13"/>
+        <tr r="K44" s="13"/>
+        <tr r="L41" s="13"/>
+        <tr r="O44" s="13"/>
+        <tr r="G44" s="13"/>
+        <tr r="K49" s="13"/>
+        <tr r="E47" s="13"/>
+        <tr r="I47" s="13"/>
+        <tr r="O41" s="13"/>
+        <tr r="E43" s="13"/>
+        <tr r="O43" s="13"/>
+        <tr r="K45" s="13"/>
+        <tr r="G43" s="13"/>
+        <tr r="M48" s="13"/>
+        <tr r="E46" s="13"/>
+        <tr r="O49" s="13"/>
+        <tr r="M43" s="13"/>
+        <tr r="N47" s="13"/>
+        <tr r="K46" s="13"/>
+        <tr r="H39" s="13"/>
+        <tr r="F43" s="13"/>
+        <tr r="F41" s="13"/>
+        <tr r="J41" s="13"/>
+        <tr r="K47" s="13"/>
+        <tr r="L42" s="13"/>
+        <tr r="J39" s="13"/>
+        <tr r="O39" s="13"/>
+        <tr r="N46" s="13"/>
+        <tr r="I45" s="13"/>
+        <tr r="J43" s="13"/>
+        <tr r="H40" s="13"/>
+        <tr r="N48" s="13"/>
+        <tr r="K42" s="13"/>
+        <tr r="L47" s="13"/>
+        <tr r="N39" s="13"/>
+        <tr r="N41" s="13"/>
+        <tr r="G39" s="13"/>
+        <tr r="L49" s="13"/>
+        <tr r="M46" s="13"/>
+        <tr r="H41" s="13"/>
+        <tr r="I39" s="13"/>
+        <tr r="G49" s="13"/>
+        <tr r="M49" s="13"/>
+        <tr r="M44" s="13"/>
+        <tr r="I46" s="13"/>
+        <tr r="K48" s="13"/>
+        <tr r="J47" s="13"/>
+        <tr r="L44" s="13"/>
+        <tr r="I41" s="13"/>
+        <tr r="O40" s="13"/>
+        <tr r="H47" s="13"/>
+        <tr r="E41" s="13"/>
+        <tr r="I40" s="13"/>
+        <tr r="L40" s="13"/>
+        <tr r="N49" s="13"/>
+        <tr r="F45" s="13"/>
+        <tr r="E42" s="13"/>
+        <tr r="G41" s="13"/>
+        <tr r="L43" s="13"/>
+        <tr r="M47" s="13"/>
+        <tr r="K39" s="13"/>
+        <tr r="L45" s="13"/>
+        <tr r="F40" s="13"/>
+        <tr r="J45" s="13"/>
+        <tr r="E40" s="13"/>
+        <tr r="O48" s="13"/>
+        <tr r="N45" s="13"/>
+        <tr r="M39" s="13"/>
+        <tr r="E49" s="13"/>
+        <tr r="J48" s="13"/>
+        <tr r="K40" s="13"/>
+        <tr r="I48" s="13"/>
+        <tr r="N43" s="13"/>
+        <tr r="M45" s="13"/>
+        <tr r="H43" s="13"/>
+        <tr r="I44" s="13"/>
       </tp>
     </main>
   </volType>
@@ -3107,7 +3123,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>212912</xdr:colOff>
+      <xdr:colOff>470647</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>73798</xdr:rowOff>
     </xdr:to>
@@ -4568,7 +4584,7 @@
   <dimension ref="B1:N37"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:J46"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5143,8 +5159,8 @@
   </sheetPr>
   <dimension ref="B1:N60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5154,13 +5170,15 @@
     <col min="3" max="3" width="1" customWidth="1"/>
     <col min="4" max="4" width="3.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="22" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.42578125" customWidth="1"/>
     <col min="10" max="10" width="22" customWidth="1"/>
-    <col min="11" max="12" width="24.28515625" customWidth="1"/>
-    <col min="13" max="13" width="52.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5444,20 +5462,20 @@
         <v>1</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="F19" s="88" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="G19" s="88"/>
       <c r="H19" s="31" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="18"/>
       <c r="K19" s="96" t="str">
-        <f>_xll.flGroupsCreate(F15,E18:I19)</f>
-        <v>Failed to create group 'Group1' in scope 'Finbourne-Examples' as a group with that identifier already exists</v>
+        <f t="array" ref="K19:K20">_xll.flGroupsCreate(F15,E18:I20)</f>
+        <v>Failed to create group 'US-FI' in scope 'Finbourne-Examples' as a group with that identifier already exists</v>
       </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -5469,13 +5487,21 @@
       <c r="D20" s="12">
         <v>2</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="85"/>
+      <c r="E20" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="F20" s="85" t="s">
+        <v>360</v>
+      </c>
       <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
+      <c r="H20" s="88" t="s">
+        <v>361</v>
+      </c>
       <c r="I20" s="9"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="85"/>
+      <c r="K20" s="96" t="str">
+        <v>Failed to create group 'Finbourne-Examples-Fund' in scope 'Finbourne-Examples' as a group with that identifier already exists</v>
+      </c>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -5642,14 +5668,16 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
+      <c r="L30" s="2" t="s">
+        <v>368</v>
+      </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
     </row>
     <row r="31" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B31" s="2"/>
       <c r="C31" s="13" t="s">
-        <v>350</v>
+        <v>363</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="2"/>
@@ -5658,10 +5686,14 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
+      <c r="K31" s="46" t="s">
+        <v>369</v>
+      </c>
       <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="M31" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="N31" s="9"/>
     </row>
     <row r="32" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
@@ -5673,8 +5705,12 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="K32" s="46" t="s">
+        <v>370</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>356</v>
+      </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
     </row>
@@ -5683,37 +5719,62 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="12" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="G33" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="K33" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="L33" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="M33" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="N33" s="19" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="12" t="s">
-        <v>352</v>
-      </c>
-      <c r="F34" s="19" t="str">
-        <f>E19</f>
-        <v>Group1</v>
-      </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+        <v>366</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>357</v>
+      </c>
       <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
+      <c r="L34" s="19" t="s">
+        <v>362</v>
+      </c>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
@@ -5722,16 +5783,23 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="12" t="s">
-        <v>353</v>
-      </c>
-      <c r="F35" s="19" t="str">
-        <f>'Create portfolio'!F15</f>
-        <v>Finbourne-Examples</v>
-      </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+        <v>348</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>321</v>
+      </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
@@ -5742,16 +5810,23 @@
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="F36" s="19" t="str">
-        <f>'Create portfolio'!G19</f>
-        <v>Global-Equity</v>
-      </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+        <v>365</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="I36" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>367</v>
+      </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
@@ -5780,10 +5855,18 @@
       <c r="F38" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
+      <c r="G38" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="I38" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>296</v>
+      </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
@@ -5796,12 +5879,24 @@
       <c r="E39" s="2"/>
       <c r="F39" s="96" t="str">
         <f>_xll.flGroupsAddPortfolio(F33,F34,F35,F36)</f>
-        <v>#ERROR: Error updating group goose/Finbourne-Examples/Group1 because the entry being added goose/Finbourne-Examples/Global-Equity already exists.</v>
-      </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
+        <v>#ERROR: Error updating group goose/Finbourne-Examples/US-FI because the entry being added goose/Finbourne-Examples/US-Treasury-Bond already exists.</v>
+      </c>
+      <c r="G39" s="96" t="str">
+        <f>_xll.flGroupsAddPortfolio(G33,G34,G35,G36)</f>
+        <v>#ERROR: Error updating group goose/Finbourne-Examples/US-FI because the entry being added goose/Finbourne-Examples/US-Corporate-Bond already exists.</v>
+      </c>
+      <c r="H39" s="96" t="str">
+        <f>_xll.flGroupsAddSubGroup(H33,H34,H35,H36)</f>
+        <v>#ERROR: The group in goose/Finbourne-Examples/US-FI is already registered as a subgroup of the group goose/Finbourne-Examples/Finbourne-Examples-Fund AsAt=2019-09-24T07:32:08.3647940+00:00</v>
+      </c>
+      <c r="I39" s="96" t="str">
+        <f>_xll.flGroupsAddPortfolio(I33,I34,I35,I36)</f>
+        <v>#ERROR: Error updating group goose/Finbourne-Examples/Finbourne-Examples-Fund because the entry being added goose/Finbourne-Examples/Global-Equity already exists.</v>
+      </c>
+      <c r="J39" s="96" t="str">
+        <f>_xll.flGroupsAddPortfolio(J33,J34,J35,J36)</f>
+        <v>#ERROR: Error updating group goose/Finbourne-Examples/Finbourne-Examples-Fund because the entry being added goose/Finbourne-Examples/UK-Equities already exists.</v>
+      </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
@@ -5840,7 +5935,7 @@
     <row r="42" spans="2:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B42" s="2"/>
       <c r="C42" s="13" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D42" s="13"/>
       <c r="E42" s="2"/>
@@ -5895,7 +5990,7 @@
       <c r="E45" s="2"/>
       <c r="F45" s="35">
         <f ca="1">TODAY()</f>
-        <v>43718</v>
+        <v>43732</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -5926,7 +6021,7 @@
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="8" t="str">
-        <f t="array" ref="E47:K52">_xll.flGroupsGet(F33,F34)</f>
+        <f t="array" ref="E47:J48">_xll.flGroupsGet(F44,E19)</f>
         <v>Id Scope</v>
       </c>
       <c r="F47" s="10" t="str">
@@ -5944,9 +6039,7 @@
       <c r="J47" s="7" t="str">
         <v>SubGroups</v>
       </c>
-      <c r="K47" s="10" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="K47" s="10"/>
       <c r="L47" s="2"/>
       <c r="M47" s="2"/>
       <c r="N47" s="2"/>
@@ -5961,23 +6054,21 @@
         <v>Finbourne-Examples</v>
       </c>
       <c r="F48" s="88" t="str">
-        <v>Group1</v>
+        <v>US-FI</v>
       </c>
       <c r="G48" s="88" t="str">
-        <v>Investment group 1</v>
+        <v>US Fixed Income group</v>
       </c>
       <c r="H48" s="31" t="str">
-        <v>Contains example portfolios</v>
+        <v>Contains Finbourne US Fixed Income portfolios</v>
       </c>
       <c r="I48" s="15">
-        <v>1</v>
-      </c>
-      <c r="J48" s="18">
-        <v>0</v>
-      </c>
-      <c r="K48" s="31" t="e">
-        <v>#N/A</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J48" s="99">
+        <v>0</v>
+      </c>
+      <c r="K48" s="31"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
       <c r="N48" s="17"/>
@@ -5985,30 +6076,14 @@
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="12">
-        <v>2</v>
-      </c>
-      <c r="E49" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F49" s="85" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G49" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H49" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I49" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J49" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K49" s="85" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="85"/>
+      <c r="G49" s="88"/>
+      <c r="H49" s="88"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="85"/>
       <c r="L49" s="2"/>
       <c r="M49" s="2"/>
       <c r="N49" s="2"/>
@@ -6016,30 +6091,27 @@
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="12">
-        <v>3</v>
-      </c>
-      <c r="E50" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F50" s="85" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G50" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H50" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I50" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J50" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K50" s="85" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="8" t="str">
+        <f t="array" ref="E50:J51">_xll.flGroupsGet(F44,E20)</f>
+        <v>Id Scope</v>
+      </c>
+      <c r="F50" s="10" t="str">
+        <v>Id Code</v>
+      </c>
+      <c r="G50" s="10" t="str">
+        <v>DisplayName</v>
+      </c>
+      <c r="H50" s="10" t="str">
+        <v>Description</v>
+      </c>
+      <c r="I50" s="8" t="str">
+        <v>Portfolios</v>
+      </c>
+      <c r="J50" s="7" t="str">
+        <v>SubGroups</v>
+      </c>
+      <c r="K50" s="10"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50" s="2"/>
@@ -6048,29 +6120,27 @@
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="12">
-        <v>4</v>
-      </c>
-      <c r="E51" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F51" s="85" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G51" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H51" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I51" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J51" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K51" s="85" t="e">
-        <v>#N/A</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E51" s="15" t="str">
+        <v>Finbourne-Examples</v>
+      </c>
+      <c r="F51" s="88" t="str">
+        <v>Finbourne-Examples-Fund</v>
+      </c>
+      <c r="G51" s="88" t="str">
+        <v>Finbourne Examples group</v>
+      </c>
+      <c r="H51" s="31" t="str">
+        <v>Contains Finbourne Examples portfolios</v>
+      </c>
+      <c r="I51" s="15">
+        <v>2</v>
+      </c>
+      <c r="J51" s="99">
+        <v>1</v>
+      </c>
+      <c r="K51" s="31"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -6081,27 +6151,13 @@
       <c r="D52" s="12">
         <v>5</v>
       </c>
-      <c r="E52" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F52" s="85" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G52" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H52" s="88" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I52" s="9" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J52" s="5" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K52" s="85" t="e">
-        <v>#N/A</v>
-      </c>
+      <c r="E52" s="9"/>
+      <c r="F52" s="85"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="85"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6238,14 +6294,14 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="8">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Code" sqref="E18 E47" xr:uid="{5186502B-0030-407B-92E0-ECD8ADE97953}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Base Currency" sqref="F38 K18" xr:uid="{45CB02F2-CB9C-492E-BDDE-04F194963C03}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date Created" sqref="K47" xr:uid="{289CB227-8390-43BD-999F-17E47A839971}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Description" sqref="J18 J47" xr:uid="{EA1B5B86-0172-4AA2-A0FC-99BAA99595A1}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Display Name" sqref="I18 I47" xr:uid="{1CB0A25E-0226-4A11-87F4-37E8F63B24ED}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sub-Holding Keys" sqref="H18 H47" xr:uid="{B548E53C-5468-47F2-AB40-A144599BD804}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Accounting Method" sqref="G18 G47" xr:uid="{B0BB2118-452B-4B46-BEBA-B2B04C5744C6}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Corporate Action Source" sqref="F18 F47" xr:uid="{E036C10F-2195-400C-A017-D13C52B1130A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Code" sqref="E18 E47 E50" xr:uid="{5186502B-0030-407B-92E0-ECD8ADE97953}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Base Currency" sqref="K18 F38:J38" xr:uid="{45CB02F2-CB9C-492E-BDDE-04F194963C03}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Date Created" sqref="K47 K50" xr:uid="{289CB227-8390-43BD-999F-17E47A839971}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Description" sqref="J18 J47 J50" xr:uid="{EA1B5B86-0172-4AA2-A0FC-99BAA99595A1}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Display Name" sqref="I18 I47 I50" xr:uid="{1CB0A25E-0226-4A11-87F4-37E8F63B24ED}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sub-Holding Keys" sqref="H18 H47 H50" xr:uid="{B548E53C-5468-47F2-AB40-A144599BD804}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Accounting Method" sqref="G18 G47 G50" xr:uid="{B0BB2118-452B-4B46-BEBA-B2B04C5744C6}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Corporate Action Source" sqref="F18 F47 F50" xr:uid="{E036C10F-2195-400C-A017-D13C52B1130A}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{44027378-72ED-4435-99AC-4D1C18747C76}"/>
@@ -7637,7 +7693,7 @@
   <dimension ref="B1:S92"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8282,32 +8338,32 @@
       <c r="D34" s="12">
         <v>5</v>
       </c>
-      <c r="E34" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F34" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G34" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H34" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I34" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J34" s="69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K34" s="70" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L34" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M34" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E34" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F34" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G34" s="29" t="str">
+        <v/>
+      </c>
+      <c r="H34" s="29" t="str">
+        <v/>
+      </c>
+      <c r="I34" s="30" t="str">
+        <v/>
+      </c>
+      <c r="J34" s="69" t="str">
+        <v/>
+      </c>
+      <c r="K34" s="70" t="str">
+        <v/>
+      </c>
+      <c r="L34" s="29" t="str">
+        <v/>
+      </c>
+      <c r="M34" s="29" t="str">
+        <v/>
       </c>
       <c r="N34" s="2"/>
     </row>
@@ -8317,32 +8373,32 @@
       <c r="D35" s="12">
         <v>6</v>
       </c>
-      <c r="E35" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F35" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G35" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H35" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I35" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="J35" s="69" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K35" s="70" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L35" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M35" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E35" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F35" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G35" s="29" t="str">
+        <v/>
+      </c>
+      <c r="H35" s="29" t="str">
+        <v/>
+      </c>
+      <c r="I35" s="30" t="str">
+        <v/>
+      </c>
+      <c r="J35" s="69" t="str">
+        <v/>
+      </c>
+      <c r="K35" s="70" t="str">
+        <v/>
+      </c>
+      <c r="L35" s="29" t="str">
+        <v/>
+      </c>
+      <c r="M35" s="29" t="str">
+        <v/>
       </c>
       <c r="N35" s="2"/>
     </row>
@@ -8514,7 +8570,7 @@
         <v>Transaction</v>
       </c>
       <c r="F46" s="29" t="str">
-        <v>US Corporate Bond Fund</v>
+        <v>Global Equity Fund</v>
       </c>
       <c r="G46" s="69">
         <v>43466</v>
@@ -8540,7 +8596,7 @@
         <v>Transaction</v>
       </c>
       <c r="F47" s="29" t="str">
-        <v>Global Equity Fund</v>
+        <v>US$ Treasury Bond Fund</v>
       </c>
       <c r="G47" s="69">
         <v>43466</v>
@@ -8566,7 +8622,7 @@
         <v>Transaction</v>
       </c>
       <c r="F48" s="29" t="str">
-        <v>UK Equity Fund</v>
+        <v>US Corporate Bond Fund</v>
       </c>
       <c r="G48" s="69">
         <v>43466</v>
@@ -8592,7 +8648,7 @@
         <v>Transaction</v>
       </c>
       <c r="F49" s="29" t="str">
-        <v>US$ Treasury Bond Fund</v>
+        <v>UK Equity Fund</v>
       </c>
       <c r="G49" s="69">
         <v>43466</v>
@@ -8614,17 +8670,17 @@
       <c r="D50" s="12">
         <v>5</v>
       </c>
-      <c r="E50" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F50" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G50" s="71" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H50" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E50" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F50" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G50" s="71" t="str">
+        <v/>
+      </c>
+      <c r="H50" s="29" t="str">
+        <v/>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -8639,17 +8695,17 @@
       <c r="D51" s="12">
         <v>6</v>
       </c>
-      <c r="E51" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F51" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G51" s="71" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H51" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E51" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F51" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G51" s="71" t="str">
+        <v/>
+      </c>
+      <c r="H51" s="29" t="str">
+        <v/>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -8664,17 +8720,17 @@
       <c r="D52" s="12">
         <v>7</v>
       </c>
-      <c r="E52" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F52" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G52" s="71" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H52" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E52" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F52" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G52" s="71" t="str">
+        <v/>
+      </c>
+      <c r="H52" s="29" t="str">
+        <v/>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -8689,17 +8745,17 @@
       <c r="D53" s="12">
         <v>8</v>
       </c>
-      <c r="E53" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F53" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G53" s="71" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H53" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E53" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F53" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G53" s="71" t="str">
+        <v/>
+      </c>
+      <c r="H53" s="29" t="str">
+        <v/>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -8714,17 +8770,17 @@
       <c r="D54" s="12">
         <v>9</v>
       </c>
-      <c r="E54" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F54" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G54" s="71" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H54" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E54" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F54" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G54" s="71" t="str">
+        <v/>
+      </c>
+      <c r="H54" s="29" t="str">
+        <v/>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -8739,17 +8795,17 @@
       <c r="D55" s="12">
         <v>10</v>
       </c>
-      <c r="E55" s="30" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F55" s="29" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G55" s="71" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="H55" s="29" t="e">
-        <v>#N/A</v>
+      <c r="E55" s="30" t="str">
+        <v/>
+      </c>
+      <c r="F55" s="29" t="str">
+        <v/>
+      </c>
+      <c r="G55" s="71" t="str">
+        <v/>
+      </c>
+      <c r="H55" s="29" t="str">
+        <v/>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -12709,19 +12765,19 @@
         <v>SourcePortfolioId</v>
       </c>
       <c r="Z33" s="10" t="str">
+        <v>SourcePortfolioScope</v>
+      </c>
+      <c r="AA33" s="10" t="str">
+        <v>Net holding as a result of the transaction</v>
+      </c>
+      <c r="AB33" s="10" t="str">
+        <v>Original Settlement Date</v>
+      </c>
+      <c r="AC33" s="10" t="str">
         <v>Exchange rate from the transaction currency to the portfolio currency.</v>
       </c>
-      <c r="AA33" s="10" t="str">
-        <v>Original Settlement Date</v>
-      </c>
-      <c r="AB33" s="10" t="str">
-        <v>SourcePortfolioScope</v>
-      </c>
-      <c r="AC33" s="10" t="str">
+      <c r="AD33" s="10" t="str">
         <v>Original Transaction Date</v>
-      </c>
-      <c r="AD33" s="10" t="str">
-        <v>Net holding as a result of the transaction</v>
       </c>
       <c r="AE33" s="10" t="str">
         <v>CostPortfolioCcy Amount</v>
@@ -12810,17 +12866,17 @@
       <c r="Z34" s="88">
         <v>0</v>
       </c>
-      <c r="AA34" s="88" t="str">
+      <c r="AA34" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB34" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="91" t="str">
+      <c r="AC34" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD34" s="86">
-        <v>0</v>
       </c>
       <c r="AE34" s="86">
         <v>0</v>
@@ -12909,17 +12965,17 @@
       <c r="Z35" s="88">
         <v>0</v>
       </c>
-      <c r="AA35" s="88" t="str">
+      <c r="AA35" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB35" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC35" s="91" t="str">
+      <c r="AC35" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD35" s="86">
-        <v>0</v>
       </c>
       <c r="AE35" s="86">
         <v>0</v>
@@ -13008,17 +13064,17 @@
       <c r="Z36" s="88">
         <v>0</v>
       </c>
-      <c r="AA36" s="88" t="str">
+      <c r="AA36" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB36" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="91" t="str">
+      <c r="AC36" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD36" s="86">
-        <v>0</v>
       </c>
       <c r="AE36" s="86">
         <v>0</v>
@@ -13107,17 +13163,17 @@
       <c r="Z37" s="88">
         <v>0</v>
       </c>
-      <c r="AA37" s="88" t="str">
+      <c r="AA37" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB37" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="91" t="str">
+      <c r="AC37" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD37" s="86">
-        <v>0</v>
       </c>
       <c r="AE37" s="86">
         <v>0</v>
@@ -13206,17 +13262,17 @@
       <c r="Z38" s="88">
         <v>0</v>
       </c>
-      <c r="AA38" s="88" t="str">
+      <c r="AA38" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB38" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="91" t="str">
+      <c r="AC38" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD38" s="86">
-        <v>0</v>
       </c>
       <c r="AE38" s="86">
         <v>0</v>
@@ -13305,17 +13361,17 @@
       <c r="Z39" s="88">
         <v>0</v>
       </c>
-      <c r="AA39" s="88" t="str">
+      <c r="AA39" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB39" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="91" t="str">
+      <c r="AC39" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD39" s="86">
-        <v>0</v>
       </c>
       <c r="AE39" s="86">
         <v>0</v>
@@ -13404,17 +13460,17 @@
       <c r="Z40" s="88">
         <v>0</v>
       </c>
-      <c r="AA40" s="88" t="str">
+      <c r="AA40" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB40" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="91" t="str">
+      <c r="AC40" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD40" s="86">
-        <v>0</v>
       </c>
       <c r="AE40" s="86">
         <v>0</v>
@@ -13503,17 +13559,17 @@
       <c r="Z41" s="88">
         <v>0</v>
       </c>
-      <c r="AA41" s="88" t="str">
+      <c r="AA41" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB41" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC41" s="91" t="str">
+      <c r="AC41" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD41" s="86">
-        <v>0</v>
       </c>
       <c r="AE41" s="86">
         <v>0</v>
@@ -13602,17 +13658,17 @@
       <c r="Z42" s="88">
         <v>0</v>
       </c>
-      <c r="AA42" s="88" t="str">
+      <c r="AA42" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB42" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="91" t="str">
+      <c r="AC42" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD42" s="86">
-        <v>0</v>
       </c>
       <c r="AE42" s="86">
         <v>0</v>
@@ -13701,17 +13757,17 @@
       <c r="Z43" s="88">
         <v>0</v>
       </c>
-      <c r="AA43" s="88" t="str">
+      <c r="AA43" s="88">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="91" t="str">
         <v>2019-04-17T00:00:00.0000000+00:00</v>
       </c>
-      <c r="AB43" s="91">
-        <v>0</v>
-      </c>
-      <c r="AC43" s="91" t="str">
+      <c r="AC43" s="91">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="86" t="str">
         <v>2019-04-15T00:00:00.0000000+00:00</v>
-      </c>
-      <c r="AD43" s="86">
-        <v>0</v>
       </c>
       <c r="AE43" s="86">
         <v>0</v>
@@ -13789,7 +13845,7 @@
         <v>0</v>
       </c>
       <c r="W44" s="90">
-        <v>43718.445308125003</v>
+        <v>43724.648770324071</v>
       </c>
       <c r="X44" s="90">
         <v>0</v>
@@ -13797,14 +13853,14 @@
       <c r="Y44" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z44" s="88">
-        <v>0</v>
+      <c r="Z44" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA44" s="88">
         <v>0</v>
       </c>
-      <c r="AB44" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB44" s="91">
+        <v>0</v>
       </c>
       <c r="AC44" s="91">
         <v>0</v>
@@ -13896,14 +13952,14 @@
       <c r="Y45" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z45" s="88">
-        <v>0</v>
+      <c r="Z45" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA45" s="88">
         <v>0</v>
       </c>
-      <c r="AB45" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB45" s="91">
+        <v>0</v>
       </c>
       <c r="AC45" s="91">
         <v>0</v>
@@ -13995,14 +14051,14 @@
       <c r="Y46" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z46" s="88">
-        <v>0</v>
+      <c r="Z46" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA46" s="88">
         <v>0</v>
       </c>
-      <c r="AB46" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB46" s="91">
+        <v>0</v>
       </c>
       <c r="AC46" s="91">
         <v>0</v>
@@ -14094,14 +14150,14 @@
       <c r="Y47" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z47" s="88">
-        <v>0</v>
+      <c r="Z47" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA47" s="88">
         <v>0</v>
       </c>
-      <c r="AB47" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB47" s="91">
+        <v>0</v>
       </c>
       <c r="AC47" s="91">
         <v>0</v>
@@ -14193,14 +14249,14 @@
       <c r="Y48" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z48" s="88">
-        <v>0</v>
+      <c r="Z48" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA48" s="88">
         <v>0</v>
       </c>
-      <c r="AB48" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB48" s="91">
+        <v>0</v>
       </c>
       <c r="AC48" s="91">
         <v>0</v>
@@ -14292,14 +14348,14 @@
       <c r="Y49" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z49" s="88">
-        <v>0</v>
+      <c r="Z49" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA49" s="88">
         <v>0</v>
       </c>
-      <c r="AB49" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB49" s="91">
+        <v>0</v>
       </c>
       <c r="AC49" s="91">
         <v>0</v>
@@ -14391,14 +14447,14 @@
       <c r="Y50" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z50" s="88">
-        <v>0</v>
+      <c r="Z50" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA50" s="88">
         <v>0</v>
       </c>
-      <c r="AB50" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB50" s="91">
+        <v>0</v>
       </c>
       <c r="AC50" s="91">
         <v>0</v>
@@ -14482,7 +14538,7 @@
         <v>0</v>
       </c>
       <c r="W51" s="90">
-        <v>43718.445308125003</v>
+        <v>43724.648770324071</v>
       </c>
       <c r="X51" s="90">
         <v>0</v>
@@ -14490,14 +14546,14 @@
       <c r="Y51" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z51" s="88">
-        <v>0</v>
+      <c r="Z51" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA51" s="88">
         <v>0</v>
       </c>
-      <c r="AB51" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB51" s="91">
+        <v>0</v>
       </c>
       <c r="AC51" s="91">
         <v>0</v>
@@ -14589,14 +14645,14 @@
       <c r="Y52" s="88" t="str">
         <v>77607da1-4705-4bf0-8cbb-febc36d83863</v>
       </c>
-      <c r="Z52" s="88">
-        <v>0</v>
+      <c r="Z52" s="88" t="str">
+        <v>Finbourne-Examples</v>
       </c>
       <c r="AA52" s="88">
         <v>0</v>
       </c>
-      <c r="AB52" s="91" t="str">
-        <v>Finbourne-Examples</v>
+      <c r="AB52" s="91">
+        <v>0</v>
       </c>
       <c r="AC52" s="91">
         <v>0</v>
@@ -15078,7 +15134,7 @@
   </sheetPr>
   <dimension ref="B1:S54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
@@ -15289,7 +15345,7 @@
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -15371,7 +15427,7 @@
     <row r="20" spans="2:15" ht="21" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
       <c r="C20" s="13" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="2"/>
@@ -15407,7 +15463,7 @@
     <row r="22" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -15511,7 +15567,7 @@
       </c>
       <c r="F27" s="92">
         <f ca="1">NOW()-1/24</f>
-        <v>43718.450923842596</v>
+        <v>43732.315038657413</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -15593,7 +15649,7 @@
       </c>
       <c r="F31" s="92">
         <f ca="1">F27-2/1440</f>
-        <v>43718.44953495371</v>
+        <v>43732.313649768526</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -15640,7 +15696,7 @@
     <row r="35" spans="2:19" ht="21" x14ac:dyDescent="0.35">
       <c r="B35" s="2"/>
       <c r="C35" s="13" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -15677,7 +15733,7 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -16303,7 +16359,7 @@
   <dimension ref="B1:R32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17869,6 +17925,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005F4F0FA1AC8B142BA5BFAEE01329AF1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="51d44e6750016a81140edd9302933050">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="7f1325bc-d786-4e92-924e-74ffe34b2b40" xmlns:ns3="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fbbf5b69800df541767d824f3fbf5177" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18094,16 +18160,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -18114,6 +18170,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F07F7B26-A8FB-44CC-BC1A-494CF9683469}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45EDF347-3168-4BEB-9A6E-9322773C07F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18133,24 +18207,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F07F7B26-A8FB-44CC-BC1A-494CF9683469}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="7f1325bc-d786-4e92-924e-74ffe34b2b40"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="655d3dbc-e9a1-4c85-8bc4-391e75a6cf80"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
   <ds:schemaRefs>

</xml_diff>